<commit_message>
BOM J connector name space
Removed spaces in BOM because it annoying
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliot Eickholtz\Documents\GitHub\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacko\OneDrive\Documents\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D39E2-541F-47CB-9570-BB06F20CE492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FA5CFB-3B93-4208-AB58-2229C3EB1FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-7320" windowWidth="16440" windowHeight="28440" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="156">
   <si>
     <t>DWG 2500 BILL OF MATERIALS (BOM)</t>
   </si>
@@ -429,9 +429,6 @@
     <t>J32</t>
   </si>
   <si>
-    <t xml:space="preserve"> J34</t>
-  </si>
-  <si>
     <t>J35</t>
   </si>
   <si>
@@ -499,6 +496,12 @@
   </si>
   <si>
     <t>JLC03</t>
+  </si>
+  <si>
+    <t>J34</t>
+  </si>
+  <si>
+    <t>J48</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1119,7 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1308,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="16" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>76</v>
@@ -1320,7 +1323,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>76</v>
@@ -1335,7 +1338,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="16" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>76</v>
@@ -1350,7 +1353,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>76</v>
@@ -1365,61 +1368,61 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="29">
         <v>971050154</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="B19" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="29">
         <v>971050154</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D20" s="29">
         <v>971050154</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D21" s="29">
         <v>971050154</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,7 +1450,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="41"/>
@@ -1475,49 +1478,49 @@
         <v>90</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="29">
         <v>2136</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="29">
         <v>1182</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>121</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>73</v>
@@ -1533,7 +1536,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>73</v>
@@ -1549,7 +1552,7 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>76</v>
@@ -1565,7 +1568,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>74</v>
@@ -1581,65 +1584,65 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D33" s="29">
         <v>971050154</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" s="29">
         <v>971050154</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D35" s="29">
         <v>971050154</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D36" s="30">
         <v>971050154</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,7 +1678,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="B40" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>12</v>
@@ -1708,7 +1711,7 @@
         <v>121</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added cables and edited connectors
Connectors now reflect what is on PCB accurately. Not finished
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30635D33-2060-4F58-9C70-FA8FF7C3FAB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AABD3E0-8834-4828-A6D1-BCE027B0EA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="123">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>LR1F120R</t>
+  </si>
+  <si>
+    <t>J34</t>
   </si>
 </sst>
 </file>
@@ -662,6 +665,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,9 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -991,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,11 +1009,11 @@
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
@@ -1321,11 +1324,11 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,11 +1515,11 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="34"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
@@ -1627,11 +1630,11 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="34"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
@@ -1758,12 +1761,12 @@
       <c r="E56" s="17"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
-      <c r="B57" s="29" t="s">
+      <c r="A57" s="29"/>
+      <c r="B57" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="31"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="34"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
@@ -1944,15 +1947,15 @@
       <c r="D70" s="25"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
-      <c r="B71" s="29" t="s">
+      <c r="A71" s="31"/>
+      <c r="B71" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C71" s="30"/>
-      <c r="D71" s="31"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="34"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="1" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +1970,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="13" t="s">
         <v>42</v>
       </c>
@@ -1976,7 +1979,7 @@
       <c r="E73" s="15"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="13" t="s">
         <v>117</v>
       </c>
@@ -1989,7 +1992,7 @@
       <c r="E74" s="15"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="34"/>
+      <c r="A75" s="31"/>
       <c r="B75" s="13" t="s">
         <v>17</v>
       </c>
@@ -1999,14 +2002,14 @@
       <c r="D75" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E75" s="33" t="s">
+      <c r="E75" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="34"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="13" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>20</v>
@@ -2019,7 +2022,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="13" t="s">
         <v>118</v>
       </c>
@@ -2034,7 +2037,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
+      <c r="A78" s="31"/>
       <c r="B78" s="9" t="s">
         <v>119</v>
       </c>
@@ -2049,7 +2052,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
+      <c r="A79" s="31"/>
       <c r="B79" s="10" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Revisions for main drawings
Summary:
-updated numbers to reflect current scheme. (1110 -> 1101, 1210 -> 1201, etc.)
-updated BOM in all drawings to correctly refference drawing numbers

whats needed:
-off-board components finished
-re-order connectors relative to schematics
-fill in on schematics
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB717FFF-59B2-4425-982D-AE61F819DF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D08E5F-DABB-400E-BACD-47FA801C0A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="149">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -439,6 +439,45 @@
   </si>
   <si>
     <t>REFFERENCE DRAWING 1x20</t>
+  </si>
+  <si>
+    <t>REFFERENCE DRAWING xxxx</t>
+  </si>
+  <si>
+    <t>CABLE_019</t>
+  </si>
+  <si>
+    <t>CABLE_004</t>
+  </si>
+  <si>
+    <t>CABLE_005</t>
+  </si>
+  <si>
+    <t>REFFERENCE DRAWING XXXX</t>
+  </si>
+  <si>
+    <t>REFFERENCE DRAWING XXX</t>
+  </si>
+  <si>
+    <t>CABLE_011</t>
+  </si>
+  <si>
+    <t>CABLE_007</t>
+  </si>
+  <si>
+    <t>CABLE_008</t>
+  </si>
+  <si>
+    <t>CABLE_009</t>
+  </si>
+  <si>
+    <t>CABLE_020</t>
+  </si>
+  <si>
+    <t>CABLE_016</t>
+  </si>
+  <si>
+    <t>CABLE_017</t>
   </si>
 </sst>
 </file>
@@ -646,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,14 +700,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -693,9 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -715,15 +745,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1039,31 +1082,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107:D118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="34" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1077,401 +1120,412 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>533751210</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>533751110</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>533750710</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>533750710</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>533750510</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>533750210</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>533750210</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>533750210</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>533750210</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>533750210</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="16">
         <v>533750210</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>533750210</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>971050154</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>971050154</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="16">
         <v>971050154</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="16">
         <v>971050154</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="16"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>124</v>
       </c>
       <c r="C24" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>125</v>
       </c>
       <c r="C25" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>126</v>
       </c>
       <c r="C26" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>127</v>
       </c>
       <c r="C27" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>129</v>
       </c>
       <c r="C29" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
         <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>132</v>
       </c>
       <c r="C32" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C33" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="14" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="34" t="s">
+      <c r="D34" s="34"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="35"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
       <c r="B44" s="1" t="s">
         <v>0</v>
       </c>
@@ -1485,731 +1539,847 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="13" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="16">
         <v>2136</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="13" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="16">
         <v>1182</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="13" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="13" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="18">
+      <c r="D48" s="16">
         <v>533750710</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="13" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="18">
+      <c r="D49" s="16">
         <v>533750710</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="13" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="16">
         <v>533750210</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="13" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="18">
+      <c r="D51" s="16">
         <v>533750510</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="13" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D52" s="18">
+      <c r="D52" s="16">
         <v>971050154</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="13" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D53" s="18">
+      <c r="D53" s="16">
         <v>971050154</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="18">
+      <c r="D54" s="16">
         <v>971050154</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="14" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="19">
+      <c r="D55" s="17">
         <v>971050154</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="12"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="20"/>
-      <c r="B57" s="34" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="33"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" s="20"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="20"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="34"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="36"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="20"/>
-      <c r="B58" s="23" t="s">
+      <c r="C64" s="29"/>
+      <c r="D64" s="30"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C65" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D65" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E65" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="20"/>
-      <c r="B59" s="2" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D66" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E66" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="20"/>
-      <c r="B60" s="2" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C67" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D67" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="20"/>
-      <c r="B61" s="2" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C68" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="18">
+      <c r="D68" s="16">
         <v>2670</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E68" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="20"/>
-      <c r="B62" s="2" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D69" s="16">
         <v>533750510</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E69" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="20"/>
-      <c r="B63" s="2" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D70" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E70" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="20"/>
-      <c r="B64" s="4" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D71" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E71" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="8"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="20"/>
-      <c r="B66" s="31" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D72" s="39"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="33"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="20"/>
-      <c r="B67" s="1" t="s">
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="20"/>
-      <c r="B68" s="25" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="18"/>
+      <c r="B77" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C77" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D77" s="24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="20"/>
-      <c r="B69" s="9" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
+      <c r="B78" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C78" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D69" s="18">
+      <c r="D78" s="16">
         <v>533750210</v>
       </c>
-      <c r="E69" s="17" t="s">
+      <c r="E78" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="20"/>
-      <c r="B70" s="9" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C79" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D70" s="18">
+      <c r="D79" s="16">
         <v>533751110</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E79" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="20"/>
-      <c r="B71" s="9" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
+      <c r="B80" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C80" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="18">
+      <c r="D80" s="16">
         <v>533750210</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E80" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="20"/>
-      <c r="B72" s="9" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C81" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="18">
+      <c r="D81" s="16">
         <v>971050154</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="E81" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="20"/>
-      <c r="B73" s="9" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
+      <c r="B82" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D82" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E82" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="20"/>
-      <c r="B74" s="10" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
+      <c r="B83" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C83" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D83" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E83" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="21"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="17"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="28"/>
-      <c r="B76" s="31" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="33"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C85" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D85" s="34"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="33"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="20"/>
-      <c r="B77" s="1" t="s">
+      <c r="C87" s="29"/>
+      <c r="D87" s="30"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E88" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="20"/>
-      <c r="B78" s="9" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="18"/>
+      <c r="B89" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="18">
+      <c r="D89" s="16">
         <v>987</v>
       </c>
-      <c r="E78" s="17" t="s">
+      <c r="E89" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="20"/>
-      <c r="B79" s="9" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="18"/>
+      <c r="B90" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D90" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E90" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="20"/>
-      <c r="B80" s="9" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="18"/>
+      <c r="B91" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D80" s="18"/>
-      <c r="E80" s="17"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="20"/>
-      <c r="B81" s="9" t="s">
+      <c r="D91" s="16"/>
+      <c r="E91" s="15"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="18"/>
+      <c r="B92" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C92" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D81" s="18" t="s">
+      <c r="D92" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="20"/>
-      <c r="B82" s="9" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="18"/>
+      <c r="B93" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D93" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E93" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="20"/>
-      <c r="B83" s="9" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
+      <c r="B94" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="18">
+      <c r="D94" s="16">
         <v>533750210</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E94" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="20"/>
-      <c r="B84" s="2" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="18"/>
+      <c r="B95" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="18">
-        <v>533750210</v>
-      </c>
-      <c r="E84" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
-      <c r="B85" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" s="18">
-        <v>533750210</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="20"/>
-      <c r="B86" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86" s="18">
-        <v>533750210</v>
-      </c>
-      <c r="E86" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="20"/>
-      <c r="B87" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D87" s="18">
-        <v>533750510</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="20"/>
-      <c r="B88" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D88" s="19">
-        <v>971050154</v>
-      </c>
-      <c r="E88" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="30"/>
-      <c r="B90" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C90" s="32"/>
-      <c r="D90" s="33"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="30"/>
-      <c r="B91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="30"/>
-      <c r="B92" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C92" s="15"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="15"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="30"/>
-      <c r="B93" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D93" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E93" s="15"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="30"/>
-      <c r="B94" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D94" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E94" s="29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="30"/>
-      <c r="B95" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D95" s="18">
+      <c r="D95" s="16">
         <v>533750210</v>
       </c>
-      <c r="E95" s="17" t="s">
+      <c r="E95" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="30"/>
-      <c r="B96" s="13" t="s">
-        <v>118</v>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="18"/>
+      <c r="B96" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D96" s="18">
+      <c r="D96" s="16">
         <v>533750210</v>
       </c>
-      <c r="E96" s="17" t="s">
+      <c r="E96" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="30"/>
-      <c r="B97" s="9" t="s">
-        <v>119</v>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="18"/>
+      <c r="B97" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D97" s="18">
+      <c r="D97" s="16">
         <v>533750210</v>
       </c>
-      <c r="E97" s="17" t="s">
+      <c r="E97" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="30"/>
-      <c r="B98" s="10" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
+      <c r="B98" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="16">
+        <v>533750510</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
+      <c r="B99" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="16" t="s">
+      <c r="C99" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D98" s="19">
+      <c r="D99" s="17">
         <v>971050154</v>
       </c>
-      <c r="E98" s="17" t="s">
+      <c r="E99" s="15" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D100" s="33"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" s="20"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C102" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D102" s="20"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D103" s="20"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C104" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D104" s="34"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="27"/>
+      <c r="B107" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C107" s="29"/>
+      <c r="D107" s="30"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="27"/>
+      <c r="B108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="27"/>
+      <c r="B109" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C109" s="13"/>
+      <c r="D109" s="20"/>
+      <c r="E109" s="13"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="27"/>
+      <c r="B110" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E110" s="13"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="27"/>
+      <c r="B111" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="27"/>
+      <c r="B112" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D112" s="16">
+        <v>533750210</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="27"/>
+      <c r="B113" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="16">
+        <v>533750210</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="27"/>
+      <c r="B114" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D114" s="16">
+        <v>533750210</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="27"/>
+      <c r="B115" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D115" s="17">
+        <v>971050154</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D116" s="33"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C117" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D117" s="20"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C118" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D118" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B107:D107"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B87:D87"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2221,11 +2391,11 @@
     <hyperlink ref="E8" r:id="rId6" xr:uid="{240EB6DB-C584-421D-994A-DE45E8120A2E}"/>
     <hyperlink ref="E11" r:id="rId7" xr:uid="{E2F47A58-74DE-4DAB-89A7-5934D1313DC0}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{2E8799C7-D339-4FE3-8C7A-FE7C71B67E61}"/>
-    <hyperlink ref="E59" r:id="rId9" xr:uid="{F23F2E0C-5535-46F3-AE18-45647BC4A186}"/>
-    <hyperlink ref="E61" r:id="rId10" xr:uid="{329F5228-1042-4F28-9F10-68E331FA9A00}"/>
-    <hyperlink ref="E62" r:id="rId11" xr:uid="{A65293D0-5A91-4FF2-9AC6-EB2239777401}"/>
-    <hyperlink ref="E63" r:id="rId12" xr:uid="{653C09D9-E0A5-4FCC-A811-3105B9C77436}"/>
-    <hyperlink ref="E64" r:id="rId13" xr:uid="{778D1647-04D6-4B31-AAE1-35CD1E3BF920}"/>
+    <hyperlink ref="E66" r:id="rId9" xr:uid="{F23F2E0C-5535-46F3-AE18-45647BC4A186}"/>
+    <hyperlink ref="E68" r:id="rId10" xr:uid="{329F5228-1042-4F28-9F10-68E331FA9A00}"/>
+    <hyperlink ref="E69" r:id="rId11" xr:uid="{A65293D0-5A91-4FF2-9AC6-EB2239777401}"/>
+    <hyperlink ref="E70" r:id="rId12" xr:uid="{653C09D9-E0A5-4FCC-A811-3105B9C77436}"/>
+    <hyperlink ref="E71" r:id="rId13" xr:uid="{778D1647-04D6-4B31-AAE1-35CD1E3BF920}"/>
     <hyperlink ref="E52" r:id="rId14" xr:uid="{E2A77305-0703-444F-B212-A6078F7AFE45}"/>
     <hyperlink ref="E53" r:id="rId15" xr:uid="{FFF48BD2-357A-4E55-82C2-BC3058578DC6}"/>
     <hyperlink ref="E54" r:id="rId16" xr:uid="{E8B0DE21-F1B8-4DBC-961C-5A92566C333C}"/>
@@ -2236,26 +2406,26 @@
     <hyperlink ref="E48" r:id="rId21" xr:uid="{04D0839B-BA7C-4F4D-B91C-97A8EFF84E0C}"/>
     <hyperlink ref="E46" r:id="rId22" xr:uid="{ACB98E67-2E7B-454D-8E93-7B836B3D7957}"/>
     <hyperlink ref="E45" r:id="rId23" xr:uid="{CBCE2BBD-E319-4CA5-99FD-4235DF810FC4}"/>
-    <hyperlink ref="E70" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
-    <hyperlink ref="E69" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
-    <hyperlink ref="E71" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
-    <hyperlink ref="E72" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
-    <hyperlink ref="E73" r:id="rId28" xr:uid="{36F7B2D2-11D1-453F-98B7-7E472CCC4124}"/>
-    <hyperlink ref="E74" r:id="rId29" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
-    <hyperlink ref="E78" r:id="rId30" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
-    <hyperlink ref="E79" r:id="rId31" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
-    <hyperlink ref="E82" r:id="rId32" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
-    <hyperlink ref="E88" r:id="rId33" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
-    <hyperlink ref="E83" r:id="rId34" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
-    <hyperlink ref="E84" r:id="rId35" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
-    <hyperlink ref="E85" r:id="rId36" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
-    <hyperlink ref="E86" r:id="rId37" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
-    <hyperlink ref="E87" r:id="rId38" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
-    <hyperlink ref="E95" r:id="rId39" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
-    <hyperlink ref="E96" r:id="rId40" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
-    <hyperlink ref="E97" r:id="rId41" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
-    <hyperlink ref="E94" r:id="rId42" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
-    <hyperlink ref="E98" r:id="rId43" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
+    <hyperlink ref="E79" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
+    <hyperlink ref="E78" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
+    <hyperlink ref="E80" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
+    <hyperlink ref="E81" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
+    <hyperlink ref="E82" r:id="rId28" xr:uid="{36F7B2D2-11D1-453F-98B7-7E472CCC4124}"/>
+    <hyperlink ref="E83" r:id="rId29" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
+    <hyperlink ref="E89" r:id="rId30" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
+    <hyperlink ref="E90" r:id="rId31" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
+    <hyperlink ref="E93" r:id="rId32" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
+    <hyperlink ref="E99" r:id="rId33" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
+    <hyperlink ref="E94" r:id="rId34" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
+    <hyperlink ref="E95" r:id="rId35" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
+    <hyperlink ref="E96" r:id="rId36" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
+    <hyperlink ref="E97" r:id="rId37" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
+    <hyperlink ref="E98" r:id="rId38" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
+    <hyperlink ref="E112" r:id="rId39" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
+    <hyperlink ref="E113" r:id="rId40" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
+    <hyperlink ref="E114" r:id="rId41" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
+    <hyperlink ref="E111" r:id="rId42" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
+    <hyperlink ref="E115" r:id="rId43" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId44"/>

</xml_diff>

<commit_message>
Reorganized Files, Renamed, and Reformatted DWG's
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C5F78C-2C00-4FFD-88A8-F5FE80A06727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265A88C-4C1B-4C7D-947F-FB92AE1D1C87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17472" yWindow="1332" windowWidth="10692" windowHeight="10488" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="206">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -490,6 +490,165 @@
   </si>
   <si>
     <t>REFFERENCE DRAWING 1620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1120 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>12-Pin On-Board Male Crimp Connector</t>
+  </si>
+  <si>
+    <t>51163-1200</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>3-Pin Female Molex Connector</t>
+  </si>
+  <si>
+    <t>3-F-MOLEX</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>7-Pin On-Board Male Crimp Connector</t>
+  </si>
+  <si>
+    <t>53375-0710</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>7-Pin On-Board Female Crimp Connector</t>
+  </si>
+  <si>
+    <t>51163-0700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     DWG 1121 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>2-Pin On-Board Male Crimp Connector</t>
+  </si>
+  <si>
+    <t>53375-0210</t>
+  </si>
+  <si>
+    <t>2-Pin Female Molex Connector</t>
+  </si>
+  <si>
+    <t>2-F-MOLEX</t>
+  </si>
+  <si>
+    <t>11-Pin On-Board Male Crimp Connector</t>
+  </si>
+  <si>
+    <t>53375-1210</t>
+  </si>
+  <si>
+    <t>11-Pin Female Molex Connector</t>
+  </si>
+  <si>
+    <t>11-F-MOLEX</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1122 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J30</t>
+  </si>
+  <si>
+    <t>J32</t>
+  </si>
+  <si>
+    <t>5-Pin On-Board Male Crimp Connector</t>
+  </si>
+  <si>
+    <t>53375-0510</t>
+  </si>
+  <si>
+    <t>5-Pin Female Molex Connector</t>
+  </si>
+  <si>
+    <t>5-F-MOLEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1123 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J46</t>
+  </si>
+  <si>
+    <t>J49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1220 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>4-Pin Female Molex Connector</t>
+  </si>
+  <si>
+    <t>4-F-MOLEX</t>
+  </si>
+  <si>
+    <t>J51</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1420 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1520 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>J22</t>
+  </si>
+  <si>
+    <t>J44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1620 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>J37</t>
+  </si>
+  <si>
+    <t>J39</t>
+  </si>
+  <si>
+    <t>DWG 1320 BILL OF MATERIALS (BOM)</t>
   </si>
 </sst>
 </file>
@@ -539,7 +698,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -692,12 +851,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,16 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -729,9 +892,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -748,28 +908,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -778,6 +928,102 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1094,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,15 +1356,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1133,1265 +1379,1994 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>533751210</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>533751110</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>533750710</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>533750710</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>533750510</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>533750210</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>533750210</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>533750210</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>533750210</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>533750210</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>533750210</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>533750210</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>971050154</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>971050154</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>971050154</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>971050154</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C24" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="20"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="20"/>
+      <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>126</v>
       </c>
       <c r="C26" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="20"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C27" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="8" t="s">
         <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="16"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C29" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="20"/>
+      <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="8" t="s">
         <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>147</v>
       </c>
-      <c r="D31" s="20"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>132</v>
       </c>
       <c r="C32" t="s">
         <v>147</v>
       </c>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>133</v>
       </c>
       <c r="C33" t="s">
         <v>148</v>
       </c>
-      <c r="D33" s="20"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="37" t="s">
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="31"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="40" t="s">
+      <c r="D34" s="25"/>
+    </row>
+    <row r="36" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="36"/>
+      <c r="C36" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="38"/>
+    </row>
+    <row r="37" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="39"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+    </row>
+    <row r="49" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="51"/>
+      <c r="C49" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="53"/>
+    </row>
+    <row r="50" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" s="45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D56" s="58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+    </row>
+    <row r="58" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="60"/>
+      <c r="C58" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="62"/>
+    </row>
+    <row r="59" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" s="56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D67" s="58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="55"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+    </row>
+    <row r="69" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="65"/>
+      <c r="C69" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="67"/>
+    </row>
+    <row r="70" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D71" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="63"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="1" t="s">
+      <c r="C76" s="31"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E77" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="11" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C78" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D78" s="13">
         <v>2136</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E78" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="11" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C79" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D79" s="13">
         <v>1182</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E79" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="11" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C80" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D80" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="11" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C81" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D81" s="13">
         <v>533750710</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E81" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="11" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C82" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D82" s="13">
         <v>533750710</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E82" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="11" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C83" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D83" s="13">
         <v>533750210</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E83" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="11" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C84" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="16">
+      <c r="D84" s="13">
         <v>533750510</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E84" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="11" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C85" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D85" s="13">
         <v>971050154</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E85" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="11" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C86" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D86" s="13">
         <v>971050154</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E86" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="11" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="14"/>
+      <c r="B87" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C87" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D87" s="13">
         <v>971050154</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E87" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="12" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C88" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D88" s="13">
         <v>971050154</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E88" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="28" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C89" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="30"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C90" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="20"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="s">
+      <c r="D90" s="16"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C91" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D58" s="20"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="12" t="s">
+      <c r="D91" s="16"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C92" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="31"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
-      <c r="B64" s="40" t="s">
+      <c r="D92" s="25"/>
+    </row>
+    <row r="94" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="70"/>
+      <c r="C94" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="D94" s="72"/>
+    </row>
+    <row r="95" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C97" s="74" t="s">
+        <v>190</v>
+      </c>
+      <c r="D97" s="56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="D98" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="D99" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="74" t="s">
+        <v>190</v>
+      </c>
+      <c r="D100" s="56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="D101" s="56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D102" s="58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="14"/>
+      <c r="B104" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="42"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="21" t="s">
+      <c r="C104" s="31"/>
+      <c r="D104" s="32"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="14"/>
+      <c r="B105" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C105" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="21" t="s">
+      <c r="D105" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E105" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="2" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="14"/>
+      <c r="B106" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D106" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E106" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="2" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="14"/>
+      <c r="B107" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C107" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D107" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="2" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="14"/>
+      <c r="B108" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C108" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D68" s="16">
+      <c r="D108" s="13">
         <v>2670</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E108" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="2" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="14"/>
+      <c r="B109" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="16">
+      <c r="D109" s="13">
         <v>533750510</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E109" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="2" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="14"/>
+      <c r="B110" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D110" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E110" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="4" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="14"/>
+      <c r="B111" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C111" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D111" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E111" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="34" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C72" s="35" t="s">
+      <c r="C112" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D72" s="36"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
-      <c r="B75" s="40" t="s">
+      <c r="D112" s="25"/>
+    </row>
+    <row r="114" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C114" s="31"/>
+      <c r="D114" s="32"/>
+    </row>
+    <row r="115" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="14"/>
+      <c r="B119" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C75" s="41"/>
-      <c r="D75" s="42"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
-      <c r="B76" s="1" t="s">
+      <c r="C119" s="31"/>
+      <c r="D119" s="32"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14"/>
+      <c r="B120" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E120" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
-      <c r="B77" s="22" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14"/>
+      <c r="B121" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C77" s="23" t="s">
+      <c r="C121" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D77" s="24" t="s">
+      <c r="D121" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="18"/>
-      <c r="B78" s="7" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14"/>
+      <c r="B122" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C122" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="16">
+      <c r="D122" s="13">
         <v>533750210</v>
       </c>
-      <c r="E78" s="15" t="s">
+      <c r="E122" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
-      <c r="B79" s="7" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14"/>
+      <c r="B123" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C123" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D79" s="16">
+      <c r="D123" s="13">
         <v>533751110</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E123" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="18"/>
-      <c r="B80" s="7" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14"/>
+      <c r="B124" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C124" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="16">
+      <c r="D124" s="13">
         <v>533750210</v>
       </c>
-      <c r="E80" s="15" t="s">
+      <c r="E124" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="18"/>
-      <c r="B81" s="7" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14"/>
+      <c r="B125" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C125" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D81" s="16">
+      <c r="D125" s="13">
         <v>971050154</v>
       </c>
-      <c r="E81" s="15" t="s">
+      <c r="E125" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
-      <c r="B82" s="7" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14"/>
+      <c r="B126" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="16" t="s">
+      <c r="D126" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E82" s="15" t="s">
+      <c r="E126" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
-      <c r="B83" s="8" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14"/>
+      <c r="B127" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C127" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D127" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E83" s="15" t="s">
+      <c r="E127" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="33" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B128" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C128" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D84" s="30"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+      <c r="D128" s="16"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C85" s="29" t="s">
+      <c r="C129" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="31"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="40" t="s">
+      <c r="D129" s="25"/>
+    </row>
+    <row r="130" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="26"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="73"/>
+    </row>
+    <row r="131" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="76"/>
+      <c r="C131" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="D131" s="78"/>
+    </row>
+    <row r="132" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="C133" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D133" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C134" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D134" s="58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="21"/>
+      <c r="B136" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="41"/>
-      <c r="D87" s="42"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="1" t="s">
+      <c r="C136" s="31"/>
+      <c r="D136" s="32"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14"/>
+      <c r="B137" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E137" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
-      <c r="B89" s="7" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14"/>
+      <c r="B138" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C138" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D89" s="16">
+      <c r="D138" s="13">
         <v>987</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="E138" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
-      <c r="B90" s="7" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14"/>
+      <c r="B139" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D139" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E90" s="15" t="s">
+      <c r="E139" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
-      <c r="B91" s="7" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14"/>
+      <c r="B140" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C140" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D91" s="16"/>
-      <c r="E91" s="15"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="18"/>
-      <c r="B92" s="7" t="s">
+      <c r="D140" s="13"/>
+      <c r="E140" s="12"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14"/>
+      <c r="B141" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C141" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D141" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
-      <c r="B93" s="7" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14"/>
+      <c r="B142" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C142" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D142" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E93" s="15" t="s">
+      <c r="E142" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="7" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14"/>
+      <c r="B143" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D94" s="16">
+      <c r="D143" s="13">
         <v>533750210</v>
       </c>
-      <c r="E94" s="15" t="s">
+      <c r="E143" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="2" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="14"/>
+      <c r="B144" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C144" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D95" s="16">
+      <c r="D144" s="13">
         <v>533750210</v>
       </c>
-      <c r="E95" s="15" t="s">
+      <c r="E144" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
-      <c r="B96" s="7" t="s">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="14"/>
+      <c r="B145" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C145" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D96" s="16">
+      <c r="D145" s="13">
         <v>533750210</v>
       </c>
-      <c r="E96" s="15" t="s">
+      <c r="E145" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
-      <c r="B97" s="7" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="14"/>
+      <c r="B146" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D97" s="16">
+      <c r="D146" s="13">
         <v>533750210</v>
       </c>
-      <c r="E97" s="15" t="s">
+      <c r="E146" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
-      <c r="B98" s="7" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="14"/>
+      <c r="B147" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D98" s="16">
+      <c r="D147" s="13">
         <v>533750510</v>
       </c>
-      <c r="E98" s="15" t="s">
+      <c r="E147" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
-      <c r="B99" s="8" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14"/>
+      <c r="B148" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C99" s="14" t="s">
+      <c r="C148" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D99" s="17">
+      <c r="D148" s="13">
         <v>971050154</v>
       </c>
-      <c r="E99" s="15" t="s">
+      <c r="E148" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="33" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C100" s="32" t="s">
+      <c r="C149" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D100" s="30"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
+      <c r="D149" s="16"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="C150" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="D101" s="20"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="2" t="s">
+      <c r="D150" s="16"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C102" s="32" t="s">
+      <c r="C151" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="D102" s="20"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
+      <c r="D151" s="16"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="C152" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="D103" s="20"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+      <c r="D152" s="16"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C104" s="38" t="s">
+      <c r="C153" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="D104" s="31"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
-      <c r="B107" s="40" t="s">
+      <c r="D153" s="25"/>
+    </row>
+    <row r="155" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="80"/>
+      <c r="C155" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="D155" s="82"/>
+    </row>
+    <row r="156" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C157" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D157" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C158" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D158" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C159" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D159" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="C160" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D160" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C161" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D161" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C162" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D162" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C163" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="D163" s="56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C164" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D164" s="58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="23"/>
+      <c r="B166" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="C107" s="41"/>
-      <c r="D107" s="42"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="27"/>
-      <c r="B108" s="1" t="s">
+      <c r="C166" s="31"/>
+      <c r="D166" s="32"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="23"/>
+      <c r="B167" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C167" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E167" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="27"/>
-      <c r="B109" s="11" t="s">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="23"/>
+      <c r="B168" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C109" s="13"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="13"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="27"/>
-      <c r="B110" s="11" t="s">
+      <c r="C168" s="10"/>
+      <c r="D168" s="16"/>
+      <c r="E168" s="10"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="23"/>
+      <c r="B169" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C169" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D110" s="16" t="s">
+      <c r="D169" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E110" s="13"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="27"/>
-      <c r="B111" s="11" t="s">
+      <c r="E169" s="10"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="23"/>
+      <c r="B170" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C170" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D111" s="16" t="s">
+      <c r="D170" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E111" s="26" t="s">
+      <c r="E170" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="27"/>
-      <c r="B112" s="11" t="s">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="23"/>
+      <c r="B171" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C171" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D112" s="16">
+      <c r="D171" s="13">
         <v>533750210</v>
       </c>
-      <c r="E112" s="15" t="s">
+      <c r="E171" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="27"/>
-      <c r="B113" s="11" t="s">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="23"/>
+      <c r="B172" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C172" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D113" s="16">
+      <c r="D172" s="13">
         <v>533750210</v>
       </c>
-      <c r="E113" s="15" t="s">
+      <c r="E172" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="27"/>
-      <c r="B114" s="7" t="s">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="23"/>
+      <c r="B173" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C173" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D114" s="16">
+      <c r="D173" s="13">
         <v>533750210</v>
       </c>
-      <c r="E114" s="15" t="s">
+      <c r="E173" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="27"/>
-      <c r="B115" s="8" t="s">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="23"/>
+      <c r="B174" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C174" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D115" s="17">
+      <c r="D174" s="13">
         <v>971050154</v>
       </c>
-      <c r="E115" s="15" t="s">
+      <c r="E174" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="39" t="s">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B175" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C116" s="32" t="s">
+      <c r="C175" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D116" s="30"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="11" t="s">
+      <c r="D175" s="16"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C117" s="32" t="s">
+      <c r="C176" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="D117" s="20"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="12" t="s">
+      <c r="D176" s="16"/>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C118" s="38" t="s">
+      <c r="C177" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="D118" s="31"/>
+      <c r="D177" s="25"/>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="84"/>
+      <c r="C179" s="85" t="s">
+        <v>202</v>
+      </c>
+      <c r="D179" s="86"/>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D180" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D181" s="49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="C182" s="88" t="s">
+        <v>171</v>
+      </c>
+      <c r="D182" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C183" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="D183" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="C184" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D184" s="58" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B107:D107"/>
+  <mergeCells count="7">
+    <mergeCell ref="B166:D166"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B114:D114"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2403,41 +3378,41 @@
     <hyperlink ref="E8" r:id="rId6" xr:uid="{240EB6DB-C584-421D-994A-DE45E8120A2E}"/>
     <hyperlink ref="E11" r:id="rId7" xr:uid="{E2F47A58-74DE-4DAB-89A7-5934D1313DC0}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{2E8799C7-D339-4FE3-8C7A-FE7C71B67E61}"/>
-    <hyperlink ref="E66" r:id="rId9" xr:uid="{F23F2E0C-5535-46F3-AE18-45647BC4A186}"/>
-    <hyperlink ref="E68" r:id="rId10" xr:uid="{329F5228-1042-4F28-9F10-68E331FA9A00}"/>
-    <hyperlink ref="E69" r:id="rId11" xr:uid="{A65293D0-5A91-4FF2-9AC6-EB2239777401}"/>
-    <hyperlink ref="E70" r:id="rId12" xr:uid="{653C09D9-E0A5-4FCC-A811-3105B9C77436}"/>
-    <hyperlink ref="E71" r:id="rId13" xr:uid="{778D1647-04D6-4B31-AAE1-35CD1E3BF920}"/>
-    <hyperlink ref="E52" r:id="rId14" xr:uid="{E2A77305-0703-444F-B212-A6078F7AFE45}"/>
-    <hyperlink ref="E53" r:id="rId15" xr:uid="{FFF48BD2-357A-4E55-82C2-BC3058578DC6}"/>
-    <hyperlink ref="E54" r:id="rId16" xr:uid="{E8B0DE21-F1B8-4DBC-961C-5A92566C333C}"/>
-    <hyperlink ref="E55" r:id="rId17" xr:uid="{F854A663-0171-4085-82CF-9CCE8DEFBEA5}"/>
-    <hyperlink ref="E51" r:id="rId18" xr:uid="{2C012892-2B5E-4466-B842-D0CB88D12306}"/>
-    <hyperlink ref="E50" r:id="rId19" xr:uid="{BD52DA9C-D744-4B02-8FCD-7B6B12660011}"/>
-    <hyperlink ref="E49" r:id="rId20" xr:uid="{8C6FEF8C-2465-4C85-B5A2-56F1A6F310EE}"/>
-    <hyperlink ref="E48" r:id="rId21" xr:uid="{04D0839B-BA7C-4F4D-B91C-97A8EFF84E0C}"/>
-    <hyperlink ref="E46" r:id="rId22" xr:uid="{ACB98E67-2E7B-454D-8E93-7B836B3D7957}"/>
-    <hyperlink ref="E45" r:id="rId23" xr:uid="{CBCE2BBD-E319-4CA5-99FD-4235DF810FC4}"/>
-    <hyperlink ref="E79" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
-    <hyperlink ref="E78" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
-    <hyperlink ref="E80" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
-    <hyperlink ref="E81" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
-    <hyperlink ref="E82" r:id="rId28" xr:uid="{36F7B2D2-11D1-453F-98B7-7E472CCC4124}"/>
-    <hyperlink ref="E83" r:id="rId29" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
-    <hyperlink ref="E89" r:id="rId30" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
-    <hyperlink ref="E90" r:id="rId31" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
-    <hyperlink ref="E93" r:id="rId32" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
-    <hyperlink ref="E99" r:id="rId33" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
-    <hyperlink ref="E94" r:id="rId34" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
-    <hyperlink ref="E95" r:id="rId35" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
-    <hyperlink ref="E96" r:id="rId36" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
-    <hyperlink ref="E97" r:id="rId37" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
-    <hyperlink ref="E98" r:id="rId38" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
-    <hyperlink ref="E112" r:id="rId39" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
-    <hyperlink ref="E113" r:id="rId40" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
-    <hyperlink ref="E114" r:id="rId41" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
-    <hyperlink ref="E111" r:id="rId42" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
-    <hyperlink ref="E115" r:id="rId43" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
+    <hyperlink ref="E106" r:id="rId9" xr:uid="{F23F2E0C-5535-46F3-AE18-45647BC4A186}"/>
+    <hyperlink ref="E108" r:id="rId10" xr:uid="{329F5228-1042-4F28-9F10-68E331FA9A00}"/>
+    <hyperlink ref="E109" r:id="rId11" xr:uid="{A65293D0-5A91-4FF2-9AC6-EB2239777401}"/>
+    <hyperlink ref="E110" r:id="rId12" xr:uid="{653C09D9-E0A5-4FCC-A811-3105B9C77436}"/>
+    <hyperlink ref="E111" r:id="rId13" xr:uid="{778D1647-04D6-4B31-AAE1-35CD1E3BF920}"/>
+    <hyperlink ref="E85" r:id="rId14" xr:uid="{E2A77305-0703-444F-B212-A6078F7AFE45}"/>
+    <hyperlink ref="E86" r:id="rId15" xr:uid="{FFF48BD2-357A-4E55-82C2-BC3058578DC6}"/>
+    <hyperlink ref="E87" r:id="rId16" xr:uid="{E8B0DE21-F1B8-4DBC-961C-5A92566C333C}"/>
+    <hyperlink ref="E88" r:id="rId17" xr:uid="{F854A663-0171-4085-82CF-9CCE8DEFBEA5}"/>
+    <hyperlink ref="E84" r:id="rId18" xr:uid="{2C012892-2B5E-4466-B842-D0CB88D12306}"/>
+    <hyperlink ref="E83" r:id="rId19" xr:uid="{BD52DA9C-D744-4B02-8FCD-7B6B12660011}"/>
+    <hyperlink ref="E82" r:id="rId20" xr:uid="{8C6FEF8C-2465-4C85-B5A2-56F1A6F310EE}"/>
+    <hyperlink ref="E81" r:id="rId21" xr:uid="{04D0839B-BA7C-4F4D-B91C-97A8EFF84E0C}"/>
+    <hyperlink ref="E79" r:id="rId22" xr:uid="{ACB98E67-2E7B-454D-8E93-7B836B3D7957}"/>
+    <hyperlink ref="E78" r:id="rId23" xr:uid="{CBCE2BBD-E319-4CA5-99FD-4235DF810FC4}"/>
+    <hyperlink ref="E123" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
+    <hyperlink ref="E122" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
+    <hyperlink ref="E124" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
+    <hyperlink ref="E125" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
+    <hyperlink ref="E126" r:id="rId28" xr:uid="{36F7B2D2-11D1-453F-98B7-7E472CCC4124}"/>
+    <hyperlink ref="E127" r:id="rId29" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
+    <hyperlink ref="E138" r:id="rId30" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
+    <hyperlink ref="E139" r:id="rId31" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
+    <hyperlink ref="E142" r:id="rId32" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
+    <hyperlink ref="E148" r:id="rId33" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
+    <hyperlink ref="E143" r:id="rId34" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
+    <hyperlink ref="E144" r:id="rId35" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
+    <hyperlink ref="E145" r:id="rId36" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
+    <hyperlink ref="E146" r:id="rId37" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
+    <hyperlink ref="E147" r:id="rId38" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
+    <hyperlink ref="E171" r:id="rId39" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
+    <hyperlink ref="E172" r:id="rId40" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
+    <hyperlink ref="E173" r:id="rId41" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
+    <hyperlink ref="E170" r:id="rId42" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
+    <hyperlink ref="E174" r:id="rId43" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId44"/>

</xml_diff>

<commit_message>
Updated 1400 to match As-Built
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265A88C-4C1B-4C7D-947F-FB92AE1D1C87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A6F6A-A33A-4DDB-A60D-22F9FA25FB23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Q8 -&gt; Q18</t>
   </si>
   <si>
-    <t>R16 -&gt; R37</t>
-  </si>
-  <si>
     <t>273-1.0K-RC</t>
   </si>
   <si>
@@ -648,7 +645,28 @@
     <t>J39</t>
   </si>
   <si>
-    <t>DWG 1320 BILL OF MATERIALS (BOM)</t>
+    <t>R16 -&gt; R26</t>
+  </si>
+  <si>
+    <t>R27 -&gt; R37</t>
+  </si>
+  <si>
+    <t>RES 220 OHMS 1/2W AXIAL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nte-electronics-inc/HWCC122/11654401</t>
+  </si>
+  <si>
+    <t>HWCC122</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/2N3906/603429</t>
+  </si>
+  <si>
+    <t>TRANS PNP 40V 0.2A TO-92</t>
+  </si>
+  <si>
+    <t>2N3906</t>
   </si>
 </sst>
 </file>
@@ -869,7 +887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -916,18 +934,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1024,6 +1030,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1340,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,11 +1372,11 @@
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="87"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -1666,520 +1681,520 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D26" s="16"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="16"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D32" s="16"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D33" s="16"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D34" s="25"/>
     </row>
-    <row r="36" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
-      <c r="C36" s="37" t="s">
+    <row r="36" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="32"/>
+      <c r="C36" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="38"/>
-    </row>
-    <row r="37" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="D38" s="39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+    </row>
+    <row r="49" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="47"/>
+      <c r="C49" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="49"/>
+    </row>
+    <row r="50" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C50" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D50" s="29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="D38" s="43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D40" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D43" s="45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-    </row>
-    <row r="49" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="51"/>
-      <c r="C49" s="52" t="s">
+    <row r="51" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="53"/>
-    </row>
-    <row r="50" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="33" t="s">
+      <c r="D51" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+    </row>
+    <row r="58" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="56"/>
+      <c r="C58" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="58"/>
+    </row>
+    <row r="59" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="54" t="s">
+      <c r="C59" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D59" s="29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="42" t="s">
+    <row r="60" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="D51" s="49" t="s">
+    </row>
+    <row r="61" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="64" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="55" t="s">
+      <c r="D61" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="D53" s="56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="55" t="s">
-        <v>175</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="55" t="s">
+    </row>
+    <row r="62" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="56" t="s">
+    </row>
+    <row r="63" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C63" s="64" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="C56" s="57" t="s">
+      <c r="D63" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="D56" s="58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-    </row>
-    <row r="58" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="60"/>
-      <c r="C58" s="61" t="s">
-        <v>178</v>
-      </c>
-      <c r="D58" s="62"/>
-    </row>
-    <row r="59" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="33" t="s">
+    </row>
+    <row r="64" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="D64" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="64" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" s="52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D67" s="54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+    </row>
+    <row r="69" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="61"/>
+      <c r="C69" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="D69" s="63"/>
+    </row>
+    <row r="70" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C59" s="79" t="s">
+      <c r="C70" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="33" t="s">
+      <c r="D70" s="29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C60" s="42" t="s">
+    <row r="71" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="49" t="s">
+    </row>
+    <row r="72" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="64" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="68" t="s">
+      <c r="D72" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="D61" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" s="68" t="s">
+    </row>
+    <row r="73" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="D62" s="56" t="s">
+    </row>
+    <row r="74" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="53" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="C63" s="68" t="s">
+      <c r="D74" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="D64" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C65" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66" s="68" t="s">
-        <v>181</v>
-      </c>
-      <c r="D66" s="56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="58" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
-    </row>
-    <row r="69" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="65"/>
-      <c r="C69" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="D69" s="67"/>
-    </row>
-    <row r="70" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="79" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" s="33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C71" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="D71" s="49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="D72" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="C73" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="D73" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="C74" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="D74" s="58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="63"/>
-      <c r="C75" s="63"/>
-      <c r="D75" s="63"/>
+    </row>
+    <row r="75" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="59"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="59"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="31"/>
-      <c r="D76" s="32"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="87"/>
       <c r="E76" s="12"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2361,142 +2376,142 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D89" s="16"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D90" s="16"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D91" s="16"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D92" s="25"/>
     </row>
-    <row r="94" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="70"/>
-      <c r="C94" s="71" t="s">
+    <row r="94" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="66"/>
+      <c r="C94" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="D94" s="68"/>
+    </row>
+    <row r="95" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D96" s="39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D94" s="72"/>
-    </row>
-    <row r="95" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C95" s="79" t="s">
-        <v>2</v>
-      </c>
-      <c r="D95" s="33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C96" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="D96" s="43" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="44" t="s">
+      <c r="C97" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="74" t="s">
+      <c r="D97" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="D97" s="56" t="s">
+    </row>
+    <row r="98" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="40" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="44" t="s">
+      <c r="C98" s="70" t="s">
+        <v>156</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="D99" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="C98" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="D98" s="45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C99" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="D99" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="44" t="s">
+      <c r="C100" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D100" s="52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="C100" s="74" t="s">
-        <v>190</v>
-      </c>
-      <c r="D100" s="56" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="C101" s="74" t="s">
+      <c r="C101" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="D101" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="D101" s="56" t="s">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="53" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C102" s="57" t="s">
+      <c r="D102" s="54" t="s">
         <v>183</v>
-      </c>
-      <c r="D102" s="58" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
-      <c r="B104" s="30" t="s">
+      <c r="B104" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="C104" s="31"/>
-      <c r="D104" s="32"/>
+      <c r="C104" s="86"/>
+      <c r="D104" s="87"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
@@ -2573,7 +2588,7 @@
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>14</v>
@@ -2588,7 +2603,7 @@
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>16</v>
@@ -2602,771 +2617,765 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D112" s="25"/>
     </row>
-    <row r="114" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="C114" s="31"/>
-      <c r="D114" s="32"/>
-    </row>
-    <row r="115" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="17" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="14"/>
+      <c r="B114" s="85" t="s">
+        <v>99</v>
+      </c>
+      <c r="C114" s="86"/>
+      <c r="D114" s="87"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="14"/>
+      <c r="B115" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C115" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D115" s="17" t="s">
+      <c r="D115" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="E115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="14"/>
+      <c r="B116" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C116" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D116" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="14"/>
+      <c r="B117" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D117" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="14"/>
+      <c r="B118" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" s="13">
+        <v>533751110</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
-      <c r="B119" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C119" s="31"/>
-      <c r="D119" s="32"/>
+      <c r="B119" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
-      <c r="B120" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E120" t="s">
-        <v>3</v>
+      <c r="B120" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D120" s="13">
+        <v>971050154</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
-      <c r="B121" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C121" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D121" s="20" t="s">
-        <v>77</v>
+      <c r="B121" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C121" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D122" s="13">
-        <v>533750210</v>
+        <v>204</v>
+      </c>
+      <c r="C122" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C123" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D123" s="13">
-        <v>533751110</v>
+        <v>205</v>
+      </c>
+      <c r="C123" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="E123" s="12" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C124" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D124" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E124" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="B124" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D124" s="16"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C125" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D125" s="13">
-        <v>971050154</v>
-      </c>
-      <c r="E125" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D126" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E126" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C127" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D127" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E127" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D128" s="16"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C129" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D129" s="25"/>
-    </row>
-    <row r="130" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="26"/>
-      <c r="C130" s="6"/>
-      <c r="D130" s="73"/>
-    </row>
-    <row r="131" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="76"/>
-      <c r="C131" s="77" t="s">
+      <c r="B125" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D125" s="25"/>
+    </row>
+    <row r="126" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="26"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="69"/>
+    </row>
+    <row r="127" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="72"/>
+      <c r="C127" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="D127" s="74"/>
+    </row>
+    <row r="128" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="D131" s="78"/>
-    </row>
-    <row r="132" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="33" t="s">
+      <c r="C129" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D129" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C130" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="D130" s="54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="21"/>
+      <c r="B132" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="C132" s="86"/>
+      <c r="D132" s="87"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14"/>
+      <c r="B133" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="79" t="s">
+      <c r="C133" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D132" s="33" t="s">
+      <c r="D133" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="C133" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="D133" s="49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C134" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="D134" s="58" t="s">
-        <v>172</v>
+      <c r="E133" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="14"/>
+      <c r="B134" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D134" s="13">
+        <v>987</v>
+      </c>
+      <c r="E134" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14"/>
+      <c r="B135" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E135" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="21"/>
-      <c r="B136" s="30" t="s">
+      <c r="A136" s="14"/>
+      <c r="B136" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C136" s="31"/>
-      <c r="D136" s="32"/>
+      <c r="C136" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D136" s="13"/>
+      <c r="E136" s="12"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
-      <c r="B137" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E137" t="s">
-        <v>3</v>
+      <c r="B137" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D137" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="5" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D138" s="13">
-        <v>987</v>
+        <v>23</v>
+      </c>
+      <c r="D138" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="E138" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D139" s="13" t="s">
-        <v>105</v>
+        <v>20</v>
+      </c>
+      <c r="D139" s="13">
+        <v>533750210</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
-      <c r="B140" s="5" t="s">
-        <v>102</v>
+      <c r="B140" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D140" s="13"/>
-      <c r="E140" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="D140" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D141" s="13" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D141" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E141" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D142" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
+      </c>
+      <c r="D142" s="13">
+        <v>533750210</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D143" s="13">
-        <v>533750210</v>
+        <v>533750510</v>
       </c>
       <c r="E143" s="12" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D144" s="13">
+        <v>971050154</v>
+      </c>
+      <c r="E144" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C145" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D145" s="16"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C146" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D146" s="16"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C147" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D147" s="16"/>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C148" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D148" s="16"/>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C149" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D149" s="25"/>
+    </row>
+    <row r="151" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="76"/>
+      <c r="C151" s="77" t="s">
+        <v>196</v>
+      </c>
+      <c r="D151" s="78"/>
+    </row>
+    <row r="152" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D152" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C153" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D153" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C154" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D154" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D144" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E144" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
-      <c r="B145" s="5" t="s">
+      <c r="C155" s="79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D155" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C156" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D156" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C145" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D145" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E145" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
-      <c r="B146" s="5" t="s">
+      <c r="C157" s="79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D157" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C158" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D158" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="C159" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="D159" s="52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C146" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D146" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E146" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
-      <c r="B147" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D147" s="13">
-        <v>533750510</v>
-      </c>
-      <c r="E147" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
-      <c r="B148" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C148" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D148" s="13">
-        <v>971050154</v>
-      </c>
-      <c r="E148" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C149" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="D149" s="16"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C150" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D150" s="16"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B151" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C151" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D151" s="16"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C152" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D152" s="16"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B153" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C153" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="D153" s="25"/>
-    </row>
-    <row r="155" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="80"/>
-      <c r="C155" s="81" t="s">
-        <v>197</v>
-      </c>
-      <c r="D155" s="82"/>
-    </row>
-    <row r="156" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="33" t="s">
+      <c r="C160" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D160" s="54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="23"/>
+      <c r="B162" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C162" s="86"/>
+      <c r="D162" s="87"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="23"/>
+      <c r="B163" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C156" s="87" t="s">
+      <c r="C163" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D156" s="33" t="s">
+      <c r="D163" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C157" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="D157" s="49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="C158" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="D158" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C159" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="D159" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="C160" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="D160" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="C161" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="D161" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="C162" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="D162" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="44" t="s">
-        <v>201</v>
-      </c>
-      <c r="C163" s="83" t="s">
-        <v>181</v>
-      </c>
-      <c r="D163" s="56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="C164" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="D164" s="58" t="s">
-        <v>184</v>
-      </c>
+      <c r="E163" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="23"/>
+      <c r="B164" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C164" s="10"/>
+      <c r="D164" s="16"/>
+      <c r="E164" s="10"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="23"/>
+      <c r="B165" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D165" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="23"/>
-      <c r="B166" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="C166" s="31"/>
-      <c r="D166" s="32"/>
+      <c r="B166" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D166" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E166" s="22" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="23"/>
-      <c r="B167" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E167" t="s">
-        <v>3</v>
+      <c r="B167" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D167" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E167" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="23"/>
       <c r="B168" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C168" s="10"/>
-      <c r="D168" s="16"/>
-      <c r="E168" s="10"/>
+        <v>117</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D168" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E168" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="23"/>
-      <c r="B169" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D169" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E169" s="10"/>
+      <c r="B169" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D169" s="13">
+        <v>533750210</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="23"/>
-      <c r="B170" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D170" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="E170" s="22" t="s">
-        <v>21</v>
+      <c r="B170" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D170" s="13">
+        <v>971050154</v>
+      </c>
+      <c r="E170" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="23"/>
       <c r="B171" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D171" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E171" s="12" t="s">
-        <v>19</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C171" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D171" s="16"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="23"/>
       <c r="B172" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C172" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D172" s="16"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B173" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C173" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D173" s="25"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B175" s="80"/>
+      <c r="C175" s="81" t="s">
+        <v>201</v>
+      </c>
+      <c r="D175" s="82"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C177" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D177" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="C178" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="D178" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C172" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D172" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E172" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="23"/>
-      <c r="B173" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D173" s="13">
-        <v>533750210</v>
-      </c>
-      <c r="E173" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="23"/>
-      <c r="B174" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C174" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D174" s="13">
-        <v>971050154</v>
-      </c>
-      <c r="E174" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B175" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C175" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="D175" s="16"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B176" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C176" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D176" s="16"/>
-    </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C177" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="D177" s="25"/>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="84"/>
-      <c r="C179" s="85" t="s">
-        <v>202</v>
-      </c>
-      <c r="D179" s="86"/>
+      <c r="C179" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="D179" s="52" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C180" s="87" t="s">
-        <v>2</v>
-      </c>
-      <c r="D180" s="33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C181" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="D181" s="49" t="s">
+      <c r="B180" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="C180" s="53" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="C182" s="88" t="s">
+      <c r="D180" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="D182" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="C183" s="88" t="s">
-        <v>169</v>
-      </c>
-      <c r="D183" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="C184" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="D184" s="58" t="s">
-        <v>172</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B166:D166"/>
+  <mergeCells count="6">
+    <mergeCell ref="B162:D162"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B136:D136"/>
     <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B132:D132"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3393,28 +3402,27 @@
     <hyperlink ref="E81" r:id="rId21" xr:uid="{04D0839B-BA7C-4F4D-B91C-97A8EFF84E0C}"/>
     <hyperlink ref="E79" r:id="rId22" xr:uid="{ACB98E67-2E7B-454D-8E93-7B836B3D7957}"/>
     <hyperlink ref="E78" r:id="rId23" xr:uid="{CBCE2BBD-E319-4CA5-99FD-4235DF810FC4}"/>
-    <hyperlink ref="E123" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
-    <hyperlink ref="E122" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
-    <hyperlink ref="E124" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
-    <hyperlink ref="E125" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
-    <hyperlink ref="E126" r:id="rId28" xr:uid="{36F7B2D2-11D1-453F-98B7-7E472CCC4124}"/>
-    <hyperlink ref="E127" r:id="rId29" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
-    <hyperlink ref="E138" r:id="rId30" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
-    <hyperlink ref="E139" r:id="rId31" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
-    <hyperlink ref="E142" r:id="rId32" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
-    <hyperlink ref="E148" r:id="rId33" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
-    <hyperlink ref="E143" r:id="rId34" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
-    <hyperlink ref="E144" r:id="rId35" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
-    <hyperlink ref="E145" r:id="rId36" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
-    <hyperlink ref="E146" r:id="rId37" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
-    <hyperlink ref="E147" r:id="rId38" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
-    <hyperlink ref="E171" r:id="rId39" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
-    <hyperlink ref="E172" r:id="rId40" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
-    <hyperlink ref="E173" r:id="rId41" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
-    <hyperlink ref="E170" r:id="rId42" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
-    <hyperlink ref="E174" r:id="rId43" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
+    <hyperlink ref="E118" r:id="rId24" xr:uid="{964F9BFE-3F85-478B-BE16-DC540DA6255B}"/>
+    <hyperlink ref="E117" r:id="rId25" xr:uid="{6B5DF9A6-B01D-4A52-85BE-17EC844E8CD5}"/>
+    <hyperlink ref="E119" r:id="rId26" xr:uid="{F79CFCAE-30B3-4BDF-B763-FF7F83A03541}"/>
+    <hyperlink ref="E120" r:id="rId27" xr:uid="{C412421B-9FFF-4FA7-9E4B-5B88A5288D74}"/>
+    <hyperlink ref="E122" r:id="rId28" xr:uid="{D347444D-B462-492B-BC36-69914A70B602}"/>
+    <hyperlink ref="E134" r:id="rId29" xr:uid="{79E5E570-88DB-40D2-86C1-EAB35681E040}"/>
+    <hyperlink ref="E135" r:id="rId30" xr:uid="{48DCCD76-8BD4-475C-96E1-939DAC0D93DA}"/>
+    <hyperlink ref="E138" r:id="rId31" xr:uid="{4760709C-1393-4566-982E-1FBA333654AE}"/>
+    <hyperlink ref="E144" r:id="rId32" xr:uid="{D507F27E-0D18-453C-84F2-7307990B31DD}"/>
+    <hyperlink ref="E139" r:id="rId33" xr:uid="{7CD25257-B159-4B84-BA4A-6348227685EF}"/>
+    <hyperlink ref="E140" r:id="rId34" xr:uid="{32279395-901C-4F0D-ACCF-D79AC47D78E0}"/>
+    <hyperlink ref="E141" r:id="rId35" xr:uid="{6FBDFDF2-234C-43FD-98A8-8855819E06A3}"/>
+    <hyperlink ref="E142" r:id="rId36" xr:uid="{C0DEACAA-B774-430B-972D-7DFB7802F0D1}"/>
+    <hyperlink ref="E143" r:id="rId37" xr:uid="{0D03B124-EF64-4C0F-B839-C06176246E0A}"/>
+    <hyperlink ref="E167" r:id="rId38" xr:uid="{96111401-738F-44D0-934D-60024799877E}"/>
+    <hyperlink ref="E168" r:id="rId39" xr:uid="{62DB1079-D460-44E5-93B2-C692DFF7B660}"/>
+    <hyperlink ref="E169" r:id="rId40" xr:uid="{7ED49E06-C8D9-4C5B-BB47-4368A41DF864}"/>
+    <hyperlink ref="E166" r:id="rId41" xr:uid="{2CF67DDE-5EBF-433A-9052-71F1A52C54F6}"/>
+    <hyperlink ref="E170" r:id="rId42" xr:uid="{5FBEF90C-90D3-4649-BB08-43E8FAAD25BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId44"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OVERKILL, PURGE, EXPLODE, and rename all drawings
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A6F6A-A33A-4DDB-A60D-22F9FA25FB23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BBC32D-DD74-4183-921A-E5B85996AB29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
@@ -1357,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Merged BOM, updated BOM on a few drawings, editing 1800 for final print.
1800 isnt done yet, need to think about how it is being executed before finishing
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BBC32D-DD74-4183-921A-E5B85996AB29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600E0356-B9B0-4DA1-9112-AD08916CA678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="290">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -667,13 +667,247 @@
   </si>
   <si>
     <t>2N3906</t>
+  </si>
+  <si>
+    <t>DWG 1110 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Servo Motor</t>
+  </si>
+  <si>
+    <t>SER-M-001</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Rotary Encoder</t>
+  </si>
+  <si>
+    <t>288T232R161A1</t>
+  </si>
+  <si>
+    <t>3-Pin  Male Molex Connector</t>
+  </si>
+  <si>
+    <t>3-M-MOLEX</t>
+  </si>
+  <si>
+    <t>DWG 1111 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>2-Pin  Male Molex Connector</t>
+  </si>
+  <si>
+    <t>2-M-MOLEX</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>NO-Push Button (Confirm Button)</t>
+  </si>
+  <si>
+    <t>PB-001</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>NO-Push Button (Reset Button)</t>
+  </si>
+  <si>
+    <t>PB-002</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>NO-Push Button (Send Power Button)</t>
+  </si>
+  <si>
+    <t>PB-003</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>NO-Push Button (Phone Switch)</t>
+  </si>
+  <si>
+    <t>PB-004</t>
+  </si>
+  <si>
+    <t>DWG 1610 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2-Pin Male Molex Connector</t>
+  </si>
+  <si>
+    <t>DS1</t>
+  </si>
+  <si>
+    <t>60W LED Light-Bulb</t>
+  </si>
+  <si>
+    <t>LED-60</t>
+  </si>
+  <si>
+    <t>DWG 1210 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>Homing Switch</t>
+  </si>
+  <si>
+    <t>Z6535-ND</t>
+  </si>
+  <si>
+    <t>4-Pin Male Molex Connector</t>
+  </si>
+  <si>
+    <t>4-M-MOLEX</t>
+  </si>
+  <si>
+    <t>7-Pin Male Molex Connector</t>
+  </si>
+  <si>
+    <t>7-M-MOLEX</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>DC Motor</t>
+  </si>
+  <si>
+    <t>2790-PC280LG-302-ND</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>1568-1105-ND</t>
+  </si>
+  <si>
+    <t>DWG 1510 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>2-Pin Male Molex Connector</t>
+  </si>
+  <si>
+    <t>LS1</t>
+  </si>
+  <si>
+    <t>Phone speaker</t>
+  </si>
+  <si>
+    <t>2056-K64WP-8OHM-ND</t>
+  </si>
+  <si>
+    <t>LS2</t>
+  </si>
+  <si>
+    <t>Left Main Speaker</t>
+  </si>
+  <si>
+    <t>LS3</t>
+  </si>
+  <si>
+    <t>Right Main Speaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      DWG 1800 BILL OF MATERIALS (BOM)</t>
+  </si>
+  <si>
+    <t>SSR</t>
+  </si>
+  <si>
+    <t>AQH3213</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>HP Desktop Monitor</t>
+  </si>
+  <si>
+    <t>L1702</t>
+  </si>
+  <si>
+    <t>+5V Power Supply</t>
+  </si>
+  <si>
+    <t>1470-LCW35US05-ND</t>
+  </si>
+  <si>
+    <t>+12V Power Supply</t>
+  </si>
+  <si>
+    <t>1470-LCW35US12-ND</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>4A Fuse Rated</t>
+  </si>
+  <si>
+    <t>507-1298-ND</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A Fuse Rated </t>
+  </si>
+  <si>
+    <t>0232001.MX125P-ND</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>1A Fuse Rated</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>0.15A Fuse</t>
+  </si>
+  <si>
+    <t>0239.150MXP-ND</t>
+  </si>
+  <si>
+    <t>REFFERENCE DRAWING 1600</t>
+  </si>
+  <si>
+    <t>SOLID STATE RELAY</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>PS2</t>
+  </si>
+  <si>
+    <t>PS3</t>
+  </si>
+  <si>
+    <t>+5 Raspberry Pi Power supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,6 +935,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -716,7 +956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -882,12 +1122,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1040,6 +1291,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1355,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:S192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E173" sqref="E173"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182:D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,18 +1645,36 @@
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="71" customWidth="1"/>
+    <col min="18" max="18" width="34.7109375" style="71" customWidth="1"/>
+    <col min="19" max="19" width="21" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="88" t="s">
+        <v>212</v>
+      </c>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="85" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="86"/>
       <c r="D2" s="87"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q2" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1392,8 +1688,17 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="R3" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -1407,8 +1712,17 @@
       <c r="E4" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q4" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R4" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
         <v>54</v>
@@ -1422,8 +1736,17 @@
       <c r="E5" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="8" t="s">
         <v>56</v>
@@ -1437,8 +1760,17 @@
       <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="R6" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="S6" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -1452,8 +1784,17 @@
       <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="8" t="s">
         <v>58</v>
@@ -1467,8 +1808,17 @@
       <c r="E8" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
         <v>57</v>
@@ -1482,8 +1832,17 @@
       <c r="E9" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q9" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="R9" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="S9" s="52" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>28</v>
@@ -1497,8 +1856,17 @@
       <c r="E10" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q10" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="R10" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="8" t="s">
         <v>59</v>
@@ -1512,8 +1880,17 @@
       <c r="E11" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q11" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="R11" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="S11" s="52" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
         <v>79</v>
@@ -1527,8 +1904,17 @@
       <c r="E12" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q12" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="R12" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="S12" s="41" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="8" t="s">
         <v>80</v>
@@ -1542,8 +1928,17 @@
       <c r="E13" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q13" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="R13" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="S13" s="41" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="8" t="s">
         <v>81</v>
@@ -1557,8 +1952,17 @@
       <c r="E14" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q14" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="R14" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="S14" s="54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="8" t="s">
         <v>82</v>
@@ -1572,8 +1976,15 @@
       <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q15" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="R15" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="S15" s="90"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="8" t="s">
         <v>78</v>
@@ -1587,8 +1998,15 @@
       <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q16" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="R16" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>83</v>
@@ -1603,7 +2021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
         <v>64</v>
@@ -1617,8 +2035,13 @@
       <c r="E18" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q18" s="88" t="s">
+        <v>221</v>
+      </c>
+      <c r="R18" s="88"/>
+      <c r="S18" s="88"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>65</v>
@@ -1632,8 +2055,17 @@
       <c r="E19" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q19" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>66</v>
@@ -1647,8 +2079,17 @@
       <c r="E20" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q20" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="R20" s="89" t="s">
+        <v>222</v>
+      </c>
+      <c r="S20" s="90" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>67</v>
@@ -1662,8 +2103,17 @@
       <c r="E21" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q21" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="R21" s="89" t="s">
+        <v>222</v>
+      </c>
+      <c r="S21" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>55</v>
@@ -1677,8 +2127,17 @@
       <c r="E22" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q22" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="R22" s="89" t="s">
+        <v>222</v>
+      </c>
+      <c r="S22" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>122</v>
@@ -1688,8 +2147,17 @@
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q23" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="R23" s="89" t="s">
+        <v>222</v>
+      </c>
+      <c r="S23" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>123</v>
       </c>
@@ -1697,8 +2165,17 @@
         <v>144</v>
       </c>
       <c r="D24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q24" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="R24" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="S24" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>124</v>
       </c>
@@ -1706,8 +2183,17 @@
         <v>144</v>
       </c>
       <c r="D25" s="16"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q25" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="R25" s="89" t="s">
+        <v>228</v>
+      </c>
+      <c r="S25" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>125</v>
       </c>
@@ -1715,8 +2201,17 @@
         <v>145</v>
       </c>
       <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q26" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="R26" s="89" t="s">
+        <v>231</v>
+      </c>
+      <c r="S26" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>126</v>
       </c>
@@ -1724,8 +2219,17 @@
         <v>145</v>
       </c>
       <c r="D27" s="16"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q27" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="R27" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="S27" s="25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>127</v>
       </c>
@@ -1733,8 +2237,15 @@
         <v>145</v>
       </c>
       <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q28" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="R28" s="89" t="s">
+        <v>145</v>
+      </c>
+      <c r="S28" s="16"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>128</v>
       </c>
@@ -1742,8 +2253,15 @@
         <v>146</v>
       </c>
       <c r="D29" s="16"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q29" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="R29" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="S29" s="16"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>129</v>
       </c>
@@ -1751,8 +2269,15 @@
         <v>146</v>
       </c>
       <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q30" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="R30" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="S30" s="16"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>130</v>
       </c>
@@ -1760,8 +2285,15 @@
         <v>146</v>
       </c>
       <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q31" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="R31" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="S31" s="25"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>131</v>
       </c>
@@ -1770,7 +2302,7 @@
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>132</v>
       </c>
@@ -1778,8 +2310,13 @@
         <v>147</v>
       </c>
       <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="Q33" s="88" t="s">
+        <v>236</v>
+      </c>
+      <c r="R33" s="88"/>
+      <c r="S33" s="88"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
         <v>133</v>
       </c>
@@ -1787,15 +2324,44 @@
         <v>147</v>
       </c>
       <c r="D34" s="25"/>
-    </row>
-    <row r="36" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q34" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="R34" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q35" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="R35" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="S35" s="90" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="33" t="s">
         <v>152</v>
       </c>
       <c r="D36" s="34"/>
-    </row>
-    <row r="37" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q36" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="R36" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="S36" s="25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
         <v>0</v>
       </c>
@@ -1805,8 +2371,15 @@
       <c r="D37" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="R37" s="92" t="s">
+        <v>151</v>
+      </c>
+      <c r="S37" s="82"/>
+    </row>
+    <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="37" t="s">
         <v>56</v>
       </c>
@@ -1816,8 +2389,11 @@
       <c r="D38" s="39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="93"/>
+    </row>
+    <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="40" t="s">
         <v>155</v>
       </c>
@@ -1827,8 +2403,13 @@
       <c r="D39" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="R39" s="86"/>
+      <c r="S39" s="87"/>
+    </row>
+    <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="40" t="s">
         <v>158</v>
       </c>
@@ -1838,8 +2419,17 @@
       <c r="D40" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q40" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="R40" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="S40" s="83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="40" t="s">
         <v>159</v>
       </c>
@@ -1849,8 +2439,17 @@
       <c r="D41" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R41" s="71" t="s">
+        <v>242</v>
+      </c>
+      <c r="S41" s="94" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="40" t="s">
         <v>160</v>
       </c>
@@ -1860,8 +2459,17 @@
       <c r="D42" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q42" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="R42" s="89" t="s">
+        <v>244</v>
+      </c>
+      <c r="S42" s="52" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="40" t="s">
         <v>58</v>
       </c>
@@ -1871,8 +2479,17 @@
       <c r="D43" s="41" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="Q43" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="R43" s="89" t="s">
+        <v>246</v>
+      </c>
+      <c r="S43" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" s="40" t="s">
         <v>163</v>
       </c>
@@ -1882,8 +2499,17 @@
       <c r="D44" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="Q44" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="R44" s="95" t="s">
+        <v>249</v>
+      </c>
+      <c r="S44" s="96" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" s="40" t="s">
         <v>164</v>
       </c>
@@ -1893,8 +2519,17 @@
       <c r="D45" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="Q45" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="R45" s="95" t="s">
+        <v>252</v>
+      </c>
+      <c r="S45" s="96" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" s="40" t="s">
         <v>57</v>
       </c>
@@ -1904,8 +2539,15 @@
       <c r="D46" s="41" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="Q46" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="R46" s="95" t="s">
+        <v>148</v>
+      </c>
+      <c r="S46" s="16"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" s="42" t="s">
         <v>62</v>
       </c>
@@ -1915,20 +2557,35 @@
       <c r="D47" s="44" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q47" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="R47" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="S47" s="25"/>
+    </row>
+    <row r="48" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="35"/>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
-    </row>
-    <row r="49" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="71"/>
+      <c r="R48" s="71"/>
+      <c r="S48" s="71"/>
+    </row>
+    <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="47"/>
       <c r="C49" s="48" t="s">
         <v>167</v>
       </c>
       <c r="D49" s="49"/>
-    </row>
-    <row r="50" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q49" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="R49" s="86"/>
+      <c r="S49" s="87"/>
+    </row>
+    <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="29" t="s">
         <v>0</v>
       </c>
@@ -1938,8 +2595,17 @@
       <c r="D50" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q50" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="R50" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="S50" s="83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="37" t="s">
         <v>59</v>
       </c>
@@ -1949,8 +2615,17 @@
       <c r="D51" s="45" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q51" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="R51" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="S51" s="52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="40" t="s">
         <v>107</v>
       </c>
@@ -1960,8 +2635,17 @@
       <c r="D52" s="41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q52" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="R52" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="S52" s="52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="40" t="s">
         <v>5</v>
       </c>
@@ -1971,8 +2655,17 @@
       <c r="D53" s="52" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q53" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="R53" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="S53" s="52" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="40" t="s">
         <v>92</v>
       </c>
@@ -1982,8 +2675,17 @@
       <c r="D54" s="41" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q54" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R54" s="95" t="s">
+        <v>257</v>
+      </c>
+      <c r="S54" s="96" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="40" t="s">
         <v>80</v>
       </c>
@@ -1993,8 +2695,17 @@
       <c r="D55" s="52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q55" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="R55" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="S55" s="96" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="42" t="s">
         <v>176</v>
       </c>
@@ -2004,20 +2715,43 @@
       <c r="D56" s="54" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q56" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="R56" s="95" t="s">
+        <v>262</v>
+      </c>
+      <c r="S56" s="96" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="51"/>
-    </row>
-    <row r="58" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q57" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="R57" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="S57" s="96"/>
+    </row>
+    <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="56"/>
       <c r="C58" s="57" t="s">
         <v>177</v>
       </c>
       <c r="D58" s="58"/>
-    </row>
-    <row r="59" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q58" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="R58" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="S58" s="16"/>
+    </row>
+    <row r="59" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="29" t="s">
         <v>0</v>
       </c>
@@ -2027,8 +2761,15 @@
       <c r="D59" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q59" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="R59" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="S59" s="25"/>
+    </row>
+    <row r="60" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="37" t="s">
         <v>81</v>
       </c>
@@ -2038,8 +2779,11 @@
       <c r="D60" s="45" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q60" s="71"/>
+      <c r="R60" s="71"/>
+      <c r="S60" s="71"/>
+    </row>
+    <row r="61" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="40" t="s">
         <v>178</v>
       </c>
@@ -2049,8 +2793,11 @@
       <c r="D61" s="41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q61" s="71"/>
+      <c r="R61" s="71"/>
+      <c r="S61" s="71"/>
+    </row>
+    <row r="62" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="40" t="s">
         <v>82</v>
       </c>
@@ -2060,8 +2807,11 @@
       <c r="D62" s="52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q62" s="71"/>
+      <c r="R62" s="71"/>
+      <c r="S62" s="71"/>
+    </row>
+    <row r="63" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="40" t="s">
         <v>179</v>
       </c>
@@ -2071,8 +2821,11 @@
       <c r="D63" s="41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q63" s="71"/>
+      <c r="R63" s="71"/>
+      <c r="S63" s="71"/>
+    </row>
+    <row r="64" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="40" t="s">
         <v>83</v>
       </c>
@@ -2082,8 +2835,11 @@
       <c r="D64" s="52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q64" s="71"/>
+      <c r="R64" s="71"/>
+      <c r="S64" s="71"/>
+    </row>
+    <row r="65" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="40" t="s">
         <v>121</v>
       </c>
@@ -2093,8 +2849,11 @@
       <c r="D65" s="41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q65" s="71"/>
+      <c r="R65" s="71"/>
+      <c r="S65" s="71"/>
+    </row>
+    <row r="66" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="40" t="s">
         <v>28</v>
       </c>
@@ -2104,8 +2863,11 @@
       <c r="D66" s="52" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q66" s="71"/>
+      <c r="R66" s="71"/>
+      <c r="S66" s="71"/>
+    </row>
+    <row r="67" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="42" t="s">
         <v>18</v>
       </c>
@@ -2115,20 +2877,29 @@
       <c r="D67" s="54" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q67" s="71"/>
+      <c r="R67" s="71"/>
+      <c r="S67" s="71"/>
+    </row>
+    <row r="68" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="51"/>
       <c r="C68" s="51"/>
       <c r="D68" s="51"/>
-    </row>
-    <row r="69" spans="1:5" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q68" s="71"/>
+      <c r="R68" s="71"/>
+      <c r="S68" s="71"/>
+    </row>
+    <row r="69" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="61"/>
       <c r="C69" s="62" t="s">
         <v>184</v>
       </c>
       <c r="D69" s="63"/>
-    </row>
-    <row r="70" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q69" s="71"/>
+      <c r="R69" s="71"/>
+      <c r="S69" s="71"/>
+    </row>
+    <row r="70" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
         <v>0</v>
       </c>
@@ -2138,8 +2909,11 @@
       <c r="D70" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q70" s="71"/>
+      <c r="R70" s="71"/>
+      <c r="S70" s="71"/>
+    </row>
+    <row r="71" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="37" t="s">
         <v>185</v>
       </c>
@@ -2149,8 +2923,11 @@
       <c r="D71" s="45" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q71" s="71"/>
+      <c r="R71" s="71"/>
+      <c r="S71" s="71"/>
+    </row>
+    <row r="72" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="40" t="s">
         <v>79</v>
       </c>
@@ -2160,8 +2937,11 @@
       <c r="D72" s="41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q72" s="71"/>
+      <c r="R72" s="71"/>
+      <c r="S72" s="71"/>
+    </row>
+    <row r="73" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="40" t="s">
         <v>78</v>
       </c>
@@ -2171,8 +2951,11 @@
       <c r="D73" s="52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q73" s="71"/>
+      <c r="R73" s="71"/>
+      <c r="S73" s="71"/>
+    </row>
+    <row r="74" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="42" t="s">
         <v>186</v>
       </c>
@@ -2182,13 +2965,19 @@
       <c r="D74" s="54" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q74" s="71"/>
+      <c r="R74" s="71"/>
+      <c r="S74" s="71"/>
+    </row>
+    <row r="75" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="59"/>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q75" s="71"/>
+      <c r="R75" s="71"/>
+      <c r="S75" s="71"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="85" t="s">
         <v>73</v>
@@ -2197,7 +2986,7 @@
       <c r="D76" s="87"/>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="1" t="s">
         <v>0</v>
@@ -2212,7 +3001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="8" t="s">
         <v>47</v>
@@ -2227,7 +3016,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" s="8" t="s">
         <v>60</v>
@@ -2242,7 +3031,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="14"/>
       <c r="B80" s="8" t="s">
         <v>61</v>
@@ -2254,7 +3043,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="14"/>
       <c r="B81" s="8" t="s">
         <v>85</v>
@@ -2269,7 +3058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
       <c r="B82" s="8" t="s">
         <v>62</v>
@@ -2284,7 +3073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="14"/>
       <c r="B83" s="8" t="s">
         <v>63</v>
@@ -2299,7 +3088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="B84" s="8" t="s">
         <v>84</v>
@@ -2314,7 +3103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="14"/>
       <c r="B85" s="8" t="s">
         <v>64</v>
@@ -2329,7 +3118,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
       <c r="B86" s="8" t="s">
         <v>65</v>
@@ -2344,7 +3133,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="8" t="s">
         <v>66</v>
@@ -2359,7 +3148,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="8" t="s">
         <v>67</v>
@@ -2374,7 +3163,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
         <v>123</v>
       </c>
@@ -2383,7 +3172,7 @@
       </c>
       <c r="D89" s="16"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>135</v>
       </c>
@@ -2392,7 +3181,7 @@
       </c>
       <c r="D90" s="16"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>136</v>
       </c>
@@ -2401,7 +3190,7 @@
       </c>
       <c r="D91" s="16"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
         <v>134</v>
       </c>
@@ -2410,14 +3199,17 @@
       </c>
       <c r="D92" s="25"/>
     </row>
-    <row r="94" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="66"/>
       <c r="C94" s="67" t="s">
         <v>187</v>
       </c>
       <c r="D94" s="68"/>
-    </row>
-    <row r="95" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q94" s="71"/>
+      <c r="R94" s="71"/>
+      <c r="S94" s="71"/>
+    </row>
+    <row r="95" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="29" t="s">
         <v>0</v>
       </c>
@@ -2427,8 +3219,11 @@
       <c r="D95" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q95" s="71"/>
+      <c r="R95" s="71"/>
+      <c r="S95" s="71"/>
+    </row>
+    <row r="96" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="37" t="s">
         <v>85</v>
       </c>
@@ -2438,8 +3233,11 @@
       <c r="D96" s="39" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q96" s="71"/>
+      <c r="R96" s="71"/>
+      <c r="S96" s="71"/>
+    </row>
+    <row r="97" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="40" t="s">
         <v>188</v>
       </c>
@@ -2449,8 +3247,11 @@
       <c r="D97" s="52" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q97" s="71"/>
+      <c r="R97" s="71"/>
+      <c r="S97" s="71"/>
+    </row>
+    <row r="98" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="40" t="s">
         <v>191</v>
       </c>
@@ -2460,8 +3261,11 @@
       <c r="D98" s="41" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q98" s="71"/>
+      <c r="R98" s="71"/>
+      <c r="S98" s="71"/>
+    </row>
+    <row r="99" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="40" t="s">
         <v>63</v>
       </c>
@@ -2471,8 +3275,11 @@
       <c r="D99" s="52" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q99" s="71"/>
+      <c r="R99" s="71"/>
+      <c r="S99" s="71"/>
+    </row>
+    <row r="100" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="40" t="s">
         <v>192</v>
       </c>
@@ -2482,8 +3289,11 @@
       <c r="D100" s="52" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q100" s="71"/>
+      <c r="R100" s="71"/>
+      <c r="S100" s="71"/>
+    </row>
+    <row r="101" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
         <v>193</v>
       </c>
@@ -2493,8 +3303,11 @@
       <c r="D101" s="52" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q101" s="71"/>
+      <c r="R101" s="71"/>
+      <c r="S101" s="71"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B102" s="42" t="s">
         <v>84</v>
       </c>
@@ -2505,7 +3318,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
       <c r="B104" s="85" t="s">
         <v>86</v>
@@ -2513,7 +3326,7 @@
       <c r="C104" s="86"/>
       <c r="D104" s="87"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="17" t="s">
         <v>0</v>
@@ -2528,7 +3341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="2" t="s">
         <v>76</v>
@@ -2543,7 +3356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="2" t="s">
         <v>43</v>
@@ -2555,7 +3368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="2" t="s">
         <v>48</v>
@@ -2570,7 +3383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="2" t="s">
         <v>18</v>
@@ -2585,7 +3398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="2" t="s">
         <v>113</v>
@@ -2600,7 +3413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="2" t="s">
         <v>114</v>
@@ -2615,7 +3428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
         <v>131</v>
       </c>
@@ -2624,7 +3437,7 @@
       </c>
       <c r="D112" s="25"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="85" t="s">
         <v>99</v>
@@ -2632,7 +3445,7 @@
       <c r="C114" s="86"/>
       <c r="D114" s="87"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="1" t="s">
         <v>0</v>
@@ -2647,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="18" t="s">
         <v>44</v>
@@ -2659,7 +3472,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="5" t="s">
         <v>91</v>
@@ -2674,7 +3487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="5" t="s">
         <v>92</v>
@@ -2689,7 +3502,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="5" t="s">
         <v>93</v>
@@ -2704,7 +3517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="5" t="s">
         <v>94</v>
@@ -2719,7 +3532,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="5" t="s">
         <v>95</v>
@@ -2734,7 +3547,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="5" t="s">
         <v>204</v>
@@ -2749,7 +3562,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="5" t="s">
         <v>205</v>
@@ -2764,7 +3577,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>126</v>
       </c>
@@ -2773,7 +3586,7 @@
       </c>
       <c r="D124" s="16"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B125" s="4" t="s">
         <v>137</v>
       </c>
@@ -2782,19 +3595,25 @@
       </c>
       <c r="D125" s="25"/>
     </row>
-    <row r="126" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="26"/>
       <c r="C126" s="6"/>
       <c r="D126" s="69"/>
-    </row>
-    <row r="127" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q126" s="71"/>
+      <c r="R126" s="71"/>
+      <c r="S126" s="71"/>
+    </row>
+    <row r="127" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="72"/>
       <c r="C127" s="73" t="s">
         <v>194</v>
       </c>
       <c r="D127" s="74"/>
-    </row>
-    <row r="128" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q127" s="71"/>
+      <c r="R127" s="71"/>
+      <c r="S127" s="71"/>
+    </row>
+    <row r="128" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="29" t="s">
         <v>0</v>
       </c>
@@ -2804,8 +3623,11 @@
       <c r="D128" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q128" s="71"/>
+      <c r="R128" s="71"/>
+      <c r="S128" s="71"/>
+    </row>
+    <row r="129" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="37" t="s">
         <v>195</v>
       </c>
@@ -2815,8 +3637,11 @@
       <c r="D129" s="45" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q129" s="71"/>
+      <c r="R129" s="71"/>
+      <c r="S129" s="71"/>
+    </row>
+    <row r="130" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="42" t="s">
         <v>91</v>
       </c>
@@ -2826,8 +3651,11 @@
       <c r="D130" s="54" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q130" s="71"/>
+      <c r="R130" s="71"/>
+      <c r="S130" s="71"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="85" t="s">
         <v>100</v>
@@ -2835,7 +3663,7 @@
       <c r="C132" s="86"/>
       <c r="D132" s="87"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
       <c r="B133" s="1" t="s">
         <v>0</v>
@@ -2850,7 +3678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
       <c r="B134" s="5" t="s">
         <v>45</v>
@@ -2865,7 +3693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="5" t="s">
         <v>46</v>
@@ -2880,7 +3708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="5" t="s">
         <v>101</v>
@@ -2891,7 +3719,7 @@
       <c r="D136" s="13"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="5" t="s">
         <v>102</v>
@@ -2903,7 +3731,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="5" t="s">
         <v>103</v>
@@ -2918,7 +3746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
         <v>107</v>
@@ -2933,7 +3761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="2" t="s">
         <v>108</v>
@@ -2948,7 +3776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
         <v>109</v>
@@ -2963,7 +3791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="5" t="s">
         <v>110</v>
@@ -2978,7 +3806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="5" t="s">
         <v>111</v>
@@ -2993,7 +3821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="5" t="s">
         <v>94</v>
@@ -3187,8 +4015,12 @@
       <c r="B164" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C164" s="10"/>
-      <c r="D164" s="16"/>
+      <c r="C164" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D164" s="16" t="s">
+        <v>265</v>
+      </c>
       <c r="E164" s="10"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3368,8 +4200,126 @@
         <v>171</v>
       </c>
     </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="98"/>
+      <c r="C182" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="D182" s="100"/>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" s="101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="C184" s="102" t="s">
+        <v>284</v>
+      </c>
+      <c r="D184" s="101"/>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B185" s="102" t="s">
+        <v>266</v>
+      </c>
+      <c r="C185" s="102" t="s">
+        <v>267</v>
+      </c>
+      <c r="D185" s="102" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="103" t="s">
+        <v>286</v>
+      </c>
+      <c r="C186" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="D186" s="102" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="103" t="s">
+        <v>287</v>
+      </c>
+      <c r="C187" s="103" t="s">
+        <v>271</v>
+      </c>
+      <c r="D187" s="102" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="97" t="s">
+        <v>288</v>
+      </c>
+      <c r="C188" s="104" t="s">
+        <v>289</v>
+      </c>
+      <c r="D188" s="102"/>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B189" s="102" t="s">
+        <v>273</v>
+      </c>
+      <c r="C189" s="102" t="s">
+        <v>274</v>
+      </c>
+      <c r="D189" s="101" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="102" t="s">
+        <v>276</v>
+      </c>
+      <c r="C190" s="102" t="s">
+        <v>277</v>
+      </c>
+      <c r="D190" s="101" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="102" t="s">
+        <v>279</v>
+      </c>
+      <c r="C191" s="102" t="s">
+        <v>280</v>
+      </c>
+      <c r="D191" s="101" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="102" t="s">
+        <v>281</v>
+      </c>
+      <c r="C192" s="102" t="s">
+        <v>282</v>
+      </c>
+      <c r="D192" s="101" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q49:S49"/>
     <mergeCell ref="B162:D162"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B76:D76"/>

</xml_diff>

<commit_message>
Fixed some details in1121
standardized font size
all caps
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atboe\Documents\GitHub\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600E0356-B9B0-4DA1-9112-AD08916CA678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA296EE9-AA61-4970-8E79-CC5F84F846D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="293">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -549,15 +549,9 @@
     <t>2-F-MOLEX</t>
   </si>
   <si>
-    <t>11-Pin On-Board Male Crimp Connector</t>
-  </si>
-  <si>
     <t>53375-1210</t>
   </si>
   <si>
-    <t>11-Pin Female Molex Connector</t>
-  </si>
-  <si>
     <t>11-F-MOLEX</t>
   </si>
   <si>
@@ -675,24 +669,15 @@
     <t>M1</t>
   </si>
   <si>
-    <t>Servo Motor</t>
-  </si>
-  <si>
     <t>SER-M-001</t>
   </si>
   <si>
     <t>M2</t>
   </si>
   <si>
-    <t>Rotary Encoder</t>
-  </si>
-  <si>
     <t>288T232R161A1</t>
   </si>
   <si>
-    <t>3-Pin  Male Molex Connector</t>
-  </si>
-  <si>
     <t>3-M-MOLEX</t>
   </si>
   <si>
@@ -901,6 +886,30 @@
   </si>
   <si>
     <t>+5 Raspberry Pi Power supply</t>
+  </si>
+  <si>
+    <t>2-PIN FEMALE MOLEX CONNECTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-PIN MALE MOLEX MINI-LOCK CONNECTOR </t>
+  </si>
+  <si>
+    <t>2-Pin MALE MOLEX MINI-LOCK CONNECTOR</t>
+  </si>
+  <si>
+    <t>11-PIN FEMALE MOLEX CONNECTOR</t>
+  </si>
+  <si>
+    <t>2-PIN MALE MOLEX MINI-LOCK CONNECTOR</t>
+  </si>
+  <si>
+    <t>SERVO MOTOR</t>
+  </si>
+  <si>
+    <t>ROTARY ENCODER</t>
+  </si>
+  <si>
+    <t>3-PIN MALE MOLEX CONNECTOR</t>
   </si>
 </sst>
 </file>
@@ -1282,18 +1291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1318,6 +1315,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1635,35 +1644,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
   <dimension ref="A1:S192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182:D192"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" style="71" customWidth="1"/>
-    <col min="18" max="18" width="34.7109375" style="71" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" style="71" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" style="71" customWidth="1"/>
     <col min="19" max="19" width="21" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q1" s="88" t="s">
-        <v>212</v>
-      </c>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="104"/>
       <c r="Q2" s="83" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1689,16 +1698,16 @@
         <v>3</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R3" s="71" t="s">
-        <v>214</v>
+        <v>290</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -1713,16 +1722,16 @@
         <v>38</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="R4" s="71" t="s">
-        <v>214</v>
+        <v>290</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
         <v>54</v>
@@ -1739,14 +1748,14 @@
       <c r="Q5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="71" t="s">
-        <v>217</v>
+      <c r="R5" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="8" t="s">
         <v>56</v>
@@ -1763,14 +1772,14 @@
       <c r="Q6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="71" t="s">
-        <v>217</v>
+      <c r="R6" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -1787,14 +1796,14 @@
       <c r="Q7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R7" s="71" t="s">
-        <v>217</v>
+      <c r="R7" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="8" t="s">
         <v>58</v>
@@ -1811,14 +1820,14 @@
       <c r="Q8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="R8" s="71" t="s">
-        <v>217</v>
+      <c r="R8" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
         <v>57</v>
@@ -1835,14 +1844,14 @@
       <c r="Q9" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="R9" s="89" t="s">
-        <v>219</v>
+      <c r="R9" s="85" t="s">
+        <v>292</v>
       </c>
       <c r="S9" s="52" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>28</v>
@@ -1859,14 +1868,14 @@
       <c r="Q10" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="R10" s="89" t="s">
-        <v>219</v>
+      <c r="R10" s="85" t="s">
+        <v>292</v>
       </c>
       <c r="S10" s="41" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="8" t="s">
         <v>59</v>
@@ -1883,14 +1892,14 @@
       <c r="Q11" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="R11" s="89" t="s">
-        <v>219</v>
+      <c r="R11" s="85" t="s">
+        <v>292</v>
       </c>
       <c r="S11" s="52" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
         <v>79</v>
@@ -1907,14 +1916,14 @@
       <c r="Q12" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="R12" s="89" t="s">
-        <v>219</v>
+      <c r="R12" s="85" t="s">
+        <v>292</v>
       </c>
       <c r="S12" s="41" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="8" t="s">
         <v>80</v>
@@ -1931,14 +1940,14 @@
       <c r="Q13" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="R13" s="89" t="s">
-        <v>219</v>
+      <c r="R13" s="85" t="s">
+        <v>292</v>
       </c>
       <c r="S13" s="41" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="8" t="s">
         <v>81</v>
@@ -1956,13 +1965,13 @@
         <v>164</v>
       </c>
       <c r="R14" s="53" t="s">
-        <v>219</v>
+        <v>292</v>
       </c>
       <c r="S14" s="54" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="8" t="s">
         <v>82</v>
@@ -1979,12 +1988,12 @@
       <c r="Q15" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="R15" s="89" t="s">
+      <c r="R15" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="S15" s="90"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" s="86"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="8" t="s">
         <v>78</v>
@@ -2006,7 +2015,7 @@
       </c>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>83</v>
@@ -2021,7 +2030,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
         <v>64</v>
@@ -2035,13 +2044,13 @@
       <c r="E18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="Q18" s="88" t="s">
-        <v>221</v>
-      </c>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q18" s="101" t="s">
+        <v>216</v>
+      </c>
+      <c r="R18" s="101"/>
+      <c r="S18" s="101"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>65</v>
@@ -2055,17 +2064,17 @@
       <c r="E19" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="Q19" s="91" t="s">
+      <c r="Q19" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="91" t="s">
+      <c r="R19" s="87" t="s">
         <v>2</v>
       </c>
       <c r="S19" s="83" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>66</v>
@@ -2080,16 +2089,16 @@
         <v>71</v>
       </c>
       <c r="Q20" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="R20" s="89" t="s">
-        <v>222</v>
-      </c>
-      <c r="S20" s="90" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="R20" s="85" t="s">
+        <v>217</v>
+      </c>
+      <c r="S20" s="86" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>67</v>
@@ -2104,16 +2113,16 @@
         <v>71</v>
       </c>
       <c r="Q21" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="R21" s="89" t="s">
-        <v>222</v>
+        <v>176</v>
+      </c>
+      <c r="R21" s="85" t="s">
+        <v>217</v>
       </c>
       <c r="S21" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>55</v>
@@ -2128,16 +2137,16 @@
         <v>36</v>
       </c>
       <c r="Q22" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="R22" s="89" t="s">
-        <v>222</v>
+        <v>177</v>
+      </c>
+      <c r="R22" s="85" t="s">
+        <v>217</v>
       </c>
       <c r="S22" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>122</v>
@@ -2148,16 +2157,16 @@
       <c r="D23" s="13"/>
       <c r="E23" s="12"/>
       <c r="Q23" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="R23" s="89" t="s">
-        <v>222</v>
+        <v>184</v>
+      </c>
+      <c r="R23" s="85" t="s">
+        <v>217</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
         <v>123</v>
       </c>
@@ -2166,16 +2175,16 @@
       </c>
       <c r="D24" s="16"/>
       <c r="Q24" s="40" t="s">
-        <v>224</v>
-      </c>
-      <c r="R24" s="89" t="s">
-        <v>225</v>
+        <v>219</v>
+      </c>
+      <c r="R24" s="85" t="s">
+        <v>220</v>
       </c>
       <c r="S24" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
         <v>124</v>
       </c>
@@ -2184,16 +2193,16 @@
       </c>
       <c r="D25" s="16"/>
       <c r="Q25" s="40" t="s">
-        <v>227</v>
-      </c>
-      <c r="R25" s="89" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="R25" s="85" t="s">
+        <v>223</v>
       </c>
       <c r="S25" s="16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
         <v>125</v>
       </c>
@@ -2202,16 +2211,16 @@
       </c>
       <c r="D26" s="16"/>
       <c r="Q26" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="R26" s="89" t="s">
-        <v>231</v>
+        <v>225</v>
+      </c>
+      <c r="R26" s="85" t="s">
+        <v>226</v>
       </c>
       <c r="S26" s="16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
         <v>126</v>
       </c>
@@ -2220,16 +2229,16 @@
       </c>
       <c r="D27" s="16"/>
       <c r="Q27" s="42" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="R27" s="53" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
         <v>127</v>
       </c>
@@ -2240,12 +2249,12 @@
       <c r="Q28" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="R28" s="89" t="s">
+      <c r="R28" s="85" t="s">
         <v>145</v>
       </c>
       <c r="S28" s="16"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>128</v>
       </c>
@@ -2256,12 +2265,12 @@
       <c r="Q29" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="R29" s="89" t="s">
+      <c r="R29" s="85" t="s">
         <v>146</v>
       </c>
       <c r="S29" s="16"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
         <v>129</v>
       </c>
@@ -2272,12 +2281,12 @@
       <c r="Q30" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="R30" s="89" t="s">
+      <c r="R30" s="85" t="s">
         <v>146</v>
       </c>
       <c r="S30" s="16"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>130</v>
       </c>
@@ -2293,7 +2302,7 @@
       </c>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
         <v>131</v>
       </c>
@@ -2302,7 +2311,7 @@
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>132</v>
       </c>
@@ -2310,13 +2319,13 @@
         <v>147</v>
       </c>
       <c r="D33" s="16"/>
-      <c r="Q33" s="88" t="s">
-        <v>236</v>
-      </c>
-      <c r="R33" s="88"/>
-      <c r="S33" s="88"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="101" t="s">
+        <v>231</v>
+      </c>
+      <c r="R33" s="101"/>
+      <c r="S33" s="101"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="27" t="s">
         <v>133</v>
       </c>
@@ -2324,44 +2333,44 @@
         <v>147</v>
       </c>
       <c r="D34" s="25"/>
-      <c r="Q34" s="91" t="s">
+      <c r="Q34" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="R34" s="91" t="s">
+      <c r="R34" s="87" t="s">
         <v>2</v>
       </c>
       <c r="S34" s="83" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="Q35" s="37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R35" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="S35" s="90" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="S35" s="86" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="32"/>
       <c r="C36" s="33" t="s">
         <v>152</v>
       </c>
       <c r="D36" s="34"/>
       <c r="Q36" s="42" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="R36" s="53" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="S36" s="25" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="29" t="s">
         <v>0</v>
       </c>
@@ -2371,15 +2380,15 @@
       <c r="D37" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="Q37" s="91" t="s">
+      <c r="Q37" s="87" t="s">
         <v>142</v>
       </c>
-      <c r="R37" s="92" t="s">
+      <c r="R37" s="88" t="s">
         <v>151</v>
       </c>
       <c r="S37" s="82"/>
     </row>
-    <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="37" t="s">
         <v>56</v>
       </c>
@@ -2389,11 +2398,11 @@
       <c r="D38" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="Q38" s="93"/>
-      <c r="R38" s="93"/>
-      <c r="S38" s="93"/>
-    </row>
-    <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="89"/>
+    </row>
+    <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="40" t="s">
         <v>155</v>
       </c>
@@ -2403,13 +2412,13 @@
       <c r="D39" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="Q39" s="85" t="s">
-        <v>241</v>
-      </c>
-      <c r="R39" s="86"/>
-      <c r="S39" s="87"/>
-    </row>
-    <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="102" t="s">
+        <v>236</v>
+      </c>
+      <c r="R39" s="103"/>
+      <c r="S39" s="104"/>
+    </row>
+    <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="40" t="s">
         <v>158</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="40" t="s">
         <v>159</v>
       </c>
@@ -2443,13 +2452,13 @@
         <v>76</v>
       </c>
       <c r="R41" s="71" t="s">
-        <v>242</v>
-      </c>
-      <c r="S41" s="94" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="S41" s="90" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="40" t="s">
         <v>160</v>
       </c>
@@ -2460,16 +2469,16 @@
         <v>157</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="R42" s="89" t="s">
-        <v>244</v>
+        <v>190</v>
+      </c>
+      <c r="R42" s="85" t="s">
+        <v>239</v>
       </c>
       <c r="S42" s="52" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="40" t="s">
         <v>58</v>
       </c>
@@ -2480,16 +2489,16 @@
         <v>162</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="R43" s="89" t="s">
-        <v>246</v>
+        <v>186</v>
+      </c>
+      <c r="R43" s="85" t="s">
+        <v>241</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B44" s="40" t="s">
         <v>163</v>
       </c>
@@ -2500,16 +2509,16 @@
         <v>157</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="R44" s="95" t="s">
-        <v>249</v>
-      </c>
-      <c r="S44" s="96" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="R44" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="S44" s="92" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B45" s="40" t="s">
         <v>164</v>
       </c>
@@ -2520,16 +2529,16 @@
         <v>157</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="R45" s="95" t="s">
-        <v>252</v>
-      </c>
-      <c r="S45" s="96" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="R45" s="91" t="s">
+        <v>247</v>
+      </c>
+      <c r="S45" s="92" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B46" s="40" t="s">
         <v>57</v>
       </c>
@@ -2542,12 +2551,12 @@
       <c r="Q46" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="R46" s="95" t="s">
+      <c r="R46" s="91" t="s">
         <v>148</v>
       </c>
       <c r="S46" s="16"/>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B47" s="42" t="s">
         <v>62</v>
       </c>
@@ -2565,7 +2574,7 @@
       </c>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="35"/>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
@@ -2573,19 +2582,19 @@
       <c r="R48" s="71"/>
       <c r="S48" s="71"/>
     </row>
-    <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="47"/>
       <c r="C49" s="48" t="s">
         <v>167</v>
       </c>
       <c r="D49" s="49"/>
-      <c r="Q49" s="85" t="s">
-        <v>254</v>
-      </c>
-      <c r="R49" s="86"/>
-      <c r="S49" s="87"/>
-    </row>
-    <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q49" s="102" t="s">
+        <v>249</v>
+      </c>
+      <c r="R49" s="103"/>
+      <c r="S49" s="104"/>
+    </row>
+    <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="29" t="s">
         <v>0</v>
       </c>
@@ -2605,153 +2614,153 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="37" t="s">
         <v>59</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>168</v>
+        <v>287</v>
       </c>
       <c r="D51" s="45" t="s">
         <v>169</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="R51" s="89" t="s">
-        <v>255</v>
+        <v>195</v>
+      </c>
+      <c r="R51" s="85" t="s">
+        <v>250</v>
       </c>
       <c r="S51" s="52" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C52" s="51" t="s">
-        <v>170</v>
+        <v>285</v>
       </c>
       <c r="D52" s="41" t="s">
         <v>171</v>
       </c>
       <c r="Q52" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="R52" s="89" t="s">
-        <v>255</v>
+        <v>196</v>
+      </c>
+      <c r="R52" s="85" t="s">
+        <v>250</v>
       </c>
       <c r="S52" s="52" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="51" t="s">
+        <v>286</v>
+      </c>
+      <c r="D53" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="D53" s="52" t="s">
-        <v>173</v>
-      </c>
       <c r="Q53" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="R53" s="89" t="s">
-        <v>255</v>
+        <v>197</v>
+      </c>
+      <c r="R53" s="85" t="s">
+        <v>250</v>
       </c>
       <c r="S53" s="52" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="40" t="s">
         <v>92</v>
       </c>
       <c r="C54" s="51" t="s">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="D54" s="41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="R54" s="95" t="s">
-        <v>257</v>
-      </c>
-      <c r="S54" s="96" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="R54" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="S54" s="92" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="40" t="s">
         <v>80</v>
       </c>
       <c r="C55" s="51" t="s">
-        <v>168</v>
+        <v>289</v>
       </c>
       <c r="D55" s="52" t="s">
         <v>169</v>
       </c>
       <c r="Q55" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="R55" s="95" t="s">
-        <v>260</v>
-      </c>
-      <c r="S55" s="96" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="R55" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="S55" s="92" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C56" s="53" t="s">
-        <v>170</v>
+        <v>285</v>
       </c>
       <c r="D56" s="54" t="s">
         <v>171</v>
       </c>
       <c r="Q56" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="R56" s="95" t="s">
-        <v>262</v>
-      </c>
-      <c r="S56" s="96" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="57" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="R56" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="S56" s="92" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="51"/>
       <c r="Q57" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="R57" s="95" t="s">
+      <c r="R57" s="91" t="s">
         <v>150</v>
       </c>
-      <c r="S57" s="96"/>
-    </row>
-    <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S57" s="92"/>
+    </row>
+    <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="56"/>
       <c r="C58" s="57" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D58" s="58"/>
       <c r="Q58" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="R58" s="95" t="s">
+      <c r="R58" s="91" t="s">
         <v>150</v>
       </c>
       <c r="S58" s="16"/>
     </row>
-    <row r="59" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="29" t="s">
         <v>0</v>
       </c>
@@ -2769,7 +2778,7 @@
       </c>
       <c r="S59" s="25"/>
     </row>
-    <row r="60" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="37" t="s">
         <v>81</v>
       </c>
@@ -2783,9 +2792,9 @@
       <c r="R60" s="71"/>
       <c r="S60" s="71"/>
     </row>
-    <row r="61" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C61" s="64" t="s">
         <v>170</v>
@@ -2797,7 +2806,7 @@
       <c r="R61" s="71"/>
       <c r="S61" s="71"/>
     </row>
-    <row r="62" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="40" t="s">
         <v>82</v>
       </c>
@@ -2811,9 +2820,9 @@
       <c r="R62" s="71"/>
       <c r="S62" s="71"/>
     </row>
-    <row r="63" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B63" s="40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C63" s="64" t="s">
         <v>170</v>
@@ -2825,7 +2834,7 @@
       <c r="R63" s="71"/>
       <c r="S63" s="71"/>
     </row>
-    <row r="64" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="40" t="s">
         <v>83</v>
       </c>
@@ -2839,7 +2848,7 @@
       <c r="R64" s="71"/>
       <c r="S64" s="71"/>
     </row>
-    <row r="65" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="40" t="s">
         <v>121</v>
       </c>
@@ -2853,35 +2862,35 @@
       <c r="R65" s="71"/>
       <c r="S65" s="71"/>
     </row>
-    <row r="66" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
         <v>28</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D66" s="52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q66" s="71"/>
       <c r="R66" s="71"/>
       <c r="S66" s="71"/>
     </row>
-    <row r="67" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C67" s="53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D67" s="54" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q67" s="71"/>
       <c r="R67" s="71"/>
       <c r="S67" s="71"/>
     </row>
-    <row r="68" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B68" s="51"/>
       <c r="C68" s="51"/>
       <c r="D68" s="51"/>
@@ -2889,17 +2898,17 @@
       <c r="R68" s="71"/>
       <c r="S68" s="71"/>
     </row>
-    <row r="69" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B69" s="61"/>
       <c r="C69" s="62" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D69" s="63"/>
       <c r="Q69" s="71"/>
       <c r="R69" s="71"/>
       <c r="S69" s="71"/>
     </row>
-    <row r="70" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="29" t="s">
         <v>0</v>
       </c>
@@ -2913,9 +2922,9 @@
       <c r="R70" s="71"/>
       <c r="S70" s="71"/>
     </row>
-    <row r="71" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="37" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C71" s="38" t="s">
         <v>168</v>
@@ -2927,7 +2936,7 @@
       <c r="R71" s="71"/>
       <c r="S71" s="71"/>
     </row>
-    <row r="72" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="40" t="s">
         <v>79</v>
       </c>
@@ -2941,7 +2950,7 @@
       <c r="R72" s="71"/>
       <c r="S72" s="71"/>
     </row>
-    <row r="73" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="40" t="s">
         <v>78</v>
       </c>
@@ -2955,9 +2964,9 @@
       <c r="R73" s="71"/>
       <c r="S73" s="71"/>
     </row>
-    <row r="74" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B74" s="42" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C74" s="53" t="s">
         <v>170</v>
@@ -2969,7 +2978,7 @@
       <c r="R74" s="71"/>
       <c r="S74" s="71"/>
     </row>
-    <row r="75" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B75" s="59"/>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
@@ -2977,16 +2986,16 @@
       <c r="R75" s="71"/>
       <c r="S75" s="71"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="14"/>
-      <c r="B76" s="85" t="s">
+      <c r="B76" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="86"/>
-      <c r="D76" s="87"/>
+      <c r="C76" s="103"/>
+      <c r="D76" s="104"/>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="14"/>
       <c r="B77" s="1" t="s">
         <v>0</v>
@@ -3001,7 +3010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="14"/>
       <c r="B78" s="8" t="s">
         <v>47</v>
@@ -3016,7 +3025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="14"/>
       <c r="B79" s="8" t="s">
         <v>60</v>
@@ -3031,7 +3040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="14"/>
       <c r="B80" s="8" t="s">
         <v>61</v>
@@ -3043,7 +3052,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="14"/>
       <c r="B81" s="8" t="s">
         <v>85</v>
@@ -3058,7 +3067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="14"/>
       <c r="B82" s="8" t="s">
         <v>62</v>
@@ -3073,7 +3082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
       <c r="B83" s="8" t="s">
         <v>63</v>
@@ -3088,7 +3097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="14"/>
       <c r="B84" s="8" t="s">
         <v>84</v>
@@ -3103,7 +3112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="14"/>
       <c r="B85" s="8" t="s">
         <v>64</v>
@@ -3118,7 +3127,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="14"/>
       <c r="B86" s="8" t="s">
         <v>65</v>
@@ -3133,7 +3142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="14"/>
       <c r="B87" s="8" t="s">
         <v>66</v>
@@ -3148,7 +3157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="14"/>
       <c r="B88" s="8" t="s">
         <v>67</v>
@@ -3163,7 +3172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B89" s="7" t="s">
         <v>123</v>
       </c>
@@ -3172,7 +3181,7 @@
       </c>
       <c r="D89" s="16"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
         <v>135</v>
       </c>
@@ -3181,7 +3190,7 @@
       </c>
       <c r="D90" s="16"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B91" s="8" t="s">
         <v>136</v>
       </c>
@@ -3190,7 +3199,7 @@
       </c>
       <c r="D91" s="16"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B92" s="9" t="s">
         <v>134</v>
       </c>
@@ -3199,17 +3208,17 @@
       </c>
       <c r="D92" s="25"/>
     </row>
-    <row r="94" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B94" s="66"/>
       <c r="C94" s="67" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D94" s="68"/>
       <c r="Q94" s="71"/>
       <c r="R94" s="71"/>
       <c r="S94" s="71"/>
     </row>
-    <row r="95" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B95" s="29" t="s">
         <v>0</v>
       </c>
@@ -3223,7 +3232,7 @@
       <c r="R95" s="71"/>
       <c r="S95" s="71"/>
     </row>
-    <row r="96" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" s="37" t="s">
         <v>85</v>
       </c>
@@ -3237,23 +3246,23 @@
       <c r="R96" s="71"/>
       <c r="S96" s="71"/>
     </row>
-    <row r="97" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B97" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="D97" s="52" t="s">
         <v>188</v>
-      </c>
-      <c r="C97" s="70" t="s">
-        <v>189</v>
-      </c>
-      <c r="D97" s="52" t="s">
-        <v>190</v>
       </c>
       <c r="Q97" s="71"/>
       <c r="R97" s="71"/>
       <c r="S97" s="71"/>
     </row>
-    <row r="98" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B98" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C98" s="70" t="s">
         <v>156</v>
@@ -3265,7 +3274,7 @@
       <c r="R98" s="71"/>
       <c r="S98" s="71"/>
     </row>
-    <row r="99" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B99" s="40" t="s">
         <v>63</v>
       </c>
@@ -3279,54 +3288,54 @@
       <c r="R99" s="71"/>
       <c r="S99" s="71"/>
     </row>
-    <row r="100" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B100" s="40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C100" s="70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D100" s="52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q100" s="71"/>
       <c r="R100" s="71"/>
       <c r="S100" s="71"/>
     </row>
-    <row r="101" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B101" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C101" s="70" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D101" s="52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q101" s="71"/>
       <c r="R101" s="71"/>
       <c r="S101" s="71"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B102" s="42" t="s">
         <v>84</v>
       </c>
       <c r="C102" s="53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D102" s="54" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
-      <c r="B104" s="85" t="s">
+      <c r="B104" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="C104" s="86"/>
-      <c r="D104" s="87"/>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C104" s="103"/>
+      <c r="D104" s="104"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="14"/>
       <c r="B105" s="17" t="s">
         <v>0</v>
@@ -3341,7 +3350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="14"/>
       <c r="B106" s="2" t="s">
         <v>76</v>
@@ -3356,7 +3365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="14"/>
       <c r="B107" s="2" t="s">
         <v>43</v>
@@ -3368,7 +3377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="14"/>
       <c r="B108" s="2" t="s">
         <v>48</v>
@@ -3383,7 +3392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="14"/>
       <c r="B109" s="2" t="s">
         <v>18</v>
@@ -3398,7 +3407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="14"/>
       <c r="B110" s="2" t="s">
         <v>113</v>
@@ -3413,7 +3422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="14"/>
       <c r="B111" s="2" t="s">
         <v>114</v>
@@ -3428,7 +3437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B112" s="4" t="s">
         <v>131</v>
       </c>
@@ -3437,15 +3446,15 @@
       </c>
       <c r="D112" s="25"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="14"/>
-      <c r="B114" s="85" t="s">
+      <c r="B114" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="C114" s="86"/>
-      <c r="D114" s="87"/>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C114" s="103"/>
+      <c r="D114" s="104"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="14"/>
       <c r="B115" s="1" t="s">
         <v>0</v>
@@ -3460,7 +3469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="14"/>
       <c r="B116" s="18" t="s">
         <v>44</v>
@@ -3472,7 +3481,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="14"/>
       <c r="B117" s="5" t="s">
         <v>91</v>
@@ -3487,7 +3496,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="14"/>
       <c r="B118" s="5" t="s">
         <v>92</v>
@@ -3502,7 +3511,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="14"/>
       <c r="B119" s="5" t="s">
         <v>93</v>
@@ -3517,7 +3526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="14"/>
       <c r="B120" s="5" t="s">
         <v>94</v>
@@ -3532,25 +3541,25 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="14"/>
       <c r="B121" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C121" s="36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="14"/>
       <c r="B122" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C122" s="36" t="s">
         <v>97</v>
@@ -3562,22 +3571,22 @@
         <v>98</v>
       </c>
     </row>
-    <row r="123" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="14"/>
       <c r="B123" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C123" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E123" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C123" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="D123" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="E123" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B124" s="2" t="s">
         <v>126</v>
       </c>
@@ -3586,7 +3595,7 @@
       </c>
       <c r="D124" s="16"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B125" s="4" t="s">
         <v>137</v>
       </c>
@@ -3595,7 +3604,7 @@
       </c>
       <c r="D125" s="25"/>
     </row>
-    <row r="126" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B126" s="26"/>
       <c r="C126" s="6"/>
       <c r="D126" s="69"/>
@@ -3603,17 +3612,17 @@
       <c r="R126" s="71"/>
       <c r="S126" s="71"/>
     </row>
-    <row r="127" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="72"/>
       <c r="C127" s="73" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D127" s="74"/>
       <c r="Q127" s="71"/>
       <c r="R127" s="71"/>
       <c r="S127" s="71"/>
     </row>
-    <row r="128" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B128" s="29" t="s">
         <v>0</v>
       </c>
@@ -3627,9 +3636,9 @@
       <c r="R128" s="71"/>
       <c r="S128" s="71"/>
     </row>
-    <row r="129" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B129" s="37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C129" s="38" t="s">
         <v>168</v>
@@ -3641,7 +3650,7 @@
       <c r="R129" s="71"/>
       <c r="S129" s="71"/>
     </row>
-    <row r="130" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B130" s="42" t="s">
         <v>91</v>
       </c>
@@ -3655,15 +3664,15 @@
       <c r="R130" s="71"/>
       <c r="S130" s="71"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="21"/>
-      <c r="B132" s="85" t="s">
+      <c r="B132" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="C132" s="86"/>
-      <c r="D132" s="87"/>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C132" s="103"/>
+      <c r="D132" s="104"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="14"/>
       <c r="B133" s="1" t="s">
         <v>0</v>
@@ -3678,7 +3687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="14"/>
       <c r="B134" s="5" t="s">
         <v>45</v>
@@ -3693,7 +3702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" s="14"/>
       <c r="B135" s="5" t="s">
         <v>46</v>
@@ -3708,7 +3717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" s="14"/>
       <c r="B136" s="5" t="s">
         <v>101</v>
@@ -3719,7 +3728,7 @@
       <c r="D136" s="13"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" s="14"/>
       <c r="B137" s="5" t="s">
         <v>102</v>
@@ -3731,7 +3740,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="14"/>
       <c r="B138" s="5" t="s">
         <v>103</v>
@@ -3746,7 +3755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
         <v>107</v>
@@ -3761,7 +3770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" s="14"/>
       <c r="B140" s="2" t="s">
         <v>108</v>
@@ -3776,7 +3785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
         <v>109</v>
@@ -3791,7 +3800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" s="14"/>
       <c r="B142" s="5" t="s">
         <v>110</v>
@@ -3806,7 +3815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="14"/>
       <c r="B143" s="5" t="s">
         <v>111</v>
@@ -3821,7 +3830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="14"/>
       <c r="B144" s="5" t="s">
         <v>94</v>
@@ -3836,7 +3845,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B145" s="2" t="s">
         <v>125</v>
       </c>
@@ -3845,7 +3854,7 @@
       </c>
       <c r="D145" s="16"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="2" t="s">
         <v>138</v>
       </c>
@@ -3854,7 +3863,7 @@
       </c>
       <c r="D146" s="16"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B147" s="2" t="s">
         <v>139</v>
       </c>
@@ -3863,7 +3872,7 @@
       </c>
       <c r="D147" s="16"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B148" s="2" t="s">
         <v>140</v>
       </c>
@@ -3872,7 +3881,7 @@
       </c>
       <c r="D148" s="16"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B149" s="4" t="s">
         <v>141</v>
       </c>
@@ -3881,14 +3890,14 @@
       </c>
       <c r="D149" s="25"/>
     </row>
-    <row r="151" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B151" s="76"/>
       <c r="C151" s="77" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D151" s="78"/>
     </row>
-    <row r="152" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B152" s="29" t="s">
         <v>0</v>
       </c>
@@ -3899,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="37" t="s">
         <v>108</v>
       </c>
@@ -3910,9 +3919,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="154" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B154" s="40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C154" s="79" t="s">
         <v>170</v>
@@ -3921,7 +3930,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="155" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B155" s="40" t="s">
         <v>109</v>
       </c>
@@ -3932,9 +3941,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="156" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B156" s="40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C156" s="79" t="s">
         <v>170</v>
@@ -3943,7 +3952,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="157" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B157" s="40" t="s">
         <v>110</v>
       </c>
@@ -3954,9 +3963,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="158" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B158" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C158" s="79" t="s">
         <v>170</v>
@@ -3965,37 +3974,37 @@
         <v>171</v>
       </c>
     </row>
-    <row r="159" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B159" s="40" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C159" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D159" s="52" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B160" s="42" t="s">
         <v>111</v>
       </c>
       <c r="C160" s="53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D160" s="54" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="23"/>
-      <c r="B162" s="85" t="s">
+      <c r="B162" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="C162" s="86"/>
-      <c r="D162" s="87"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C162" s="103"/>
+      <c r="D162" s="104"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="23"/>
       <c r="B163" s="1" t="s">
         <v>0</v>
@@ -4010,20 +4019,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="23"/>
       <c r="B164" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D164" s="16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E164" s="10"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="23"/>
       <c r="B165" s="8" t="s">
         <v>116</v>
@@ -4036,7 +4045,7 @@
       </c>
       <c r="E165" s="10"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="23"/>
       <c r="B166" s="8" t="s">
         <v>17</v>
@@ -4051,7 +4060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="23"/>
       <c r="B167" s="8" t="s">
         <v>121</v>
@@ -4066,7 +4075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="23"/>
       <c r="B168" s="8" t="s">
         <v>117</v>
@@ -4081,7 +4090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="23"/>
       <c r="B169" s="5" t="s">
         <v>118</v>
@@ -4096,7 +4105,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="23"/>
       <c r="B170" s="5" t="s">
         <v>94</v>
@@ -4111,7 +4120,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B171" s="8" t="s">
         <v>130</v>
       </c>
@@ -4120,7 +4129,7 @@
       </c>
       <c r="D171" s="16"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B172" s="8" t="s">
         <v>142</v>
       </c>
@@ -4129,7 +4138,7 @@
       </c>
       <c r="D172" s="16"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B173" s="9" t="s">
         <v>143</v>
       </c>
@@ -4138,14 +4147,14 @@
       </c>
       <c r="D173" s="25"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B175" s="80"/>
       <c r="C175" s="81" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D175" s="82"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B176" s="29" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B177" s="37" t="s">
         <v>117</v>
       </c>
@@ -4167,9 +4176,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B178" s="40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C178" s="84" t="s">
         <v>170</v>
@@ -4178,7 +4187,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B179" s="40" t="s">
         <v>118</v>
       </c>
@@ -4189,9 +4198,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B180" s="42" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C180" s="53" t="s">
         <v>170</v>
@@ -4200,132 +4209,132 @@
         <v>171</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="98"/>
-      <c r="C182" s="99" t="s">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B182" s="94"/>
+      <c r="C182" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D182" s="96"/>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B183" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" s="97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B184" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C184" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="D184" s="97"/>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B185" s="98" t="s">
+        <v>261</v>
+      </c>
+      <c r="C185" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D185" s="98" t="s">
         <v>263</v>
       </c>
-      <c r="D182" s="100"/>
-    </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C183" s="101" t="s">
-        <v>2</v>
-      </c>
-      <c r="D183" s="101" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="102" t="s">
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B186" s="99" t="s">
+        <v>281</v>
+      </c>
+      <c r="C186" s="99" t="s">
         <v>264</v>
       </c>
-      <c r="C184" s="102" t="s">
+      <c r="D186" s="98" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B187" s="99" t="s">
+        <v>282</v>
+      </c>
+      <c r="C187" s="99" t="s">
+        <v>266</v>
+      </c>
+      <c r="D187" s="98" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B188" s="93" t="s">
+        <v>283</v>
+      </c>
+      <c r="C188" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="D184" s="101"/>
-    </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="102" t="s">
-        <v>266</v>
-      </c>
-      <c r="C185" s="102" t="s">
-        <v>267</v>
-      </c>
-      <c r="D185" s="102" t="s">
+      <c r="D188" s="98"/>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B189" s="98" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="103" t="s">
-        <v>286</v>
-      </c>
-      <c r="C186" s="103" t="s">
+      <c r="C189" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="D186" s="102" t="s">
+      <c r="D189" s="97" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="103" t="s">
-        <v>287</v>
-      </c>
-      <c r="C187" s="103" t="s">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B190" s="98" t="s">
         <v>271</v>
       </c>
-      <c r="D187" s="102" t="s">
+      <c r="C190" s="98" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="97" t="s">
-        <v>288</v>
-      </c>
-      <c r="C188" s="104" t="s">
-        <v>289</v>
-      </c>
-      <c r="D188" s="102"/>
-    </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="102" t="s">
+      <c r="D190" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="C189" s="102" t="s">
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B191" s="98" t="s">
         <v>274</v>
       </c>
-      <c r="D189" s="101" t="s">
+      <c r="C191" s="98" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="102" t="s">
+      <c r="D191" s="97" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B192" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="C190" s="102" t="s">
+      <c r="C192" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="D190" s="101" t="s">
+      <c r="D192" s="97" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="102" t="s">
-        <v>279</v>
-      </c>
-      <c r="C191" s="102" t="s">
-        <v>280</v>
-      </c>
-      <c r="D191" s="101" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="C192" s="102" t="s">
-        <v>282</v>
-      </c>
-      <c r="D192" s="101" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Q49:S49"/>
     <mergeCell ref="B162:D162"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B114:D114"/>
     <mergeCell ref="B132:D132"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q49:S49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Zoomed on drawings and finished 1800
1800 needs reviewed, that is all
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atboe\Documents\GitHub\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF0551D-A4E0-4E1F-87FE-1445513D5ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7F603-3C9E-4A6B-9C53-0FA43C6D31AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="303">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -928,6 +928,18 @@
   </si>
   <si>
     <t>BIPOLAR (BJT) TRANSISTOR NPN 40 V 600 mA</t>
+  </si>
+  <si>
+    <t>BUS_001</t>
+  </si>
+  <si>
+    <t>BUS_002</t>
+  </si>
+  <si>
+    <t>Terminal Bus Connector</t>
+  </si>
+  <si>
+    <t>TBS-CON</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1333,9 +1345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,6 +1354,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1660,37 +1677,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
-  <dimension ref="A1:S192"/>
+  <dimension ref="A1:S198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182:D198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" style="71" customWidth="1"/>
-    <col min="18" max="18" width="34.6640625" style="71" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="71" customWidth="1"/>
+    <col min="18" max="18" width="34.7109375" style="71" customWidth="1"/>
     <col min="19" max="19" width="21" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q1" s="101" t="s">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="104"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="103"/>
       <c r="Q2" s="83" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1725,7 +1742,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -1749,7 +1766,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
         <v>50</v>
@@ -1773,7 +1790,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="8" t="s">
         <v>52</v>
@@ -1797,7 +1814,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -1821,7 +1838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="8" t="s">
         <v>54</v>
@@ -1845,7 +1862,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
         <v>53</v>
@@ -1869,7 +1886,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>24</v>
@@ -1893,7 +1910,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="8" t="s">
         <v>55</v>
@@ -1917,7 +1934,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
         <v>75</v>
@@ -1941,7 +1958,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="8" t="s">
         <v>76</v>
@@ -1965,7 +1982,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="8" t="s">
         <v>77</v>
@@ -1989,7 +2006,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="8" t="s">
         <v>78</v>
@@ -2011,7 +2028,7 @@
       </c>
       <c r="S15" s="86"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="8" t="s">
         <v>74</v>
@@ -2033,7 +2050,7 @@
       </c>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>79</v>
@@ -2048,7 +2065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
         <v>60</v>
@@ -2062,13 +2079,13 @@
       <c r="E18" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="Q18" s="101" t="s">
+      <c r="Q18" s="104" t="s">
         <v>211</v>
       </c>
-      <c r="R18" s="101"/>
-      <c r="S18" s="101"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>61</v>
@@ -2092,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>62</v>
@@ -2116,7 +2133,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>63</v>
@@ -2140,7 +2157,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>51</v>
@@ -2164,7 +2181,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>118</v>
@@ -2184,7 +2201,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>119</v>
       </c>
@@ -2202,7 +2219,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>120</v>
       </c>
@@ -2220,7 +2237,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>121</v>
       </c>
@@ -2238,7 +2255,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>122</v>
       </c>
@@ -2256,7 +2273,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>123</v>
       </c>
@@ -2272,7 +2289,7 @@
       </c>
       <c r="S28" s="16"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>124</v>
       </c>
@@ -2288,7 +2305,7 @@
       </c>
       <c r="S29" s="16"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>125</v>
       </c>
@@ -2304,7 +2321,7 @@
       </c>
       <c r="S30" s="16"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>126</v>
       </c>
@@ -2320,7 +2337,7 @@
       </c>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>127</v>
       </c>
@@ -2329,7 +2346,7 @@
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>128</v>
       </c>
@@ -2337,13 +2354,13 @@
         <v>143</v>
       </c>
       <c r="D33" s="16"/>
-      <c r="Q33" s="101" t="s">
+      <c r="Q33" s="104" t="s">
         <v>226</v>
       </c>
-      <c r="R33" s="101"/>
-      <c r="S33" s="101"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="R33" s="104"/>
+      <c r="S33" s="104"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
         <v>129</v>
       </c>
@@ -2361,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="Q35" s="37" t="s">
         <v>195</v>
       </c>
@@ -2372,7 +2389,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="33" t="s">
         <v>148</v>
@@ -2388,7 +2405,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2423,7 @@
       </c>
       <c r="S37" s="82"/>
     </row>
-    <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="37" t="s">
         <v>52</v>
       </c>
@@ -2420,7 +2437,7 @@
       <c r="R38" s="89"/>
       <c r="S38" s="89"/>
     </row>
-    <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="40" t="s">
         <v>151</v>
       </c>
@@ -2430,13 +2447,13 @@
       <c r="D39" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="Q39" s="102" t="s">
+      <c r="Q39" s="101" t="s">
         <v>231</v>
       </c>
-      <c r="R39" s="103"/>
-      <c r="S39" s="104"/>
-    </row>
-    <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R39" s="102"/>
+      <c r="S39" s="103"/>
+    </row>
+    <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="40" t="s">
         <v>154</v>
       </c>
@@ -2456,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="40" t="s">
         <v>155</v>
       </c>
@@ -2476,7 +2493,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="40" t="s">
         <v>156</v>
       </c>
@@ -2496,7 +2513,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="40" t="s">
         <v>54</v>
       </c>
@@ -2516,7 +2533,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" s="40" t="s">
         <v>159</v>
       </c>
@@ -2536,7 +2553,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" s="40" t="s">
         <v>160</v>
       </c>
@@ -2556,7 +2573,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" s="40" t="s">
         <v>53</v>
       </c>
@@ -2574,7 +2591,7 @@
       </c>
       <c r="S46" s="16"/>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" s="42" t="s">
         <v>58</v>
       </c>
@@ -2592,7 +2609,7 @@
       </c>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="35"/>
       <c r="C48" s="36"/>
       <c r="D48" s="36"/>
@@ -2600,19 +2617,19 @@
       <c r="R48" s="71"/>
       <c r="S48" s="71"/>
     </row>
-    <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="47"/>
       <c r="C49" s="48" t="s">
         <v>163</v>
       </c>
       <c r="D49" s="49"/>
-      <c r="Q49" s="102" t="s">
+      <c r="Q49" s="101" t="s">
         <v>244</v>
       </c>
-      <c r="R49" s="103"/>
-      <c r="S49" s="104"/>
-    </row>
-    <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R49" s="102"/>
+      <c r="S49" s="103"/>
+    </row>
+    <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="29" t="s">
         <v>0</v>
       </c>
@@ -2632,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="37" t="s">
         <v>55</v>
       </c>
@@ -2652,7 +2669,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="40" t="s">
         <v>103</v>
       </c>
@@ -2672,7 +2689,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="40" t="s">
         <v>5</v>
       </c>
@@ -2692,7 +2709,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="40" t="s">
         <v>88</v>
       </c>
@@ -2712,7 +2729,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="40" t="s">
         <v>76</v>
       </c>
@@ -2732,7 +2749,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="42" t="s">
         <v>170</v>
       </c>
@@ -2752,7 +2769,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="51"/>
@@ -2764,7 +2781,7 @@
       </c>
       <c r="S57" s="92"/>
     </row>
-    <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="56"/>
       <c r="C58" s="57" t="s">
         <v>171</v>
@@ -2778,7 +2795,7 @@
       </c>
       <c r="S58" s="16"/>
     </row>
-    <row r="59" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="29" t="s">
         <v>0</v>
       </c>
@@ -2796,7 +2813,7 @@
       </c>
       <c r="S59" s="25"/>
     </row>
-    <row r="60" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="37" t="s">
         <v>77</v>
       </c>
@@ -2810,7 +2827,7 @@
       <c r="R60" s="71"/>
       <c r="S60" s="71"/>
     </row>
-    <row r="61" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="40" t="s">
         <v>172</v>
       </c>
@@ -2824,7 +2841,7 @@
       <c r="R61" s="71"/>
       <c r="S61" s="71"/>
     </row>
-    <row r="62" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="40" t="s">
         <v>78</v>
       </c>
@@ -2838,7 +2855,7 @@
       <c r="R62" s="71"/>
       <c r="S62" s="71"/>
     </row>
-    <row r="63" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="40" t="s">
         <v>173</v>
       </c>
@@ -2852,7 +2869,7 @@
       <c r="R63" s="71"/>
       <c r="S63" s="71"/>
     </row>
-    <row r="64" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="40" t="s">
         <v>79</v>
       </c>
@@ -2866,7 +2883,7 @@
       <c r="R64" s="71"/>
       <c r="S64" s="71"/>
     </row>
-    <row r="65" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="40" t="s">
         <v>117</v>
       </c>
@@ -2880,7 +2897,7 @@
       <c r="R65" s="71"/>
       <c r="S65" s="71"/>
     </row>
-    <row r="66" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="40" t="s">
         <v>24</v>
       </c>
@@ -2894,7 +2911,7 @@
       <c r="R66" s="71"/>
       <c r="S66" s="71"/>
     </row>
-    <row r="67" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="42" t="s">
         <v>14</v>
       </c>
@@ -2908,7 +2925,7 @@
       <c r="R67" s="71"/>
       <c r="S67" s="71"/>
     </row>
-    <row r="68" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="51"/>
       <c r="C68" s="51"/>
       <c r="D68" s="51"/>
@@ -2916,7 +2933,7 @@
       <c r="R68" s="71"/>
       <c r="S68" s="71"/>
     </row>
-    <row r="69" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="61"/>
       <c r="C69" s="62" t="s">
         <v>178</v>
@@ -2926,7 +2943,7 @@
       <c r="R69" s="71"/>
       <c r="S69" s="71"/>
     </row>
-    <row r="70" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
         <v>0</v>
       </c>
@@ -2940,7 +2957,7 @@
       <c r="R70" s="71"/>
       <c r="S70" s="71"/>
     </row>
-    <row r="71" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="37" t="s">
         <v>179</v>
       </c>
@@ -2954,7 +2971,7 @@
       <c r="R71" s="71"/>
       <c r="S71" s="71"/>
     </row>
-    <row r="72" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="40" t="s">
         <v>75</v>
       </c>
@@ -2968,7 +2985,7 @@
       <c r="R72" s="71"/>
       <c r="S72" s="71"/>
     </row>
-    <row r="73" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="40" t="s">
         <v>74</v>
       </c>
@@ -2982,7 +2999,7 @@
       <c r="R73" s="71"/>
       <c r="S73" s="71"/>
     </row>
-    <row r="74" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="42" t="s">
         <v>180</v>
       </c>
@@ -2996,7 +3013,7 @@
       <c r="R74" s="71"/>
       <c r="S74" s="71"/>
     </row>
-    <row r="75" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="59"/>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
@@ -3004,16 +3021,16 @@
       <c r="R75" s="71"/>
       <c r="S75" s="71"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
-      <c r="B76" s="102" t="s">
+      <c r="B76" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="C76" s="103"/>
-      <c r="D76" s="104"/>
+      <c r="C76" s="102"/>
+      <c r="D76" s="103"/>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="1" t="s">
         <v>0</v>
@@ -3028,7 +3045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="8" t="s">
         <v>43</v>
@@ -3043,7 +3060,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" s="8" t="s">
         <v>56</v>
@@ -3058,7 +3075,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="14"/>
       <c r="B80" s="8" t="s">
         <v>57</v>
@@ -3070,7 +3087,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="14"/>
       <c r="B81" s="8" t="s">
         <v>81</v>
@@ -3085,7 +3102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
       <c r="B82" s="8" t="s">
         <v>58</v>
@@ -3100,7 +3117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="14"/>
       <c r="B83" s="8" t="s">
         <v>59</v>
@@ -3115,7 +3132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="B84" s="8" t="s">
         <v>80</v>
@@ -3130,7 +3147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="14"/>
       <c r="B85" s="8" t="s">
         <v>60</v>
@@ -3145,7 +3162,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
       <c r="B86" s="8" t="s">
         <v>61</v>
@@ -3160,7 +3177,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="8" t="s">
         <v>62</v>
@@ -3175,7 +3192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="8" t="s">
         <v>63</v>
@@ -3190,7 +3207,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
         <v>119</v>
       </c>
@@ -3199,7 +3216,7 @@
       </c>
       <c r="D89" s="16"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>131</v>
       </c>
@@ -3208,7 +3225,7 @@
       </c>
       <c r="D90" s="16"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>132</v>
       </c>
@@ -3217,7 +3234,7 @@
       </c>
       <c r="D91" s="16"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
         <v>130</v>
       </c>
@@ -3226,7 +3243,7 @@
       </c>
       <c r="D92" s="25"/>
     </row>
-    <row r="94" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="66"/>
       <c r="C94" s="67" t="s">
         <v>181</v>
@@ -3236,7 +3253,7 @@
       <c r="R94" s="71"/>
       <c r="S94" s="71"/>
     </row>
-    <row r="95" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="29" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3267,7 @@
       <c r="R95" s="71"/>
       <c r="S95" s="71"/>
     </row>
-    <row r="96" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="37" t="s">
         <v>81</v>
       </c>
@@ -3264,7 +3281,7 @@
       <c r="R96" s="71"/>
       <c r="S96" s="71"/>
     </row>
-    <row r="97" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="40" t="s">
         <v>182</v>
       </c>
@@ -3278,7 +3295,7 @@
       <c r="R97" s="71"/>
       <c r="S97" s="71"/>
     </row>
-    <row r="98" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="40" t="s">
         <v>184</v>
       </c>
@@ -3292,7 +3309,7 @@
       <c r="R98" s="71"/>
       <c r="S98" s="71"/>
     </row>
-    <row r="99" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="40" t="s">
         <v>59</v>
       </c>
@@ -3306,7 +3323,7 @@
       <c r="R99" s="71"/>
       <c r="S99" s="71"/>
     </row>
-    <row r="100" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="40" t="s">
         <v>185</v>
       </c>
@@ -3320,7 +3337,7 @@
       <c r="R100" s="71"/>
       <c r="S100" s="71"/>
     </row>
-    <row r="101" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
         <v>186</v>
       </c>
@@ -3334,7 +3351,7 @@
       <c r="R101" s="71"/>
       <c r="S101" s="71"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B102" s="42" t="s">
         <v>80</v>
       </c>
@@ -3345,15 +3362,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
-      <c r="B104" s="102" t="s">
+      <c r="B104" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="103"/>
-      <c r="D104" s="104"/>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C104" s="102"/>
+      <c r="D104" s="103"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="17" t="s">
         <v>0</v>
@@ -3368,7 +3385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="2" t="s">
         <v>72</v>
@@ -3383,7 +3400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="2" t="s">
         <v>39</v>
@@ -3395,7 +3412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="2" t="s">
         <v>44</v>
@@ -3410,7 +3427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="2" t="s">
         <v>14</v>
@@ -3425,7 +3442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="2" t="s">
         <v>109</v>
@@ -3440,7 +3457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="2" t="s">
         <v>110</v>
@@ -3455,7 +3472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
         <v>127</v>
       </c>
@@ -3464,15 +3481,15 @@
       </c>
       <c r="D112" s="25"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
-      <c r="B114" s="102" t="s">
+      <c r="B114" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="C114" s="103"/>
-      <c r="D114" s="104"/>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C114" s="102"/>
+      <c r="D114" s="103"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="1" t="s">
         <v>0</v>
@@ -3487,7 +3504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="18" t="s">
         <v>40</v>
@@ -3499,7 +3516,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="5" t="s">
         <v>87</v>
@@ -3514,7 +3531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="5" t="s">
         <v>88</v>
@@ -3529,7 +3546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="5" t="s">
         <v>89</v>
@@ -3544,7 +3561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="5" t="s">
         <v>90</v>
@@ -3559,7 +3576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="5" t="s">
         <v>91</v>
@@ -3574,7 +3591,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="5" t="s">
         <v>197</v>
@@ -3589,7 +3606,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="123" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="5" t="s">
         <v>198</v>
@@ -3604,7 +3621,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>122</v>
       </c>
@@ -3613,7 +3630,7 @@
       </c>
       <c r="D124" s="16"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B125" s="4" t="s">
         <v>133</v>
       </c>
@@ -3622,7 +3639,7 @@
       </c>
       <c r="D125" s="25"/>
     </row>
-    <row r="126" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="26"/>
       <c r="C126" s="6"/>
       <c r="D126" s="69"/>
@@ -3630,7 +3647,7 @@
       <c r="R126" s="71"/>
       <c r="S126" s="71"/>
     </row>
-    <row r="127" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="72"/>
       <c r="C127" s="73" t="s">
         <v>187</v>
@@ -3640,7 +3657,7 @@
       <c r="R127" s="71"/>
       <c r="S127" s="71"/>
     </row>
-    <row r="128" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="29" t="s">
         <v>0</v>
       </c>
@@ -3654,7 +3671,7 @@
       <c r="R128" s="71"/>
       <c r="S128" s="71"/>
     </row>
-    <row r="129" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="37" t="s">
         <v>188</v>
       </c>
@@ -3668,7 +3685,7 @@
       <c r="R129" s="71"/>
       <c r="S129" s="71"/>
     </row>
-    <row r="130" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="42" t="s">
         <v>87</v>
       </c>
@@ -3682,15 +3699,15 @@
       <c r="R130" s="71"/>
       <c r="S130" s="71"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
-      <c r="B132" s="102" t="s">
+      <c r="B132" s="101" t="s">
         <v>96</v>
       </c>
-      <c r="C132" s="103"/>
-      <c r="D132" s="104"/>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C132" s="102"/>
+      <c r="D132" s="103"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
       <c r="B133" s="1" t="s">
         <v>0</v>
@@ -3705,7 +3722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
       <c r="B134" s="5" t="s">
         <v>41</v>
@@ -3720,7 +3737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="5" t="s">
         <v>42</v>
@@ -3735,7 +3752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="5" t="s">
         <v>97</v>
@@ -3746,7 +3763,7 @@
       <c r="D136" s="13"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="5" t="s">
         <v>98</v>
@@ -3758,7 +3775,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="5" t="s">
         <v>99</v>
@@ -3773,7 +3790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
         <v>103</v>
@@ -3788,7 +3805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="2" t="s">
         <v>104</v>
@@ -3803,7 +3820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
         <v>105</v>
@@ -3818,7 +3835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="5" t="s">
         <v>106</v>
@@ -3833,7 +3850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="5" t="s">
         <v>107</v>
@@ -3848,7 +3865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="5" t="s">
         <v>90</v>
@@ -3863,7 +3880,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="2" t="s">
         <v>121</v>
       </c>
@@ -3872,7 +3889,7 @@
       </c>
       <c r="D145" s="16"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
         <v>134</v>
       </c>
@@ -3881,7 +3898,7 @@
       </c>
       <c r="D146" s="16"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
         <v>135</v>
       </c>
@@ -3890,7 +3907,7 @@
       </c>
       <c r="D147" s="16"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="2" t="s">
         <v>136</v>
       </c>
@@ -3899,7 +3916,7 @@
       </c>
       <c r="D148" s="16"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
         <v>137</v>
       </c>
@@ -3908,14 +3925,14 @@
       </c>
       <c r="D149" s="25"/>
     </row>
-    <row r="151" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B151" s="76"/>
       <c r="C151" s="77" t="s">
         <v>189</v>
       </c>
       <c r="D151" s="78"/>
     </row>
-    <row r="152" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B152" s="29" t="s">
         <v>0</v>
       </c>
@@ -3926,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B153" s="37" t="s">
         <v>104</v>
       </c>
@@ -3937,7 +3954,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B154" s="40" t="s">
         <v>190</v>
       </c>
@@ -3948,7 +3965,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="155" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B155" s="40" t="s">
         <v>105</v>
       </c>
@@ -3959,7 +3976,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="156" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="40" t="s">
         <v>191</v>
       </c>
@@ -3970,7 +3987,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="157" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="40" t="s">
         <v>106</v>
       </c>
@@ -3981,7 +3998,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="158" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B158" s="40" t="s">
         <v>192</v>
       </c>
@@ -3992,7 +4009,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="159" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B159" s="40" t="s">
         <v>193</v>
       </c>
@@ -4003,7 +4020,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="160" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B160" s="42" t="s">
         <v>107</v>
       </c>
@@ -4014,15 +4031,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="23"/>
-      <c r="B162" s="102" t="s">
+      <c r="B162" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="C162" s="103"/>
-      <c r="D162" s="104"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C162" s="102"/>
+      <c r="D162" s="103"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="23"/>
       <c r="B163" s="1" t="s">
         <v>0</v>
@@ -4037,7 +4054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="23"/>
       <c r="B164" s="8" t="s">
         <v>38</v>
@@ -4050,7 +4067,7 @@
       </c>
       <c r="E164" s="10"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="23"/>
       <c r="B165" s="8" t="s">
         <v>112</v>
@@ -4063,7 +4080,7 @@
       </c>
       <c r="E165" s="10"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="23"/>
       <c r="B166" s="8" t="s">
         <v>13</v>
@@ -4078,7 +4095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="23"/>
       <c r="B167" s="8" t="s">
         <v>117</v>
@@ -4093,7 +4110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="23"/>
       <c r="B168" s="8" t="s">
         <v>113</v>
@@ -4108,7 +4125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="23"/>
       <c r="B169" s="5" t="s">
         <v>114</v>
@@ -4123,7 +4140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="23"/>
       <c r="B170" s="5" t="s">
         <v>90</v>
@@ -4138,7 +4155,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B171" s="8" t="s">
         <v>126</v>
       </c>
@@ -4147,7 +4164,7 @@
       </c>
       <c r="D171" s="16"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B172" s="8" t="s">
         <v>138</v>
       </c>
@@ -4156,7 +4173,7 @@
       </c>
       <c r="D172" s="16"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>139</v>
       </c>
@@ -4165,14 +4182,14 @@
       </c>
       <c r="D173" s="25"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B175" s="80"/>
       <c r="C175" s="81" t="s">
         <v>194</v>
       </c>
       <c r="D175" s="82"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B176" s="29" t="s">
         <v>0</v>
       </c>
@@ -4183,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="37" t="s">
         <v>113</v>
       </c>
@@ -4194,7 +4211,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="40" t="s">
         <v>195</v>
       </c>
@@ -4205,7 +4222,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="40" t="s">
         <v>114</v>
       </c>
@@ -4216,7 +4233,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="42" t="s">
         <v>196</v>
       </c>
@@ -4227,14 +4244,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="94"/>
       <c r="C182" s="95" t="s">
         <v>253</v>
       </c>
       <c r="D182" s="96"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="97" t="s">
         <v>0</v>
       </c>
@@ -4245,7 +4262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="98" t="s">
         <v>254</v>
       </c>
@@ -4254,7 +4271,7 @@
       </c>
       <c r="D184" s="97"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="98" t="s">
         <v>256</v>
       </c>
@@ -4265,7 +4282,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="99" t="s">
         <v>276</v>
       </c>
@@ -4276,7 +4293,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="99" t="s">
         <v>277</v>
       </c>
@@ -4287,7 +4304,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="93" t="s">
         <v>278</v>
       </c>
@@ -4296,7 +4313,7 @@
       </c>
       <c r="D188" s="98"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="98" t="s">
         <v>263</v>
       </c>
@@ -4307,7 +4324,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="98" t="s">
         <v>266</v>
       </c>
@@ -4318,7 +4335,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" s="98" t="s">
         <v>269</v>
       </c>
@@ -4329,7 +4346,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" s="98" t="s">
         <v>271</v>
       </c>
@@ -4340,19 +4357,77 @@
         <v>273</v>
       </c>
     </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="106" t="s">
+        <v>299</v>
+      </c>
+      <c r="C193" s="107" t="s">
+        <v>301</v>
+      </c>
+      <c r="D193" s="108" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D194" s="109" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="93" t="s">
+        <v>133</v>
+      </c>
+      <c r="C195" t="s">
+        <v>145</v>
+      </c>
+      <c r="D195" s="16"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="93" t="s">
+        <v>130</v>
+      </c>
+      <c r="C196" t="s">
+        <v>144</v>
+      </c>
+      <c r="D196" s="16"/>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="93" t="s">
+        <v>137</v>
+      </c>
+      <c r="C197" t="s">
+        <v>146</v>
+      </c>
+      <c r="D197" s="16"/>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="105" t="s">
+        <v>128</v>
+      </c>
+      <c r="C198" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D198" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q49:S49"/>
     <mergeCell ref="B162:D162"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B114:D114"/>
     <mergeCell ref="B132:D132"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Q49:S49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Reformatted BOM, deleted old ones
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Samuel Mattingly\Documents\GitHub\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34892\Documents\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7F603-3C9E-4A6B-9C53-0FA43C6D31AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63FAC21-DDD0-47DE-BFE3-330A65E7B3E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -995,7 +995,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1161,23 +1161,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1328,23 +1317,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1354,14 +1339,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1679,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
   <dimension ref="A1:S198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182:D198"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,23 +1674,23 @@
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" style="71" customWidth="1"/>
     <col min="18" max="18" width="34.7109375" style="71" customWidth="1"/>
-    <col min="19" max="19" width="21" style="71" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q1" s="104" t="s">
+      <c r="Q1" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="R1" s="104"/>
-      <c r="S1" s="104"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
       <c r="Q2" s="83" t="s">
         <v>0</v>
       </c>
@@ -1732,13 +1715,13 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="R3" s="71" t="s">
+      <c r="R3" s="88" t="s">
         <v>285</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="86" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1759,7 +1742,7 @@
       <c r="Q4" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="R4" s="71" t="s">
+      <c r="R4" s="69" t="s">
         <v>285</v>
       </c>
       <c r="S4" s="16" t="s">
@@ -1879,7 +1862,7 @@
       <c r="Q9" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="R9" s="85" t="s">
+      <c r="R9" s="84" t="s">
         <v>287</v>
       </c>
       <c r="S9" s="52" t="s">
@@ -1903,7 +1886,7 @@
       <c r="Q10" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="R10" s="85" t="s">
+      <c r="R10" s="84" t="s">
         <v>287</v>
       </c>
       <c r="S10" s="41" t="s">
@@ -1927,7 +1910,7 @@
       <c r="Q11" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="R11" s="85" t="s">
+      <c r="R11" s="84" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="52" t="s">
@@ -1951,7 +1934,7 @@
       <c r="Q12" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="R12" s="85" t="s">
+      <c r="R12" s="84" t="s">
         <v>287</v>
       </c>
       <c r="S12" s="41" t="s">
@@ -1975,7 +1958,7 @@
       <c r="Q13" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="R13" s="85" t="s">
+      <c r="R13" s="84" t="s">
         <v>287</v>
       </c>
       <c r="S13" s="41" t="s">
@@ -1996,13 +1979,13 @@
       <c r="E14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Q14" s="42" t="s">
+      <c r="Q14" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="R14" s="53" t="s">
+      <c r="R14" s="84" t="s">
         <v>287</v>
       </c>
-      <c r="S14" s="54" t="s">
+      <c r="S14" s="41" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2023,10 +2006,10 @@
       <c r="Q15" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="R15" s="85" t="s">
+      <c r="R15" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="S15" s="86"/>
+      <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
@@ -2079,11 +2062,11 @@
       <c r="E18" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="Q18" s="104" t="s">
+      <c r="Q18" s="96" t="s">
         <v>211</v>
       </c>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
+      <c r="R18" s="96"/>
+      <c r="S18" s="96"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
@@ -2126,7 +2109,7 @@
       <c r="Q20" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="R20" s="85" t="s">
+      <c r="R20" s="38" t="s">
         <v>212</v>
       </c>
       <c r="S20" s="86" t="s">
@@ -2150,7 +2133,7 @@
       <c r="Q21" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="R21" s="85" t="s">
+      <c r="R21" s="84" t="s">
         <v>212</v>
       </c>
       <c r="S21" s="16" t="s">
@@ -2174,7 +2157,7 @@
       <c r="Q22" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="R22" s="85" t="s">
+      <c r="R22" s="84" t="s">
         <v>212</v>
       </c>
       <c r="S22" s="16" t="s">
@@ -2194,7 +2177,7 @@
       <c r="Q23" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="R23" s="85" t="s">
+      <c r="R23" s="84" t="s">
         <v>212</v>
       </c>
       <c r="S23" s="16" t="s">
@@ -2212,7 +2195,7 @@
       <c r="Q24" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="R24" s="85" t="s">
+      <c r="R24" s="84" t="s">
         <v>215</v>
       </c>
       <c r="S24" s="16" t="s">
@@ -2230,7 +2213,7 @@
       <c r="Q25" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="R25" s="85" t="s">
+      <c r="R25" s="84" t="s">
         <v>218</v>
       </c>
       <c r="S25" s="16" t="s">
@@ -2248,7 +2231,7 @@
       <c r="Q26" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="R26" s="85" t="s">
+      <c r="R26" s="84" t="s">
         <v>221</v>
       </c>
       <c r="S26" s="16" t="s">
@@ -2263,13 +2246,13 @@
         <v>141</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="Q27" s="42" t="s">
+      <c r="Q27" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="R27" s="53" t="s">
+      <c r="R27" s="84" t="s">
         <v>224</v>
       </c>
-      <c r="S27" s="25" t="s">
+      <c r="S27" s="16" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2284,7 +2267,7 @@
       <c r="Q28" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="R28" s="85" t="s">
+      <c r="R28" s="84" t="s">
         <v>141</v>
       </c>
       <c r="S28" s="16"/>
@@ -2300,7 +2283,7 @@
       <c r="Q29" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="R29" s="85" t="s">
+      <c r="R29" s="84" t="s">
         <v>142</v>
       </c>
       <c r="S29" s="16"/>
@@ -2316,7 +2299,7 @@
       <c r="Q30" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="R30" s="85" t="s">
+      <c r="R30" s="84" t="s">
         <v>142</v>
       </c>
       <c r="S30" s="16"/>
@@ -2354,11 +2337,11 @@
         <v>143</v>
       </c>
       <c r="D33" s="16"/>
-      <c r="Q33" s="104" t="s">
+      <c r="Q33" s="96" t="s">
         <v>226</v>
       </c>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
+      <c r="R33" s="96"/>
+      <c r="S33" s="96"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
@@ -2395,13 +2378,13 @@
         <v>148</v>
       </c>
       <c r="D36" s="34"/>
-      <c r="Q36" s="42" t="s">
+      <c r="Q36" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="R36" s="53" t="s">
+      <c r="R36" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="S36" s="25" t="s">
+      <c r="S36" s="16" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2415,13 +2398,13 @@
       <c r="D37" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="Q37" s="87" t="s">
+      <c r="Q37" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="R37" s="88" t="s">
+      <c r="R37" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="S37" s="82"/>
+      <c r="S37" s="25"/>
     </row>
     <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="37" t="s">
@@ -2433,9 +2416,9 @@
       <c r="D38" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="Q38" s="89"/>
-      <c r="R38" s="89"/>
-      <c r="S38" s="89"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
     </row>
     <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="40" t="s">
@@ -2447,11 +2430,11 @@
       <c r="D39" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="Q39" s="101" t="s">
+      <c r="Q39" s="97" t="s">
         <v>231</v>
       </c>
-      <c r="R39" s="102"/>
-      <c r="S39" s="103"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="99"/>
     </row>
     <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="40" t="s">
@@ -2489,7 +2472,7 @@
       <c r="R41" s="71" t="s">
         <v>232</v>
       </c>
-      <c r="S41" s="90" t="s">
+      <c r="S41" s="89" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2546,10 +2529,10 @@
       <c r="Q44" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="R44" s="91" t="s">
+      <c r="R44" s="90" t="s">
         <v>239</v>
       </c>
-      <c r="S44" s="92" t="s">
+      <c r="S44" s="91" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2566,10 +2549,10 @@
       <c r="Q45" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="R45" s="91" t="s">
+      <c r="R45" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="S45" s="92" t="s">
+      <c r="S45" s="91" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2586,7 +2569,7 @@
       <c r="Q46" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="R46" s="91" t="s">
+      <c r="R46" s="90" t="s">
         <v>144</v>
       </c>
       <c r="S46" s="16"/>
@@ -2623,11 +2606,11 @@
         <v>163</v>
       </c>
       <c r="D49" s="49"/>
-      <c r="Q49" s="101" t="s">
+      <c r="Q49" s="97" t="s">
         <v>244</v>
       </c>
-      <c r="R49" s="102"/>
-      <c r="S49" s="103"/>
+      <c r="R49" s="98"/>
+      <c r="S49" s="99"/>
     </row>
     <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="29" t="s">
@@ -2722,10 +2705,10 @@
       <c r="Q54" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="R54" s="91" t="s">
+      <c r="R54" s="90" t="s">
         <v>247</v>
       </c>
-      <c r="S54" s="92" t="s">
+      <c r="S54" s="91" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2742,10 +2725,10 @@
       <c r="Q55" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="R55" s="91" t="s">
+      <c r="R55" s="90" t="s">
         <v>250</v>
       </c>
-      <c r="S55" s="92" t="s">
+      <c r="S55" s="91" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2762,10 +2745,10 @@
       <c r="Q56" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="R56" s="91" t="s">
+      <c r="R56" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="S56" s="92" t="s">
+      <c r="S56" s="91" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2776,10 +2759,10 @@
       <c r="Q57" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="R57" s="91" t="s">
+      <c r="R57" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="S57" s="92"/>
+      <c r="S57" s="91"/>
     </row>
     <row r="58" spans="2:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="56"/>
@@ -2790,7 +2773,7 @@
       <c r="Q58" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="R58" s="91" t="s">
+      <c r="R58" s="90" t="s">
         <v>146</v>
       </c>
       <c r="S58" s="16"/>
@@ -3023,11 +3006,11 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
-      <c r="B76" s="101" t="s">
+      <c r="B76" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="C76" s="102"/>
-      <c r="D76" s="103"/>
+      <c r="C76" s="98"/>
+      <c r="D76" s="99"/>
       <c r="E76" s="12"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -3364,11 +3347,11 @@
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
-      <c r="B104" s="101" t="s">
+      <c r="B104" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="102"/>
-      <c r="D104" s="103"/>
+      <c r="C104" s="98"/>
+      <c r="D104" s="99"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
@@ -3483,11 +3466,11 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
-      <c r="B114" s="101" t="s">
+      <c r="B114" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="C114" s="102"/>
-      <c r="D114" s="103"/>
+      <c r="C114" s="98"/>
+      <c r="D114" s="99"/>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
@@ -3701,11 +3684,11 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
-      <c r="B132" s="101" t="s">
+      <c r="B132" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="C132" s="102"/>
-      <c r="D132" s="103"/>
+      <c r="C132" s="98"/>
+      <c r="D132" s="99"/>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
@@ -4033,11 +4016,11 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="23"/>
-      <c r="B162" s="101" t="s">
+      <c r="B162" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="C162" s="102"/>
-      <c r="D162" s="103"/>
+      <c r="C162" s="98"/>
+      <c r="D162" s="99"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="23"/>
@@ -4245,169 +4228,169 @@
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="94"/>
-      <c r="C182" s="95" t="s">
+      <c r="B182" s="92"/>
+      <c r="C182" s="93" t="s">
         <v>253</v>
       </c>
-      <c r="D182" s="96"/>
+      <c r="D182" s="94"/>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="97" t="s">
+      <c r="B183" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C183" s="97" t="s">
+      <c r="C183" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D183" s="97" t="s">
+      <c r="D183" s="95" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="98" t="s">
+      <c r="B184" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C184" s="98" t="s">
+      <c r="C184" s="69" t="s">
         <v>274</v>
       </c>
-      <c r="D184" s="97"/>
+      <c r="D184" s="102"/>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="98" t="s">
+      <c r="B185" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="C185" s="98" t="s">
+      <c r="C185" s="69" t="s">
         <v>257</v>
       </c>
-      <c r="D185" s="98" t="s">
+      <c r="D185" s="16" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="99" t="s">
+      <c r="B186" s="103" t="s">
         <v>276</v>
       </c>
-      <c r="C186" s="99" t="s">
+      <c r="C186" s="100" t="s">
         <v>259</v>
       </c>
-      <c r="D186" s="98" t="s">
+      <c r="D186" s="16" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="99" t="s">
+      <c r="B187" s="103" t="s">
         <v>277</v>
       </c>
-      <c r="C187" s="99" t="s">
+      <c r="C187" s="100" t="s">
         <v>261</v>
       </c>
-      <c r="D187" s="98" t="s">
+      <c r="D187" s="16" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="93" t="s">
+      <c r="B188" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C188" s="100" t="s">
+      <c r="C188" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="D188" s="98"/>
+      <c r="D188" s="16"/>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="98" t="s">
+      <c r="B189" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C189" s="98" t="s">
+      <c r="C189" s="69" t="s">
         <v>264</v>
       </c>
-      <c r="D189" s="97" t="s">
+      <c r="D189" s="102" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="98" t="s">
+      <c r="B190" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="C190" s="98" t="s">
+      <c r="C190" s="69" t="s">
         <v>267</v>
       </c>
-      <c r="D190" s="97" t="s">
+      <c r="D190" s="102" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="98" t="s">
+      <c r="B191" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C191" s="98" t="s">
+      <c r="C191" s="69" t="s">
         <v>270</v>
       </c>
-      <c r="D191" s="97" t="s">
+      <c r="D191" s="102" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="98" t="s">
+      <c r="B192" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C192" s="98" t="s">
+      <c r="C192" s="69" t="s">
         <v>272</v>
       </c>
-      <c r="D192" s="97" t="s">
+      <c r="D192" s="102" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="106" t="s">
+      <c r="B193" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="C193" s="107" t="s">
+      <c r="C193" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="D193" s="108" t="s">
+      <c r="D193" s="104" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="105" t="s">
+      <c r="B194" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="C194" s="9" t="s">
+      <c r="C194" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="D194" s="109" t="s">
+      <c r="D194" s="104" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="93" t="s">
+      <c r="B195" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="69" t="s">
         <v>145</v>
       </c>
       <c r="D195" s="16"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="93" t="s">
+      <c r="B196" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="69" t="s">
         <v>144</v>
       </c>
       <c r="D196" s="16"/>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="93" t="s">
+      <c r="B197" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="69" t="s">
         <v>146</v>
       </c>
       <c r="D197" s="16"/>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B198" s="105" t="s">
+      <c r="B198" s="9" t="s">
         <v>128</v>
       </c>
       <c r="C198" s="11" t="s">
@@ -4417,17 +4400,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Q49:S49"/>
     <mergeCell ref="B162:D162"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B114:D114"/>
     <mergeCell ref="B132:D132"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q49:S49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Finalized formatting for 1100 series drawings
final edits in readability and aesthetics
</commit_message>
<xml_diff>
--- a/docs/BOM_OLE.xlsx
+++ b/docs/BOM_OLE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacko\OneDrive\Documents\GitHub\Gallagher-Station-Duke-Energy-Museum-Exhibit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5A21A5-EA7E-4046-A2ED-6352F20E9133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88EF1A8-EE44-4D55-B34B-AD60D7B1250E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F9C4A7-2F91-47A6-87E7-FD502526FA96}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="304">
   <si>
     <t>IDENTIFIER</t>
   </si>
@@ -139,12 +139,6 @@
     <t>https://www.digikey.com/en/products/detail/dfrobot/DFR0229/6588460</t>
   </si>
   <si>
-    <t>ARDUINO MEGA2560 ATMEGA2560</t>
-  </si>
-  <si>
-    <t>MICROSD CARD MODULE FOR ARDUINO</t>
-  </si>
-  <si>
     <t>U15</t>
   </si>
   <si>
@@ -941,6 +935,18 @@
   </si>
   <si>
     <t>ROB-09238</t>
+  </si>
+  <si>
+    <t>ARDUINO MEGA 2560 ATMEGA2560</t>
+  </si>
+  <si>
+    <t>MICRO-SD CARD MODULE FOR ARDUINO</t>
+  </si>
+  <si>
+    <t>ADAFRUIT SERVO MOTOR</t>
+  </si>
+  <si>
+    <t>CTS ELECTRONICS ROTARY ENCODER</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1342,18 +1348,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1397,6 +1391,47 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1714,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8E8FB-31E6-4C12-BDEF-C37A27F0E5DF}">
   <dimension ref="A1:S198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q61" sqref="Q61:S70"/>
+    <sheetView tabSelected="1" topLeftCell="K6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,19 +1765,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q1" s="98" t="s">
-        <v>194</v>
-      </c>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
+      <c r="Q1" s="119" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
+      <c r="B2" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="118"/>
       <c r="Q2" s="80" t="s">
         <v>0</v>
       </c>
@@ -1768,13 +1803,13 @@
         <v>3</v>
       </c>
       <c r="Q3" s="94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="R3" s="84" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S3" s="82" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1783,52 +1818,52 @@
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>300</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>32</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R4" s="67" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>35</v>
+        <v>301</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>24</v>
@@ -1840,13 +1875,13 @@
         <v>23</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1864,19 +1899,19 @@
         <v>25</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>28</v>
@@ -1888,19 +1923,19 @@
         <v>27</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>28</v>
@@ -1912,13 +1947,13 @@
         <v>27</v>
       </c>
       <c r="Q9" s="40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R9" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S9" s="51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1936,19 +1971,19 @@
         <v>7</v>
       </c>
       <c r="Q10" s="40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="R10" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S10" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>31</v>
@@ -1960,19 +1995,19 @@
         <v>30</v>
       </c>
       <c r="Q11" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R11" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S11" s="51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>31</v>
@@ -1984,19 +2019,19 @@
         <v>30</v>
       </c>
       <c r="Q12" s="40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R12" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S12" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>31</v>
@@ -2008,19 +2043,19 @@
         <v>30</v>
       </c>
       <c r="Q13" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R13" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S13" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>31</v>
@@ -2032,19 +2067,19 @@
         <v>30</v>
       </c>
       <c r="Q14" s="40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="R14" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S14" s="41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>31</v>
@@ -2056,17 +2091,17 @@
         <v>30</v>
       </c>
       <c r="Q15" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R15" s="81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>31</v>
@@ -2078,17 +2113,17 @@
         <v>30</v>
       </c>
       <c r="Q16" s="42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R16" s="52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S16" s="25"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>31</v>
@@ -2103,36 +2138,36 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D18" s="13">
         <v>971050154</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q18" s="98" t="s">
-        <v>200</v>
-      </c>
-      <c r="R18" s="98"/>
-      <c r="S18" s="98"/>
+        <v>63</v>
+      </c>
+      <c r="Q18" s="119" t="s">
+        <v>198</v>
+      </c>
+      <c r="R18" s="119"/>
+      <c r="S18" s="119"/>
     </row>
     <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D19" s="13">
         <v>971050154</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q19" s="83" t="s">
         <v>0</v>
@@ -2147,260 +2182,260 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D20" s="13">
         <v>971050154</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q20" s="37" t="s">
-        <v>161</v>
-      </c>
-      <c r="R20" s="99" t="s">
-        <v>272</v>
+        <v>159</v>
+      </c>
+      <c r="R20" s="95" t="s">
+        <v>270</v>
       </c>
       <c r="S20" s="82" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="67" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D21" s="13">
         <v>971050154</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q21" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="R21" s="100" t="s">
-        <v>272</v>
+        <v>161</v>
+      </c>
+      <c r="R21" s="96" t="s">
+        <v>270</v>
       </c>
       <c r="S21" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>30</v>
       </c>
       <c r="Q22" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="R22" s="100" t="s">
-        <v>272</v>
+        <v>162</v>
+      </c>
+      <c r="R22" s="96" t="s">
+        <v>270</v>
       </c>
       <c r="S22" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="12"/>
       <c r="Q23" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="R23" s="100" t="s">
-        <v>272</v>
+        <v>167</v>
+      </c>
+      <c r="R23" s="96" t="s">
+        <v>270</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D24" s="16"/>
       <c r="Q24" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="R24" s="100" t="s">
-        <v>273</v>
+        <v>200</v>
+      </c>
+      <c r="R24" s="96" t="s">
+        <v>271</v>
       </c>
       <c r="S24" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D25" s="16"/>
       <c r="Q25" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="R25" s="100" t="s">
-        <v>273</v>
+        <v>202</v>
+      </c>
+      <c r="R25" s="96" t="s">
+        <v>271</v>
       </c>
       <c r="S25" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D26" s="16"/>
       <c r="Q26" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="R26" s="100" t="s">
-        <v>273</v>
+        <v>204</v>
+      </c>
+      <c r="R26" s="96" t="s">
+        <v>271</v>
       </c>
       <c r="S26" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D27" s="16"/>
       <c r="Q27" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="R27" s="100" t="s">
-        <v>273</v>
+        <v>206</v>
+      </c>
+      <c r="R27" s="96" t="s">
+        <v>271</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D28" s="16"/>
       <c r="Q28" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="R28" s="100" t="s">
-        <v>138</v>
+        <v>118</v>
+      </c>
+      <c r="R28" s="96" t="s">
+        <v>136</v>
       </c>
       <c r="S28" s="16"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29" s="16"/>
       <c r="Q29" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="R29" s="100" t="s">
-        <v>139</v>
+        <v>119</v>
+      </c>
+      <c r="R29" s="96" t="s">
+        <v>137</v>
       </c>
       <c r="S29" s="16"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="16"/>
       <c r="Q30" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="R30" s="100" t="s">
-        <v>139</v>
+        <v>120</v>
+      </c>
+      <c r="R30" s="96" t="s">
+        <v>137</v>
       </c>
       <c r="S30" s="16"/>
     </row>
     <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D31" s="16"/>
       <c r="Q31" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="R31" s="101" t="s">
-        <v>140</v>
+        <v>124</v>
+      </c>
+      <c r="R31" s="97" t="s">
+        <v>138</v>
       </c>
       <c r="S31" s="25"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D32" s="16"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D33" s="16"/>
-      <c r="Q33" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="R33" s="98"/>
-      <c r="S33" s="98"/>
+      <c r="Q33" s="119" t="s">
+        <v>208</v>
+      </c>
+      <c r="R33" s="119"/>
+      <c r="S33" s="119"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D34" s="25"/>
       <c r="Q34" s="83" t="s">
@@ -2415,29 +2450,29 @@
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="Q35" s="37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="R35" s="38" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="S35" s="82" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="32"/>
       <c r="C36" s="33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D36" s="34"/>
       <c r="Q36" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="R36" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="S36" s="16" t="s">
         <v>211</v>
-      </c>
-      <c r="R36" s="81" t="s">
-        <v>212</v>
-      </c>
-      <c r="S36" s="16" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="37" spans="2:19" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2451,56 +2486,56 @@
         <v>1</v>
       </c>
       <c r="Q37" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R37" s="52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="S37" s="25"/>
     </row>
     <row r="38" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="99" t="s">
-        <v>264</v>
+        <v>48</v>
+      </c>
+      <c r="C38" s="95" t="s">
+        <v>262</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q38" s="102" t="s">
-        <v>136</v>
-      </c>
-      <c r="R38" s="103" t="s">
         <v>144</v>
+      </c>
+      <c r="Q38" s="98" t="s">
+        <v>134</v>
+      </c>
+      <c r="R38" s="99" t="s">
+        <v>142</v>
       </c>
       <c r="S38" s="79"/>
     </row>
     <row r="39" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="100" t="s">
-        <v>250</v>
+        <v>145</v>
+      </c>
+      <c r="C39" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q39" s="95" t="s">
-        <v>214</v>
-      </c>
-      <c r="R39" s="96"/>
-      <c r="S39" s="97"/>
+        <v>146</v>
+      </c>
+      <c r="Q39" s="116" t="s">
+        <v>212</v>
+      </c>
+      <c r="R39" s="117"/>
+      <c r="S39" s="118"/>
     </row>
     <row r="40" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="100" t="s">
-        <v>250</v>
+        <v>147</v>
+      </c>
+      <c r="C40" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q40" s="80" t="s">
         <v>0</v>
@@ -2514,137 +2549,137 @@
     </row>
     <row r="41" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" s="100" t="s">
-        <v>250</v>
+        <v>148</v>
+      </c>
+      <c r="C41" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q41" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="R41" s="100" t="s">
-        <v>275</v>
+        <v>67</v>
+      </c>
+      <c r="R41" s="96" t="s">
+        <v>273</v>
       </c>
       <c r="S41" s="85" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="100" t="s">
-        <v>250</v>
+        <v>149</v>
+      </c>
+      <c r="C42" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="R42" s="100" t="s">
-        <v>276</v>
+        <v>172</v>
+      </c>
+      <c r="R42" s="96" t="s">
+        <v>274</v>
       </c>
       <c r="S42" s="51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="2:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="100" t="s">
-        <v>265</v>
+        <v>50</v>
+      </c>
+      <c r="C43" s="96" t="s">
+        <v>263</v>
       </c>
       <c r="D43" s="41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="R43" s="100" t="s">
-        <v>277</v>
+        <v>169</v>
+      </c>
+      <c r="R43" s="96" t="s">
+        <v>275</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B44" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="100" t="s">
-        <v>250</v>
+        <v>151</v>
+      </c>
+      <c r="C44" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D44" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="R44" s="100" t="s">
-        <v>278</v>
+        <v>216</v>
+      </c>
+      <c r="R44" s="96" t="s">
+        <v>276</v>
       </c>
       <c r="S44" s="86" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B45" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="100" t="s">
-        <v>250</v>
+        <v>152</v>
+      </c>
+      <c r="C45" s="96" t="s">
+        <v>248</v>
       </c>
       <c r="D45" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="R45" s="100" t="s">
-        <v>279</v>
+        <v>218</v>
+      </c>
+      <c r="R45" s="96" t="s">
+        <v>277</v>
       </c>
       <c r="S45" s="86" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B46" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="100" t="s">
-        <v>265</v>
+        <v>49</v>
+      </c>
+      <c r="C46" s="96" t="s">
+        <v>263</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="R46" s="100" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+      <c r="R46" s="96" t="s">
+        <v>139</v>
       </c>
       <c r="S46" s="16"/>
     </row>
     <row r="47" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="101" t="s">
-        <v>266</v>
+        <v>54</v>
+      </c>
+      <c r="C47" s="97" t="s">
+        <v>264</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q47" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="R47" s="101" t="s">
-        <v>141</v>
+        <v>127</v>
+      </c>
+      <c r="R47" s="97" t="s">
+        <v>139</v>
       </c>
       <c r="S47" s="25"/>
     </row>
@@ -2659,14 +2694,14 @@
     <row r="49" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="46"/>
       <c r="C49" s="47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D49" s="48"/>
-      <c r="Q49" s="95" t="s">
-        <v>222</v>
-      </c>
-      <c r="R49" s="96"/>
-      <c r="S49" s="97"/>
+      <c r="Q49" s="116" t="s">
+        <v>220</v>
+      </c>
+      <c r="R49" s="117"/>
+      <c r="S49" s="118"/>
     </row>
     <row r="50" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="29" t="s">
@@ -2690,42 +2725,42 @@
     </row>
     <row r="51" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="R51" s="100" t="s">
-        <v>280</v>
+        <v>177</v>
+      </c>
+      <c r="R51" s="96" t="s">
+        <v>278</v>
       </c>
       <c r="S51" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D52" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q52" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="R52" s="100" t="s">
-        <v>280</v>
+        <v>178</v>
+      </c>
+      <c r="R52" s="96" t="s">
+        <v>278</v>
       </c>
       <c r="S52" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -2733,79 +2768,79 @@
         <v>5</v>
       </c>
       <c r="C53" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q53" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="R53" s="100" t="s">
-        <v>280</v>
+        <v>179</v>
+      </c>
+      <c r="R53" s="96" t="s">
+        <v>278</v>
       </c>
       <c r="S53" s="51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C54" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D54" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="R54" s="100" t="s">
-        <v>288</v>
+        <v>221</v>
+      </c>
+      <c r="R54" s="96" t="s">
+        <v>286</v>
       </c>
       <c r="S54" s="86" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C55" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D55" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q55" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="R55" s="100" t="s">
-        <v>288</v>
+        <v>222</v>
+      </c>
+      <c r="R55" s="96" t="s">
+        <v>286</v>
       </c>
       <c r="S55" s="86" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D56" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q56" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="R56" s="100" t="s">
-        <v>288</v>
+        <v>223</v>
+      </c>
+      <c r="R56" s="96" t="s">
+        <v>286</v>
       </c>
       <c r="S56" s="86" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
@@ -2813,24 +2848,24 @@
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
       <c r="Q57" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="R57" s="100" t="s">
-        <v>143</v>
+        <v>129</v>
+      </c>
+      <c r="R57" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="S57" s="86"/>
     </row>
     <row r="58" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="55"/>
       <c r="C58" s="56" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D58" s="57"/>
       <c r="Q58" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="R58" s="100" t="s">
-        <v>143</v>
+        <v>130</v>
+      </c>
+      <c r="R58" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="S58" s="16"/>
     </row>
@@ -2845,22 +2880,22 @@
         <v>1</v>
       </c>
       <c r="Q59" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="R59" s="101" t="s">
-        <v>143</v>
+        <v>131</v>
+      </c>
+      <c r="R59" s="97" t="s">
+        <v>141</v>
       </c>
       <c r="S59" s="25"/>
     </row>
     <row r="60" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="99" t="s">
-        <v>267</v>
+        <v>72</v>
+      </c>
+      <c r="C60" s="95" t="s">
+        <v>265</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q60" s="69"/>
       <c r="R60" s="69"/>
@@ -2868,167 +2903,167 @@
     </row>
     <row r="61" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" s="100" t="s">
-        <v>238</v>
+        <v>161</v>
+      </c>
+      <c r="C61" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D61" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q61" s="95" t="s">
-        <v>214</v>
-      </c>
-      <c r="R61" s="96"/>
-      <c r="S61" s="97"/>
+        <v>156</v>
+      </c>
+      <c r="Q61" s="116" t="s">
+        <v>212</v>
+      </c>
+      <c r="R61" s="117"/>
+      <c r="S61" s="118"/>
     </row>
     <row r="62" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C62" s="100" t="s">
-        <v>267</v>
+        <v>73</v>
+      </c>
+      <c r="C62" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D62" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q62" s="105" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q62" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="R62" s="105" t="s">
+      <c r="R62" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="S62" s="105" t="s">
+      <c r="S62" s="101" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B63" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C63" s="100" t="s">
-        <v>238</v>
+        <v>162</v>
+      </c>
+      <c r="C63" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q63" s="107" t="s">
-        <v>69</v>
-      </c>
-      <c r="R63" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="S63" s="118" t="s">
-        <v>297</v>
+        <v>156</v>
+      </c>
+      <c r="Q63" s="103" t="s">
+        <v>67</v>
+      </c>
+      <c r="R63" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="S63" s="114" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="2:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="100" t="s">
-        <v>267</v>
+        <v>74</v>
+      </c>
+      <c r="C64" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D64" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q64" s="107" t="s">
-        <v>174</v>
-      </c>
-      <c r="R64" s="116" t="s">
-        <v>238</v>
-      </c>
-      <c r="S64" s="117" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="Q64" s="103" t="s">
+        <v>172</v>
+      </c>
+      <c r="R64" s="112" t="s">
+        <v>236</v>
+      </c>
+      <c r="S64" s="113" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="100" t="s">
-        <v>238</v>
+        <v>112</v>
+      </c>
+      <c r="C65" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D65" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q65" s="107" t="s">
-        <v>171</v>
-      </c>
-      <c r="R65" s="116" t="s">
-        <v>249</v>
-      </c>
-      <c r="S65" s="110" t="s">
-        <v>172</v>
+        <v>156</v>
+      </c>
+      <c r="Q65" s="103" t="s">
+        <v>169</v>
+      </c>
+      <c r="R65" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="S65" s="106" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="100" t="s">
-        <v>268</v>
+      <c r="C66" s="96" t="s">
+        <v>266</v>
       </c>
       <c r="D66" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q66" s="119" t="s">
-        <v>173</v>
-      </c>
-      <c r="R66" s="116" t="s">
-        <v>250</v>
-      </c>
-      <c r="S66" s="110" t="s">
-        <v>148</v>
+        <v>163</v>
+      </c>
+      <c r="Q66" s="115" t="s">
+        <v>171</v>
+      </c>
+      <c r="R66" s="112" t="s">
+        <v>248</v>
+      </c>
+      <c r="S66" s="106" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:19" s="45" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="101" t="s">
-        <v>251</v>
+      <c r="C67" s="97" t="s">
+        <v>249</v>
       </c>
       <c r="D67" s="53" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q67" s="107" t="s">
-        <v>218</v>
-      </c>
-      <c r="R67" s="106" t="s">
-        <v>298</v>
-      </c>
-      <c r="S67" s="115" t="s">
-        <v>299</v>
+        <v>164</v>
+      </c>
+      <c r="Q67" s="103" t="s">
+        <v>216</v>
+      </c>
+      <c r="R67" s="102" t="s">
+        <v>296</v>
+      </c>
+      <c r="S67" s="111" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="68" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B68" s="50"/>
       <c r="C68" s="50"/>
       <c r="D68" s="50"/>
-      <c r="Q68" s="107" t="s">
-        <v>220</v>
-      </c>
-      <c r="R68" s="106" t="s">
-        <v>300</v>
-      </c>
-      <c r="S68" s="115" t="s">
-        <v>301</v>
+      <c r="Q68" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="R68" s="102" t="s">
+        <v>298</v>
+      </c>
+      <c r="S68" s="111" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B69" s="60"/>
       <c r="C69" s="61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D69" s="62"/>
-      <c r="Q69" s="107" t="s">
-        <v>128</v>
-      </c>
-      <c r="R69" s="113" t="s">
-        <v>141</v>
-      </c>
-      <c r="S69" s="111"/>
+      <c r="Q69" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="R69" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="S69" s="107"/>
     </row>
     <row r="70" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="29" t="s">
@@ -3040,23 +3075,23 @@
       <c r="D70" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="Q70" s="108" t="s">
-        <v>129</v>
-      </c>
-      <c r="R70" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="S70" s="112"/>
+      <c r="Q70" s="104" t="s">
+        <v>127</v>
+      </c>
+      <c r="R70" s="110" t="s">
+        <v>139</v>
+      </c>
+      <c r="S70" s="108"/>
     </row>
     <row r="71" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D71" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q71" s="69"/>
       <c r="R71" s="69"/>
@@ -3064,62 +3099,91 @@
     </row>
     <row r="72" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C72" s="81" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D72" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q72" s="69"/>
-      <c r="R72" s="69"/>
-      <c r="S72" s="69"/>
+        <v>156</v>
+      </c>
+      <c r="Q72" s="119" t="s">
+        <v>192</v>
+      </c>
+      <c r="R72" s="119"/>
+      <c r="S72" s="119"/>
     </row>
     <row r="73" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" s="81" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D73" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q73" s="69"/>
-      <c r="R73" s="69"/>
-      <c r="S73" s="69"/>
+        <v>155</v>
+      </c>
+      <c r="Q73" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="R73" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="S73" s="121" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B74" s="42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C74" s="52" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D74" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q74" s="69"/>
-      <c r="R74" s="69"/>
-      <c r="S74" s="69"/>
+        <v>156</v>
+      </c>
+      <c r="Q74" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="R74" s="120" t="s">
+        <v>302</v>
+      </c>
+      <c r="S74" s="106">
+        <v>154</v>
+      </c>
     </row>
     <row r="75" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B75" s="58"/>
       <c r="C75" s="58"/>
       <c r="D75" s="58"/>
-      <c r="Q75" s="69"/>
-      <c r="R75" s="69"/>
-      <c r="S75" s="69"/>
+      <c r="Q75" s="127" t="s">
+        <v>195</v>
+      </c>
+      <c r="R75" s="120" t="s">
+        <v>302</v>
+      </c>
+      <c r="S75" s="106">
+        <v>154</v>
+      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="14"/>
-      <c r="B76" s="95" t="s">
-        <v>66</v>
-      </c>
-      <c r="C76" s="96"/>
-      <c r="D76" s="97"/>
+      <c r="B76" s="116" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" s="117"/>
+      <c r="D76" s="118"/>
       <c r="E76" s="12"/>
+      <c r="Q76" s="127" t="s">
+        <v>39</v>
+      </c>
+      <c r="R76" s="120" t="s">
+        <v>303</v>
+      </c>
+      <c r="S76" s="130" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="14"/>
@@ -3135,55 +3199,91 @@
       <c r="E77" t="s">
         <v>3</v>
       </c>
+      <c r="Q77" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="R77" s="120" t="s">
+        <v>303</v>
+      </c>
+      <c r="S77" s="130" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="14"/>
       <c r="B78" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D78" s="13">
         <v>2136</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="Q78" s="127" t="s">
+        <v>53</v>
+      </c>
+      <c r="R78" s="120" t="s">
+        <v>303</v>
+      </c>
+      <c r="S78" s="130" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="14"/>
       <c r="B79" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79" s="100" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="C79" s="96" t="s">
+        <v>61</v>
       </c>
       <c r="D79" s="13">
         <v>1182</v>
       </c>
       <c r="E79" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q79" s="127" t="s">
         <v>67</v>
+      </c>
+      <c r="R79" s="120" t="s">
+        <v>303</v>
+      </c>
+      <c r="S79" s="130" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="14"/>
       <c r="B80" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C80" s="100" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="C80" s="96" t="s">
+        <v>44</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="Q80" s="122" t="s">
+        <v>145</v>
+      </c>
+      <c r="R80" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S80" s="124" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="14"/>
       <c r="B81" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C81" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="C81" s="96" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="13">
@@ -3191,14 +3291,23 @@
       </c>
       <c r="E81" s="12" t="s">
         <v>27</v>
+      </c>
+      <c r="Q81" s="122" t="s">
+        <v>147</v>
+      </c>
+      <c r="R81" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S81" s="123" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="14"/>
       <c r="B82" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="100" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="96" t="s">
         <v>28</v>
       </c>
       <c r="D82" s="13">
@@ -3206,14 +3315,23 @@
       </c>
       <c r="E82" s="12" t="s">
         <v>27</v>
+      </c>
+      <c r="Q82" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="R82" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S82" s="124" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
       <c r="B83" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C83" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="96" t="s">
         <v>31</v>
       </c>
       <c r="D83" s="13">
@@ -3221,14 +3339,23 @@
       </c>
       <c r="E83" s="12" t="s">
         <v>30</v>
+      </c>
+      <c r="Q83" s="122" t="s">
+        <v>149</v>
+      </c>
+      <c r="R83" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S83" s="123" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="14"/>
       <c r="B84" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C84" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="96" t="s">
         <v>29</v>
       </c>
       <c r="D84" s="13">
@@ -3236,108 +3363,140 @@
       </c>
       <c r="E84" s="12" t="s">
         <v>7</v>
+      </c>
+      <c r="Q84" s="128" t="s">
+        <v>151</v>
+      </c>
+      <c r="R84" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S84" s="123" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="14"/>
       <c r="B85" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C85" s="100" t="s">
-        <v>260</v>
+        <v>56</v>
+      </c>
+      <c r="C85" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D85" s="13">
         <v>971050154</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="Q85" s="128" t="s">
+        <v>152</v>
+      </c>
+      <c r="R85" s="125" t="s">
+        <v>243</v>
+      </c>
+      <c r="S85" s="123" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="14"/>
       <c r="B86" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C86" s="100" t="s">
-        <v>260</v>
+        <v>57</v>
+      </c>
+      <c r="C86" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D86" s="13">
         <v>971050154</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="Q86" s="128" t="s">
+        <v>113</v>
+      </c>
+      <c r="R86" s="126" t="s">
+        <v>135</v>
+      </c>
+      <c r="S86" s="130"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="14"/>
       <c r="B87" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="100" t="s">
-        <v>260</v>
+        <v>58</v>
+      </c>
+      <c r="C87" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D87" s="13">
         <v>971050154</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="Q87" s="129" t="s">
+        <v>115</v>
+      </c>
+      <c r="R87" s="132" t="s">
+        <v>135</v>
+      </c>
+      <c r="S87" s="131"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="14"/>
       <c r="B88" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C88" s="100" t="s">
-        <v>260</v>
+        <v>59</v>
+      </c>
+      <c r="C88" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D88" s="13">
         <v>971050154</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B89" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C89" s="100" t="s">
-        <v>137</v>
+        <v>114</v>
+      </c>
+      <c r="C89" s="96" t="s">
+        <v>135</v>
       </c>
       <c r="D89" s="16"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C90" s="100" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+      <c r="C90" s="96" t="s">
+        <v>139</v>
       </c>
       <c r="D90" s="16"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B91" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C91" s="100" t="s">
-        <v>141</v>
+        <v>127</v>
+      </c>
+      <c r="C91" s="96" t="s">
+        <v>139</v>
       </c>
       <c r="D91" s="16"/>
     </row>
     <row r="92" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B92" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C92" s="101" t="s">
-        <v>141</v>
+        <v>125</v>
+      </c>
+      <c r="C92" s="97" t="s">
+        <v>139</v>
       </c>
       <c r="D92" s="25"/>
     </row>
     <row r="94" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B94" s="64"/>
       <c r="C94" s="65" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D94" s="66"/>
       <c r="Q94" s="69"/>
@@ -3360,13 +3519,13 @@
     </row>
     <row r="96" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C96" s="38" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D96" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q96" s="69"/>
       <c r="R96" s="69"/>
@@ -3374,13 +3533,13 @@
     </row>
     <row r="97" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B97" s="40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C97" s="68" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D97" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q97" s="69"/>
       <c r="R97" s="69"/>
@@ -3388,13 +3547,13 @@
     </row>
     <row r="98" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B98" s="40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C98" s="68" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D98" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q98" s="69"/>
       <c r="R98" s="69"/>
@@ -3402,13 +3561,13 @@
     </row>
     <row r="99" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B99" s="40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C99" s="68" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D99" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q99" s="69"/>
       <c r="R99" s="69"/>
@@ -3416,13 +3575,13 @@
     </row>
     <row r="100" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B100" s="40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C100" s="68" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D100" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q100" s="69"/>
       <c r="R100" s="69"/>
@@ -3430,13 +3589,13 @@
     </row>
     <row r="101" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B101" s="40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C101" s="68" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D101" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q101" s="69"/>
       <c r="R101" s="69"/>
@@ -3444,22 +3603,22 @@
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B102" s="42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C102" s="52" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D102" s="53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
-      <c r="B104" s="95" t="s">
-        <v>79</v>
-      </c>
-      <c r="C104" s="96"/>
-      <c r="D104" s="97"/>
+      <c r="B104" s="116" t="s">
+        <v>77</v>
+      </c>
+      <c r="C104" s="117"/>
+      <c r="D104" s="118"/>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="14"/>
@@ -3479,13 +3638,13 @@
     <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="14"/>
       <c r="B106" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E106" s="12" t="s">
         <v>6</v>
@@ -3494,10 +3653,10 @@
     <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="14"/>
       <c r="B107" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D107" s="16" t="s">
         <v>9</v>
@@ -3506,10 +3665,10 @@
     <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="14"/>
       <c r="B108" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D108" s="13">
         <v>2670</v>
@@ -3524,7 +3683,7 @@
         <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D109" s="13">
         <v>533750510</v>
@@ -3536,13 +3695,13 @@
     <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="14"/>
       <c r="B110" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E110" s="12" t="s">
         <v>10</v>
@@ -3551,13 +3710,13 @@
     <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="14"/>
       <c r="B111" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E111" s="12" t="s">
         <v>11</v>
@@ -3565,20 +3724,20 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B112" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D112" s="25"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="14"/>
-      <c r="B114" s="95" t="s">
-        <v>92</v>
-      </c>
-      <c r="C114" s="96"/>
-      <c r="D114" s="97"/>
+      <c r="B114" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="C114" s="117"/>
+      <c r="D114" s="118"/>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="14"/>
@@ -3598,19 +3757,19 @@
     <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="14"/>
       <c r="B116" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D116" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="14"/>
       <c r="B117" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>31</v>
@@ -3625,7 +3784,7 @@
     <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="14"/>
       <c r="B118" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>26</v>
@@ -3640,7 +3799,7 @@
     <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="14"/>
       <c r="B119" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>31</v>
@@ -3655,78 +3814,78 @@
     <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="14"/>
       <c r="B120" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D120" s="13">
         <v>971050154</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="14"/>
       <c r="B121" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C121" s="36" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="14"/>
       <c r="B122" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C122" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D122" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E122" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="E122" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:19" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="14"/>
       <c r="B123" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C123" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E123" s="12" t="s">
         <v>187</v>
-      </c>
-      <c r="C123" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="D123" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="E123" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B124" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D124" s="16"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B125" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D125" s="25"/>
     </row>
@@ -3741,7 +3900,7 @@
     <row r="127" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="70"/>
       <c r="C127" s="71" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D127" s="72"/>
       <c r="Q127" s="69"/>
@@ -3764,13 +3923,13 @@
     </row>
     <row r="129" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B129" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="C129" s="100" t="s">
-        <v>267</v>
+        <v>175</v>
+      </c>
+      <c r="C129" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D129" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q129" s="69"/>
       <c r="R129" s="69"/>
@@ -3778,13 +3937,13 @@
     </row>
     <row r="130" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B130" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C130" s="100" t="s">
-        <v>238</v>
+        <v>82</v>
+      </c>
+      <c r="C130" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D130" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q130" s="69"/>
       <c r="R130" s="69"/>
@@ -3792,11 +3951,11 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="21"/>
-      <c r="B132" s="95" t="s">
-        <v>93</v>
-      </c>
-      <c r="C132" s="96"/>
-      <c r="D132" s="97"/>
+      <c r="B132" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C132" s="117"/>
+      <c r="D132" s="118"/>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="14"/>
@@ -3816,9 +3975,9 @@
     <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="14"/>
       <c r="B134" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C134" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="C134" s="96" t="s">
         <v>21</v>
       </c>
       <c r="D134" s="13">
@@ -3831,13 +3990,13 @@
     <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" s="14"/>
       <c r="B135" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C135" s="100" t="s">
+        <v>38</v>
+      </c>
+      <c r="C135" s="96" t="s">
         <v>18</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E135" s="12" t="s">
         <v>19</v>
@@ -3846,38 +4005,38 @@
     <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" s="14"/>
       <c r="B136" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C136" s="100" t="s">
-        <v>105</v>
+        <v>92</v>
+      </c>
+      <c r="C136" s="96" t="s">
+        <v>103</v>
       </c>
       <c r="D136" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E136" s="12"/>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" s="14"/>
       <c r="B137" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C137" s="100" t="s">
-        <v>46</v>
+        <v>93</v>
+      </c>
+      <c r="C137" s="96" t="s">
+        <v>44</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="14"/>
       <c r="B138" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C138" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="C138" s="96" t="s">
         <v>17</v>
       </c>
       <c r="D138" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E138" s="12" t="s">
         <v>16</v>
@@ -3886,10 +4045,10 @@
     <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" s="14"/>
       <c r="B139" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C139" s="100" t="s">
-        <v>269</v>
+        <v>98</v>
+      </c>
+      <c r="C139" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D139" s="13">
         <v>533750210</v>
@@ -3901,10 +4060,10 @@
     <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" s="14"/>
       <c r="B140" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C140" s="100" t="s">
-        <v>269</v>
+        <v>99</v>
+      </c>
+      <c r="C140" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D140" s="13">
         <v>533750210</v>
@@ -3916,10 +4075,10 @@
     <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" s="14"/>
       <c r="B141" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C141" s="100" t="s">
-        <v>269</v>
+        <v>100</v>
+      </c>
+      <c r="C141" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D141" s="13">
         <v>533750210</v>
@@ -3931,10 +4090,10 @@
     <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" s="14"/>
       <c r="B142" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C142" s="100" t="s">
-        <v>269</v>
+        <v>101</v>
+      </c>
+      <c r="C142" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D142" s="13">
         <v>533750210</v>
@@ -3946,10 +4105,10 @@
     <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="14"/>
       <c r="B143" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C143" s="100" t="s">
-        <v>254</v>
+        <v>102</v>
+      </c>
+      <c r="C143" s="96" t="s">
+        <v>252</v>
       </c>
       <c r="D143" s="13">
         <v>533750510</v>
@@ -3961,67 +4120,67 @@
     <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="14"/>
       <c r="B144" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C144" s="100" t="s">
-        <v>260</v>
+        <v>85</v>
+      </c>
+      <c r="C144" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D144" s="13">
         <v>971050154</v>
       </c>
       <c r="E144" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B145" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C145" s="100" t="s">
-        <v>138</v>
+        <v>116</v>
+      </c>
+      <c r="C145" s="96" t="s">
+        <v>136</v>
       </c>
       <c r="D145" s="16"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C146" s="100" t="s">
-        <v>143</v>
+        <v>129</v>
+      </c>
+      <c r="C146" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="D146" s="16"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B147" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C147" s="100" t="s">
-        <v>143</v>
+        <v>130</v>
+      </c>
+      <c r="C147" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="D147" s="16"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B148" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C148" s="100" t="s">
-        <v>143</v>
+        <v>131</v>
+      </c>
+      <c r="C148" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="D148" s="16"/>
     </row>
     <row r="149" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C149" s="101" t="s">
-        <v>143</v>
+        <v>132</v>
+      </c>
+      <c r="C149" s="97" t="s">
+        <v>141</v>
       </c>
       <c r="D149" s="25"/>
     </row>
     <row r="151" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B151" s="74"/>
       <c r="C151" s="75" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D151" s="76"/>
     </row>
@@ -4038,99 +4197,99 @@
     </row>
     <row r="153" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C153" s="99" t="s">
-        <v>267</v>
+        <v>99</v>
+      </c>
+      <c r="C153" s="95" t="s">
+        <v>265</v>
       </c>
       <c r="D153" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B154" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="C154" s="100" t="s">
-        <v>238</v>
+        <v>177</v>
+      </c>
+      <c r="C154" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D154" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B155" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C155" s="100" t="s">
-        <v>267</v>
+        <v>100</v>
+      </c>
+      <c r="C155" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D155" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B156" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="C156" s="100" t="s">
-        <v>238</v>
+        <v>178</v>
+      </c>
+      <c r="C156" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D156" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B157" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C157" s="100" t="s">
-        <v>267</v>
+        <v>101</v>
+      </c>
+      <c r="C157" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D157" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B158" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="C158" s="100" t="s">
-        <v>238</v>
+        <v>179</v>
+      </c>
+      <c r="C158" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D158" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B159" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="C159" s="100" t="s">
-        <v>268</v>
+        <v>180</v>
+      </c>
+      <c r="C159" s="96" t="s">
+        <v>266</v>
       </c>
       <c r="D159" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="160" spans="2:4" s="69" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C160" s="101" t="s">
-        <v>251</v>
+        <v>102</v>
+      </c>
+      <c r="C160" s="97" t="s">
+        <v>249</v>
       </c>
       <c r="D160" s="53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="23"/>
-      <c r="B162" s="95" t="s">
-        <v>108</v>
-      </c>
-      <c r="C162" s="96"/>
-      <c r="D162" s="97"/>
+      <c r="B162" s="116" t="s">
+        <v>106</v>
+      </c>
+      <c r="C162" s="117"/>
+      <c r="D162" s="118"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="23"/>
@@ -4150,26 +4309,26 @@
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="23"/>
       <c r="B164" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C164" s="100" t="s">
-        <v>234</v>
+        <v>34</v>
+      </c>
+      <c r="C164" s="96" t="s">
+        <v>232</v>
       </c>
       <c r="D164" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E164" s="10"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="23"/>
       <c r="B165" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C165" s="100" t="s">
-        <v>46</v>
+        <v>107</v>
+      </c>
+      <c r="C165" s="96" t="s">
+        <v>44</v>
       </c>
       <c r="D165" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E165" s="10"/>
     </row>
@@ -4178,11 +4337,11 @@
       <c r="B166" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C166" s="100" t="s">
-        <v>112</v>
+      <c r="C166" s="96" t="s">
+        <v>110</v>
       </c>
       <c r="D166" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E166" s="22" t="s">
         <v>15</v>
@@ -4191,10 +4350,10 @@
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="23"/>
       <c r="B167" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C167" s="100" t="s">
-        <v>269</v>
+        <v>112</v>
+      </c>
+      <c r="C167" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D167" s="13">
         <v>533750210</v>
@@ -4206,10 +4365,10 @@
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="23"/>
       <c r="B168" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C168" s="100" t="s">
-        <v>269</v>
+        <v>108</v>
+      </c>
+      <c r="C168" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D168" s="13">
         <v>533750210</v>
@@ -4221,10 +4380,10 @@
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="23"/>
       <c r="B169" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C169" s="100" t="s">
-        <v>269</v>
+        <v>109</v>
+      </c>
+      <c r="C169" s="96" t="s">
+        <v>267</v>
       </c>
       <c r="D169" s="13">
         <v>533750210</v>
@@ -4236,49 +4395,49 @@
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="23"/>
       <c r="B170" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C170" s="100" t="s">
-        <v>260</v>
+        <v>85</v>
+      </c>
+      <c r="C170" s="96" t="s">
+        <v>258</v>
       </c>
       <c r="D170" s="13">
         <v>971050154</v>
       </c>
       <c r="E170" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B171" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C171" s="100" t="s">
-        <v>139</v>
+        <v>121</v>
+      </c>
+      <c r="C171" s="96" t="s">
+        <v>137</v>
       </c>
       <c r="D171" s="16"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B172" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C172" s="100" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="C172" s="96" t="s">
+        <v>142</v>
       </c>
       <c r="D172" s="16"/>
     </row>
     <row r="173" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B173" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C173" s="101" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="C173" s="97" t="s">
+        <v>142</v>
       </c>
       <c r="D173" s="25"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B175" s="77"/>
       <c r="C175" s="78" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D175" s="79"/>
     </row>
@@ -4295,52 +4454,52 @@
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B177" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="C177" s="99" t="s">
-        <v>267</v>
+        <v>108</v>
+      </c>
+      <c r="C177" s="95" t="s">
+        <v>265</v>
       </c>
       <c r="D177" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B178" s="40" t="s">
-        <v>184</v>
-      </c>
-      <c r="C178" s="100" t="s">
-        <v>238</v>
+        <v>182</v>
+      </c>
+      <c r="C178" s="96" t="s">
+        <v>236</v>
       </c>
       <c r="D178" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B179" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="C179" s="100" t="s">
-        <v>267</v>
+        <v>109</v>
+      </c>
+      <c r="C179" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D179" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="180" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B180" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="C180" s="101" t="s">
-        <v>238</v>
+        <v>183</v>
+      </c>
+      <c r="C180" s="97" t="s">
+        <v>236</v>
       </c>
       <c r="D180" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B182" s="87"/>
       <c r="C182" s="88" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D182" s="89"/>
     </row>
@@ -4356,174 +4515,175 @@
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B184" s="104" t="s">
-        <v>136</v>
-      </c>
-      <c r="C184" s="100" t="s">
-        <v>144</v>
+      <c r="B184" s="100" t="s">
+        <v>134</v>
+      </c>
+      <c r="C184" s="96" t="s">
+        <v>142</v>
       </c>
       <c r="D184" s="91"/>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B185" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C185" s="100" t="s">
-        <v>270</v>
+        <v>226</v>
+      </c>
+      <c r="C185" s="96" t="s">
+        <v>268</v>
       </c>
       <c r="D185" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B186" s="92" t="s">
-        <v>235</v>
-      </c>
-      <c r="C186" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="C186" s="96" t="s">
+        <v>282</v>
+      </c>
+      <c r="D186" s="16" t="s">
         <v>284</v>
-      </c>
-      <c r="D186" s="16" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B187" s="92" t="s">
-        <v>236</v>
-      </c>
-      <c r="C187" s="100" t="s">
+        <v>234</v>
+      </c>
+      <c r="C187" s="96" t="s">
+        <v>281</v>
+      </c>
+      <c r="D187" s="16" t="s">
         <v>283</v>
-      </c>
-      <c r="D187" s="16" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B188" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C188" s="100" t="s">
-        <v>271</v>
+        <v>235</v>
+      </c>
+      <c r="C188" s="96" t="s">
+        <v>269</v>
       </c>
       <c r="D188" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B189" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C189" s="100" t="s">
-        <v>295</v>
+        <v>228</v>
+      </c>
+      <c r="C189" s="96" t="s">
+        <v>293</v>
       </c>
       <c r="D189" s="91" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B190" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C190" s="100" t="s">
-        <v>290</v>
+        <v>229</v>
+      </c>
+      <c r="C190" s="96" t="s">
+        <v>288</v>
       </c>
       <c r="D190" s="91" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B191" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C191" s="100" t="s">
-        <v>290</v>
+        <v>230</v>
+      </c>
+      <c r="C191" s="96" t="s">
+        <v>288</v>
       </c>
       <c r="D191" s="91" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B192" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C192" s="100" t="s">
-        <v>293</v>
+        <v>231</v>
+      </c>
+      <c r="C192" s="96" t="s">
+        <v>291</v>
       </c>
       <c r="D192" s="91" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B193" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="C193" s="100" t="s">
-        <v>281</v>
+        <v>255</v>
+      </c>
+      <c r="C193" s="96" t="s">
+        <v>279</v>
       </c>
       <c r="D193" s="93" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B194" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="C194" s="100" t="s">
-        <v>281</v>
+        <v>256</v>
+      </c>
+      <c r="C194" s="96" t="s">
+        <v>279</v>
       </c>
       <c r="D194" s="93" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B195" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C195" s="100" t="s">
-        <v>142</v>
+        <v>128</v>
+      </c>
+      <c r="C195" s="96" t="s">
+        <v>140</v>
       </c>
       <c r="D195" s="16"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B196" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C196" s="100" t="s">
-        <v>141</v>
+        <v>125</v>
+      </c>
+      <c r="C196" s="96" t="s">
+        <v>139</v>
       </c>
       <c r="D196" s="16"/>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B197" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C197" s="100" t="s">
-        <v>143</v>
+        <v>132</v>
+      </c>
+      <c r="C197" s="96" t="s">
+        <v>141</v>
       </c>
       <c r="D197" s="16"/>
     </row>
     <row r="198" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B198" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C198" s="101" t="s">
-        <v>140</v>
+        <v>123</v>
+      </c>
+      <c r="C198" s="97" t="s">
+        <v>138</v>
       </c>
       <c r="D198" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="Q72:S72"/>
+    <mergeCell ref="B162:D162"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B132:D132"/>
     <mergeCell ref="Q61:S61"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q18:S18"/>
     <mergeCell ref="Q33:S33"/>
     <mergeCell ref="Q39:S39"/>
     <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="B162:D162"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B132:D132"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>